<commit_message>
added selectNext, selectAll, and clearAll
</commit_message>
<xml_diff>
--- a/static_content/jobs/jobs.xlsx
+++ b/static_content/jobs/jobs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="113">
   <si>
     <t>role</t>
   </si>
@@ -55,10 +55,10 @@
     <t>darkcyan</t>
   </si>
   <si>
-    <t>#008b8b</t>
-  </si>
-  <si>
-    <t>black</t>
+    <t>#006688</t>
+  </si>
+  <si>
+    <t>white</t>
   </si>
   <si>
     <t>• Working as a consulting data engineer in the data cyber security team of the [Cigna Group](url).</t>
@@ -71,9 +71,6 @@
   </si>
   <si>
     <t>#0000ff</t>
-  </si>
-  <si>
-    <t>white</t>
   </si>
   <si>
     <t>• Worked as a consulting data engineer in the analytics team of [Warner Brothers Interactive Entertainment](url) Division.
@@ -88,7 +85,7 @@
     <t>mediumblue</t>
   </si>
   <si>
-    <t>#0000cd</t>
+    <t>#4400cd</t>
   </si>
   <si>
     <t>• Worked as a consulting data engineer for [Angel Studios](url], a streaming media service that offers family-friendly entertainment that amplifies light, with titles including The Chosen, Dry Bar Comedy, and Tuttle Twins.
@@ -132,7 +129,7 @@
     <t xml:space="preserve">Senior Data Engineer </t>
   </si>
   <si>
-    <t>SeniorLiink</t>
+    <t>b</t>
   </si>
   <si>
     <t>maroon</t>
@@ -176,6 +173,9 @@
   </si>
   <si>
     <t>#ff4500</t>
+  </si>
+  <si>
+    <t>black</t>
   </si>
   <si>
     <t>• Co-founded a company that envisioned building a web destination where users could easily record and share their favorite pieces of content like facts, authored stories, quotes, articles, chapters, or personal thoughts, as a way of concretely defining their personal mindset.
@@ -226,6 +226,9 @@
   </si>
   <si>
     <t xml:space="preserve">BuildingBlocks LLC </t>
+  </si>
+  <si>
+    <t>#008b8b</t>
   </si>
   <si>
     <t>• As lead software developer, built a CD-ROM-based home design application for selecting premium home design products for previewing in the context of images of any household rooms. 
@@ -256,6 +259,9 @@
   </si>
   <si>
     <t>BYU</t>
+  </si>
+  <si>
+    <t>#0000cd</t>
   </si>
   <si>
     <t>• Masters of Science degree, Brigham Young University, Provo, Utah
@@ -1026,7 +1032,7 @@
         <v>45047</v>
       </c>
       <c r="D2" s="6">
-        <v>45108</v>
+        <v>45139</v>
       </c>
       <c r="E2" s="7">
         <v>3</v>
@@ -1069,10 +1075,10 @@
       </c>
       <c r="H3" s="10"/>
       <c r="I3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="9" t="s">
         <v>19</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>20</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="157.5">
@@ -1080,7 +1086,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="6">
         <v>44501</v>
@@ -1092,17 +1098,17 @@
         <v>1</v>
       </c>
       <c r="F4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>23</v>
       </c>
       <c r="H4" s="11"/>
       <c r="I4" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="88.5">
@@ -1110,7 +1116,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="6">
         <v>44136</v>
@@ -1122,25 +1128,25 @@
         <v>2</v>
       </c>
       <c r="F5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>27</v>
       </c>
       <c r="H5" s="12"/>
       <c r="I5" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="60.75">
       <c r="A6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>30</v>
       </c>
       <c r="C6" s="6">
         <v>43770</v>
@@ -1152,25 +1158,25 @@
         <v>1</v>
       </c>
       <c r="F6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="H6" s="13"/>
       <c r="I6" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="J6" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="212.25">
+      <c r="A7" s="5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="168">
-      <c r="A7" s="5" t="s">
+      <c r="B7" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>35</v>
       </c>
       <c r="C7" s="6">
         <v>42795</v>
@@ -1182,25 +1188,25 @@
         <v>2</v>
       </c>
       <c r="F7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>37</v>
       </c>
       <c r="H7" s="14"/>
       <c r="I7" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="J7" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="88.5">
+      <c r="A8" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="75.75">
-      <c r="A8" s="5" t="s">
+      <c r="B8" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>40</v>
       </c>
       <c r="C8" s="6">
         <v>42705</v>
@@ -1212,25 +1218,25 @@
         <v>1</v>
       </c>
       <c r="F8" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="H8" s="15"/>
       <c r="I8" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="J8" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="212.25">
+      <c r="A9" s="5" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="168">
-      <c r="A9" s="5" t="s">
+      <c r="B9" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>45</v>
       </c>
       <c r="C9" s="6">
         <v>40575</v>
@@ -1242,22 +1248,22 @@
         <v>2</v>
       </c>
       <c r="F9" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>46</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>47</v>
       </c>
       <c r="H9" s="16"/>
       <c r="I9" s="5" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="J9" s="9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="156.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="184.5">
       <c r="A10" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>49</v>
@@ -1279,7 +1285,7 @@
       </c>
       <c r="H10" s="17"/>
       <c r="I10" s="5" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="J10" s="9" t="s">
         <v>52</v>
@@ -1287,7 +1293,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="133.5">
       <c r="A11" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>53</v>
@@ -1309,7 +1315,7 @@
       </c>
       <c r="H11" s="18"/>
       <c r="I11" s="5" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="J11" s="9" t="s">
         <v>56</v>
@@ -1335,22 +1341,22 @@
         <v>12</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="H12" s="8"/>
       <c r="I12" s="5" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="214.5">
       <c r="A13" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C13" s="6">
         <v>33117</v>
@@ -1369,18 +1375,18 @@
       </c>
       <c r="H13" s="10"/>
       <c r="I13" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="179.25">
       <c r="A14" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C14" s="6">
         <v>32021</v>
@@ -1392,25 +1398,25 @@
         <v>2</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>23</v>
+        <v>66</v>
       </c>
       <c r="H14" s="11"/>
       <c r="I14" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="J14" s="9" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="40.5">
       <c r="A15" s="5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C15" s="6">
         <v>32295</v>
@@ -1422,25 +1428,25 @@
         <v>3</v>
       </c>
       <c r="F15" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>27</v>
       </c>
       <c r="H15" s="12"/>
       <c r="I15" s="5" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="J15" s="9" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
       <c r="A16" s="5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C16" s="6">
         <v>30926</v>
@@ -1452,25 +1458,25 @@
         <v>2</v>
       </c>
       <c r="F16" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G16" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="H16" s="13"/>
       <c r="I16" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="J16" s="9" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="40.5">
       <c r="A17" s="5" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C17" s="6">
         <v>30682</v>
@@ -1482,25 +1488,25 @@
         <v>1</v>
       </c>
       <c r="F17" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G17" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>37</v>
       </c>
       <c r="H17" s="14"/>
       <c r="I17" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="J17" s="9" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="29.25">
       <c r="A18" s="5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C18" s="6">
         <v>30133</v>
@@ -1512,25 +1518,25 @@
         <v>3</v>
       </c>
       <c r="F18" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G18" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="H18" s="15"/>
       <c r="I18" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="J18" s="9" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
       <c r="A19" s="5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C19" s="6">
         <v>29830</v>
@@ -1542,25 +1548,25 @@
         <v>2</v>
       </c>
       <c r="F19" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G19" s="5" t="s">
         <v>46</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>47</v>
       </c>
       <c r="H19" s="16"/>
       <c r="I19" s="5" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="J19" s="9" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="40.5">
       <c r="A20" s="5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C20" s="6">
         <v>29677</v>
@@ -1579,18 +1585,18 @@
       </c>
       <c r="H20" s="17"/>
       <c r="I20" s="5" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="J20" s="9" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="41.25">
       <c r="A21" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C21" s="6">
         <v>28369</v>
@@ -1602,25 +1608,25 @@
         <v>1</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H21" s="19"/>
       <c r="I21" s="5" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="J21" s="9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="109.5">
       <c r="A22" s="5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C22" s="6">
         <v>39417</v>
@@ -1632,25 +1638,25 @@
         <v>2</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="H22" s="20"/>
       <c r="I22" s="5" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="J22" s="21" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="75.75">
       <c r="A23" s="5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C23" s="6">
         <v>38749</v>
@@ -1662,25 +1668,25 @@
         <v>2</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="H23" s="22"/>
       <c r="I23" s="5" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="J23" s="9" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="63.75">
       <c r="A24" s="5" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C24" s="6">
         <v>38384</v>
@@ -1692,25 +1698,25 @@
         <v>2</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="H24" s="23"/>
       <c r="I24" s="5" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="J24" s="9" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="63.75">
       <c r="A25" s="5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C25" s="6">
         <v>38018</v>
@@ -1722,25 +1728,25 @@
         <v>2</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H25" s="24"/>
       <c r="I25" s="5" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="J25" s="9" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="87.75">
       <c r="A26" s="5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C26" s="6">
         <v>37681</v>
@@ -1752,17 +1758,17 @@
         <v>2</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="H26" s="25"/>
       <c r="I26" s="5" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="J26" s="9" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bizcards are now animating to the top, but not staying there - animationendlistener not firing
</commit_message>
<xml_diff>
--- a/static_content/jobs/jobs.xlsx
+++ b/static_content/jobs/jobs.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10709"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbecker11/workspace-modules/flock-of-postcards/static_content/jobs/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91FC39CB-B793-1647-83E7-3F9384DC1CC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-52600" yWindow="4580" windowWidth="18200" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="jobs"/>
+    <sheet name="jobs" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -56,9 +62,6 @@
   </si>
   <si>
     <t>#006688</t>
-  </si>
-  <si>
-    <t>white</t>
   </si>
   <si>
     <t>• Working as a consulting data engineer in the data cyber security team of the [Cigna Group](url).</t>
@@ -173,9 +176,6 @@
   </si>
   <si>
     <t>#ff4500</t>
-  </si>
-  <si>
-    <t>black</t>
   </si>
   <si>
     <t>• Co-founded a company that envisioned building a web destination where users could easily record and share their favorite pieces of content like facts, authored stories, quotes, articles, chapters, or personal thoughts, as a way of concretely defining their personal mindset.
@@ -428,13 +428,19 @@
 •  Used [Java](url), [ObjectDesign](url), [JavaScript ES3](url), [MySQL 4](url), and [Adobe Photoshop v5.0](url). 
 </t>
   </si>
+  <si>
+    <t>#FFFFFF</t>
+  </si>
+  <si>
+    <t>#000000</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -467,22 +473,22 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF008b8b"/>
+        <fgColor rgb="FF008B8B"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF0000ff"/>
+        <fgColor rgb="FF0000FF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF0000cd"/>
+        <fgColor rgb="FF0000CD"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF8a2be2"/>
+        <fgColor rgb="FF8A2BE2"/>
       </patternFill>
     </fill>
     <fill>
@@ -497,17 +503,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFdc143c"/>
+        <fgColor rgb="FFDC143C"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFff4500"/>
+        <fgColor rgb="FFFF4500"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFffa500"/>
+        <fgColor rgb="FFFFA500"/>
       </patternFill>
     </fill>
     <fill>
@@ -517,32 +523,32 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFffd700"/>
+        <fgColor rgb="FFFFD700"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFffff00"/>
+        <fgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00ff00"/>
+        <fgColor rgb="FF00FF00"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF32cd32"/>
+        <fgColor rgb="FF32CD32"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF6b8e23"/>
+        <fgColor rgb="FF6B8E23"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF228b22"/>
+        <fgColor rgb="FF228B22"/>
       </patternFill>
     </fill>
   </fills>
@@ -581,103 +587,106 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="30">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="7" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="8" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="9" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="10" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="11" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="12" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="13" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="14" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="15" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="16" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="17" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -688,10 +697,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -729,71 +738,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -821,7 +830,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -844,11 +853,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -857,13 +866,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -873,7 +882,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -882,7 +891,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -891,7 +900,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -899,10 +908,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -967,29 +976,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" style="26" width="22.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="26" width="18.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="27" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="27" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="28" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="26" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="26" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="26" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="26" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="29" width="96.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="22.1640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.83203125" style="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="28" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="10.83203125" style="26" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="96" style="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1021,7 +1028,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row r="2" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -1045,18 +1052,18 @@
       </c>
       <c r="H2" s="8"/>
       <c r="I2" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="J2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="129.75">
+    </row>
+    <row r="3" spans="1:10" ht="129.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="6">
         <v>44805</v>
@@ -1068,25 +1075,25 @@
         <v>2</v>
       </c>
       <c r="F3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="H3" s="10"/>
       <c r="I3" s="5" t="s">
-        <v>14</v>
+        <v>111</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="157.5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="157.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" s="6">
         <v>44501</v>
@@ -1098,25 +1105,25 @@
         <v>1</v>
       </c>
       <c r="F4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>22</v>
       </c>
       <c r="H4" s="11"/>
       <c r="I4" s="5" t="s">
-        <v>14</v>
+        <v>111</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="88.5">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="6">
         <v>44136</v>
@@ -1128,25 +1135,25 @@
         <v>2</v>
       </c>
       <c r="F5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>26</v>
       </c>
       <c r="H5" s="12"/>
       <c r="I5" s="5" t="s">
-        <v>14</v>
+        <v>111</v>
       </c>
       <c r="J5" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="60.75">
-      <c r="A6" s="5" t="s">
+      <c r="B6" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>29</v>
       </c>
       <c r="C6" s="6">
         <v>43770</v>
@@ -1158,25 +1165,25 @@
         <v>1</v>
       </c>
       <c r="F6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>31</v>
       </c>
       <c r="H6" s="13"/>
       <c r="I6" s="5" t="s">
-        <v>14</v>
+        <v>111</v>
       </c>
       <c r="J6" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="212.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="212.25">
-      <c r="A7" s="5" t="s">
+      <c r="B7" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>34</v>
       </c>
       <c r="C7" s="6">
         <v>42795</v>
@@ -1188,25 +1195,25 @@
         <v>2</v>
       </c>
       <c r="F7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>36</v>
       </c>
       <c r="H7" s="14"/>
       <c r="I7" s="5" t="s">
-        <v>14</v>
+        <v>111</v>
       </c>
       <c r="J7" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="88.5">
-      <c r="A8" s="5" t="s">
+      <c r="B8" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="C8" s="6">
         <v>42705</v>
@@ -1218,25 +1225,25 @@
         <v>1</v>
       </c>
       <c r="F8" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="H8" s="15"/>
       <c r="I8" s="5" t="s">
-        <v>14</v>
+        <v>111</v>
       </c>
       <c r="J8" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="212.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="212.25">
-      <c r="A9" s="5" t="s">
+      <c r="B9" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>44</v>
       </c>
       <c r="C9" s="6">
         <v>40575</v>
@@ -1248,25 +1255,25 @@
         <v>2</v>
       </c>
       <c r="F9" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>46</v>
       </c>
       <c r="H9" s="16"/>
       <c r="I9" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="184.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="J9" s="9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="184.5">
-      <c r="A10" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>49</v>
       </c>
       <c r="C10" s="6">
         <v>37561</v>
@@ -1278,25 +1285,25 @@
         <v>1</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H10" s="17"/>
       <c r="I10" s="5" t="s">
-        <v>47</v>
+        <v>112</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="133.5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="133.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C11" s="6">
         <v>35827</v>
@@ -1308,25 +1315,25 @@
         <v>1</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H11" s="18"/>
       <c r="I11" s="5" t="s">
-        <v>47</v>
+        <v>112</v>
       </c>
       <c r="J11" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="75.75">
-      <c r="A12" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>58</v>
       </c>
       <c r="C12" s="6">
         <v>35217</v>
@@ -1341,22 +1348,22 @@
         <v>12</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H12" s="8"/>
       <c r="I12" s="5" t="s">
-        <v>47</v>
+        <v>112</v>
       </c>
       <c r="J12" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="214.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="214.5">
-      <c r="A13" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>62</v>
       </c>
       <c r="C13" s="6">
         <v>33117</v>
@@ -1368,25 +1375,25 @@
         <v>2</v>
       </c>
       <c r="F13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="H13" s="10"/>
       <c r="I13" s="5" t="s">
-        <v>14</v>
+        <v>111</v>
       </c>
       <c r="J13" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="179.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="179.25">
-      <c r="A14" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>65</v>
       </c>
       <c r="C14" s="6">
         <v>32021</v>
@@ -1398,25 +1405,25 @@
         <v>2</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H14" s="11"/>
       <c r="I14" s="5" t="s">
-        <v>14</v>
+        <v>111</v>
       </c>
       <c r="J14" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="40.5">
-      <c r="A15" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>69</v>
       </c>
       <c r="C15" s="6">
         <v>32295</v>
@@ -1428,25 +1435,25 @@
         <v>3</v>
       </c>
       <c r="F15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" s="5" t="s">
         <v>25</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>26</v>
       </c>
       <c r="H15" s="12"/>
       <c r="I15" s="5" t="s">
-        <v>47</v>
+        <v>112</v>
       </c>
       <c r="J15" s="9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C16" s="6">
         <v>30926</v>
@@ -1458,25 +1465,25 @@
         <v>2</v>
       </c>
       <c r="F16" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>31</v>
       </c>
       <c r="H16" s="13"/>
       <c r="I16" s="5" t="s">
-        <v>14</v>
+        <v>111</v>
       </c>
       <c r="J16" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="40.5">
-      <c r="A17" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>74</v>
       </c>
       <c r="C17" s="6">
         <v>30682</v>
@@ -1488,25 +1495,25 @@
         <v>1</v>
       </c>
       <c r="F17" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G17" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>36</v>
       </c>
       <c r="H17" s="14"/>
       <c r="I17" s="5" t="s">
-        <v>14</v>
+        <v>111</v>
       </c>
       <c r="J17" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="29.25">
-      <c r="A18" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>77</v>
       </c>
       <c r="C18" s="6">
         <v>30133</v>
@@ -1518,25 +1525,25 @@
         <v>3</v>
       </c>
       <c r="F18" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G18" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="H18" s="15"/>
       <c r="I18" s="5" t="s">
-        <v>14</v>
+        <v>111</v>
       </c>
       <c r="J18" s="9" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C19" s="6">
         <v>29830</v>
@@ -1548,25 +1555,25 @@
         <v>2</v>
       </c>
       <c r="F19" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G19" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>46</v>
       </c>
       <c r="H19" s="16"/>
       <c r="I19" s="5" t="s">
-        <v>47</v>
+        <v>112</v>
       </c>
       <c r="J19" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="40.5">
-      <c r="A20" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>82</v>
       </c>
       <c r="C20" s="6">
         <v>29677</v>
@@ -1578,25 +1585,25 @@
         <v>1</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H20" s="17"/>
       <c r="I20" s="5" t="s">
-        <v>47</v>
+        <v>112</v>
       </c>
       <c r="J20" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="41.25">
-      <c r="A21" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>85</v>
       </c>
       <c r="C21" s="6">
         <v>28369</v>
@@ -1608,25 +1615,25 @@
         <v>1</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H21" s="19"/>
       <c r="I21" s="5" t="s">
-        <v>47</v>
+        <v>112</v>
       </c>
       <c r="J21" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="109.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>88</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="109.5">
-      <c r="A22" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>90</v>
       </c>
       <c r="C22" s="6">
         <v>39417</v>
@@ -1638,25 +1645,25 @@
         <v>2</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H22" s="20"/>
       <c r="I22" s="5" t="s">
-        <v>47</v>
+        <v>112</v>
       </c>
       <c r="J22" s="21" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="75.75">
-      <c r="A23" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>95</v>
       </c>
       <c r="C23" s="6">
         <v>38749</v>
@@ -1668,25 +1675,25 @@
         <v>2</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H23" s="22"/>
       <c r="I23" s="5" t="s">
-        <v>47</v>
+        <v>112</v>
       </c>
       <c r="J23" s="9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>98</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="63.75">
-      <c r="A24" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>100</v>
       </c>
       <c r="C24" s="6">
         <v>38384</v>
@@ -1698,25 +1705,25 @@
         <v>2</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H24" s="23"/>
       <c r="I24" s="5" t="s">
-        <v>47</v>
+        <v>112</v>
       </c>
       <c r="J24" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>103</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="63.75">
-      <c r="A25" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>105</v>
       </c>
       <c r="C25" s="6">
         <v>38018</v>
@@ -1728,25 +1735,25 @@
         <v>2</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H25" s="24"/>
       <c r="I25" s="5" t="s">
-        <v>47</v>
+        <v>112</v>
       </c>
       <c r="J25" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="87.75">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="87.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C26" s="6">
         <v>37681</v>
@@ -1758,17 +1765,17 @@
         <v>2</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H26" s="25"/>
       <c r="I26" s="5" t="s">
-        <v>47</v>
+        <v>112</v>
       </c>
       <c r="J26" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
auto-computing timeline min-max years, and interpolating CURRENT_DATE  in xlsx file
</commit_message>
<xml_diff>
--- a/static_content/jobs/jobs.xlsx
+++ b/static_content/jobs/jobs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbecker11/workspace-modules/flock-of-postcards/static_content/jobs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbecker11/workspace-parallax/flock-of-postcards/static_content/jobs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91FC39CB-B793-1647-83E7-3F9384DC1CC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73B494B0-C665-7B45-A8C0-7C960F5B24BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-52600" yWindow="4580" windowWidth="18200" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="114">
   <si>
     <t>role</t>
   </si>
@@ -433,6 +433,9 @@
   </si>
   <si>
     <t>#000000</t>
+  </si>
+  <si>
+    <t>CURRENT_DATE</t>
   </si>
 </sst>
 </file>
@@ -983,14 +986,15 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.1640625" style="26" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.6640625" style="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.83203125" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" style="27" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="28" bestFit="1" customWidth="1"/>
     <col min="6" max="9" width="10.83203125" style="26" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="96" style="29" bestFit="1" customWidth="1"/>
@@ -1038,8 +1042,8 @@
       <c r="C2" s="6">
         <v>45047</v>
       </c>
-      <c r="D2" s="6">
-        <v>45139</v>
+      <c r="D2" s="6" t="s">
+        <v>113</v>
       </c>
       <c r="E2" s="7">
         <v>3</v>

</xml_diff>

<commit_message>
tagLink spans now visible in both cardDivs and cardDivLineItems
</commit_message>
<xml_diff>
--- a/static_content/jobs/jobs.xlsx
+++ b/static_content/jobs/jobs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbecker11/workspace-parallax/flock-of-postcards/static_content/jobs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48EEB573-DA0D-5840-BB78-F8C15C75695A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB784541-B0DD-1B49-B546-0F5C13E472DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-35080" yWindow="4080" windowWidth="28960" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -112,14 +112,6 @@
     <t>#800000</t>
   </si>
   <si>
-    <t>• As a senior data engineer for SeniorLink a homeservices support platform, helped create [ETL](url) processes using [AWS Kinesis](url), [Python](url), [PySpark](url), and pAWS Data Pipeline](url) to load structured event data from [PostgreSQL](url) databases into a centralized [Redshift warehouse](url). 
-• Saved data as [self-describing data assets](url) in [S3](url) using [AWS Kinesis](url) and [AWS Lambda](url) to aggregate event data into [schema-on-read](url) file formats, [Apache Avro](url), and [Parquet](url).
-• Steered efforts in creating a [Data Lake](url) using [PostgreSQL](url) and [FlyWay](url) with [Python](url) and [PySpark](url) pre-processing on [EC2 instances](url) with [AWS EFS](url), [EBS](url), and [S3](url) storage.
-• Used streaming event messages queued in [RabbitMQ](url) and [AWS Kinesis](url) to build [type-2 slowly changing dimensions]](url) and accumulative facts tables. 
-• Designed and implemented a custom [star-schema warehouse](url) and [ETL](url) processes to [de-normalize](url) and load data into an [AWS Redshift](url) data warehouse for BI reporting using [Tableau](url).
-• [Test-driven development]](url) using [Python](url), [PyCharm](url), [PyTest](url), [GitHub](url), [Jira](url), and [Jenkins CI/CD](url).</t>
-  </si>
-  <si>
     <t xml:space="preserve">Consulting Back-End Engineer </t>
   </si>
   <si>
@@ -142,15 +134,6 @@
   </si>
   <si>
     <t>#ff4500</t>
-  </si>
-  <si>
-    <t>• Co-founded a company that envisioned building a web destination where users could easily record and share their favorite pieces of content like facts, authored stories, quotes, articles, chapters, or personal thoughts, as a way of concretely defining their personal mindset.
-• Implemented [fuzzy matching](url), word clustering](url), [semantic similarity scores](url), and collaborative filtering](url) to help users find content that matched or differed from thieir own mindset.
-• Launched a novel [SaaS](url) using [Amazon Web Services](url) that let individuals and content creators search and share [mindsets](url).
-• Conceptualized patented technology by designing and implementing a fuil-stack consumer-facing [CMS](url) that supported tuned matching among selected attributes.
-• [Java 8](url), [JSP](url), [Servlets](url), [Spring](url), [AWS services](url), [JavaScript](url), [JQuery](url), [HTML5](url), [CSS](url), [JUnit](url), [JMeter](url), JProfile.
-• Utilized [REST](url), [Swagger](url), [Apache Shiro](url), [Eclipse IDE](url), [Maven](url), [Ant](url), [Git](url), [Hibernate](url), [SimpleDB](url), [CentOS Linux](url), [Tomcat](url), [Jetty](url), and [Spring MVC](url).
-• Served as co-founder and co-authored [four patents](url).</t>
   </si>
   <si>
     <t>Sierra Vista Group LLC</t>
@@ -179,262 +162,277 @@
     <t>#008080</t>
   </si>
   <si>
+    <t xml:space="preserve">Lead Software Developer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BuildingBlocks LLC </t>
+  </si>
+  <si>
+    <t>#008b8b</t>
+  </si>
+  <si>
+    <t>Ph.D. Media Arts &amp; Science</t>
+  </si>
+  <si>
+    <t>MIT Media Lab</t>
+  </si>
+  <si>
+    <t>MS Computer Science</t>
+  </si>
+  <si>
+    <t>BYU</t>
+  </si>
+  <si>
+    <t>#0000cd</t>
+  </si>
+  <si>
+    <t>Software Developer</t>
+  </si>
+  <si>
+    <t>Cimmetrix LLC</t>
+  </si>
+  <si>
+    <t>BS Design Engineering Technology</t>
+  </si>
+  <si>
+    <t>• Completed bachelor degree in Design Engineering Technologies
+• Drafting, CAD/CAM, machine design, fluid dynamics, ferrous metallurgy, static load bearing mathematics.</t>
+  </si>
+  <si>
+    <t>Call Center Reservationist</t>
+  </si>
+  <si>
+    <t>Dell Webb Properties</t>
+  </si>
+  <si>
+    <t>Missonary</t>
+  </si>
+  <si>
+    <t>Taiwan Taibei Mission</t>
+  </si>
+  <si>
+    <t>BS GED</t>
+  </si>
+  <si>
+    <t>• Majored in mathematics, took general education required classes as well as design and oil painting.</t>
+  </si>
+  <si>
+    <t>Data Processing</t>
+  </si>
+  <si>
+    <t>Greyhound Corp</t>
+  </si>
+  <si>
+    <t>• Worked as an intern in the Pension Department at Greyhound Corporaate.
+• Manully sorted thousands of pension checks and doing handwriting comparisons to find fraudulent cashing of checks for deceased pensioners.</t>
+  </si>
+  <si>
+    <t>Newspaper Delivery</t>
+  </si>
+  <si>
+    <t>Arizona Republic</t>
+  </si>
+  <si>
+    <t>gold</t>
+  </si>
+  <si>
+    <t>#ffd700</t>
+  </si>
+  <si>
+    <t>• Seven-day paper delivery for the Arizona Republic Newspaper.
+• Weekly collections
+• Used [Schwinn banana seat](url), [Schwinn 10 speed](url).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project Manager / Technical Lead </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MSC </t>
+  </si>
+  <si>
+    <t>yellow</t>
+  </si>
+  <si>
+    <t>#ffff00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consulting Architect </t>
+  </si>
+  <si>
+    <t>Eleven LLC</t>
+  </si>
+  <si>
+    <t>lime</t>
+  </si>
+  <si>
+    <t>#00ff00</t>
+  </si>
+  <si>
+    <t>Consulting Architect</t>
+  </si>
+  <si>
+    <t>Intrusic LLC</t>
+  </si>
+  <si>
+    <t>limegreen</t>
+  </si>
+  <si>
+    <t>#32cd32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consulting Architect / Technical Lead </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMI Entertainment </t>
+  </si>
+  <si>
+    <t>olivedrab</t>
+  </si>
+  <si>
+    <t>#6b8e23</t>
+  </si>
+  <si>
+    <t>Rowe International</t>
+  </si>
+  <si>
+    <t>forestgreen</t>
+  </si>
+  <si>
+    <t>#228b22</t>
+  </si>
+  <si>
+    <t>#FFFFFF</t>
+  </si>
+  <si>
+    <t>#000000</t>
+  </si>
+  <si>
+    <t>CURRENT_DATE</t>
+  </si>
+  <si>
+    <t>• As a consulting data engineer in the data cyber security team of the [Cigna Group](https://www.thecignagroup.com/) created a [REST API](url) using [Postman](https://www.postman.com/) and [OpenAP](https://openapi-generator.tech/)I for pulling credentials from the [CyberArk identity security platform](https://www.cyberark.com/) using [mutual TLS SSL authentication](https://docs.solace.com/Security/Two-Way-SSL-Authentication.htm) with [AWS API Gateway](https://docs.aws.amazon.com/apigateway/). 
+•  Migrated a suite of legacy data pipeline elements running on the [Unity IoC platform](http://unitycontainer.org/articles/introduction.html) to pull credentials from the CyberArk service at runtime rather than using [Fernet](https://cryptography.io/en/latest/fernet/) encrypted local files. 
+•  Upgraded GitHub apps to use [CloudBees/Jenkins](https://docs.aws.amazon.com/apigateway/) CI/CD pipeline for build, applying sofware and cyber-secutity code checks, and on-prem server installation.</t>
+  </si>
+  <si>
+    <t>SeniorLink</t>
+  </si>
+  <si>
+    <t>• [Intrusic LLC](https://www.crunchbase.com/organization/intrusic) built real-time network monitoring systems that identified external and internal network intrusion attempts
+• As a Sierra Vista Group consulting architech, I helped design and develop an approach for buffering live streaming network traffic for asynchronous package processing. 
+• Used [Debian Linux](https://www.debian.org/), [C](https://www.cprogramming.com/books/ritchie.html), and [Visio](https://www.microsoft.com/en-us/microsoft-365/visio/flowchart-software).</t>
+  </si>
+  <si>
+    <t>•  AMI (https://amientertainment.com/) was the internet-music distribution incarnation of Rowe International.  
+•  As a Sierra Vista Group consulting architect and technical lead, I helped design and implement their system for making monthly ACH royalty payments to music copyright owners for mechanical and performance licensing rights.
+•  Used [FileMaker Pro](https://www.claris.com/filemaker/) and [Visio](https://www.microsoft.com/en-us/microsoft-365/visio/flowchart-software).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">•  [Rowe International](https://pitchbook.com/profiles/company/13178-08) was the leading manufacturer of music jukeboxes. 
+•  Sierra Vista Group was consulted to assess their available technologies and create a plan to build their back-end systems to let them become a leading provider of internet-based music.
+•  As consulting architect and technical lead created the project plan and led the development of a full-stack web application used by  jukebox owners and Rowe sales and marketing.
+•  Used Java, [ObjectDesign](https://object.design/), JavaScript , [MySQL](https://www.mysql.com/), and [Adobe Photoshop](https://www.adobe.com/products/photoshop.html). 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• [Eleven LLC](https://www.eleven.net/) built mobile apps used by beverage industry distributors to help manage placement  of their products in the shelves and coolers in retail locations. The work done by the Sierra Vista Group was instrumental in their company being acquired by [Trimble Mobile Solutions](https://help.trimblegeospatial.com/TMM/Home.htm). 
+• As the consulting architect and team lead, we used Java 5 and  [JBoss](https://developers.redhat.com/products/eap/overview) message-oriented middleware platform, [Sybase Anywhere](https://texas.gs.shi.com/Product/30451452/Sybase-SQL-Anywhere-Advanced-Edition) for the client/server based database, and [Windows Mobile 5](https://en.wikipedia.org/wiki/Windows_Mobile_5.0) running on ruggedized mobile devices. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">• MSC, now called [OneCall](https://onecallcm.com/), is a leading workers compensation services company. 
+• As project manager and technical lead for this Sierra Vista Group project, I presented fixed schedule-fixed budget project proposals to C-level executives to add features to their legacy call center system used by 10 different healthcare divisions. 
+• Interviewed stakeholders to create functional requirements and technical spefications for each stage of development.
+• Worked with development team to create work plan, assign tasks.
+• Oversaw quality assurance and customer approval testing.
+• Used the MS Office suite of business apps a well as MS Visio. </t>
+  </si>
+  <si>
+    <t>• Served as a missionary for the Church of Jesus Christ of Latter-day Saints in the [Taiwan Taibei mission](https://www.mymission.com/lds-missions/taiwan-taipei-mission).
+• Served as branch president in the town [Yuli](https://en.wikivoyage.org/wiki/Yuli) in the Hualien County on the east coast of Taiwan.</t>
+  </si>
+  <si>
+    <t>• Worked as a reservations agent for Dell Webb resorts and [houseboat rentals](https://www.lake-powell-country.com/lake-powell-houseboat-history.html) at the various marinas url on [Lake Powell](https://www.lakepowell.com/) in Utah</t>
+  </si>
+  <si>
+    <t>• Front-end software developer of a reverse kinametics path planning system for multi-axis industrial robots.
+• Technologies used include C, [Borne shell](https://en.wikipedia.org/wiki/Bourne_shell), X11 Window System, [Xt toolkit intrinsics](https://en.wikipedia.org/wiki/X_Toolkit_Intrinsics), [Silicon Graphics Irix](https://en.wikipedia.org/wiki/Silicon_Graphics), and [HP-UX](https://en.wikipedia.org/wiki/HP-UX).</t>
+  </si>
+  <si>
+    <t>• Masters of Science degree, Brigham Young University, Provo, Utah
+Took all courses required for both bachelors and masters degrees in Computer Science
+• Thesis project [“Interactive Measurement of Three-Dimensional Objects Using a Depth Buffer &amp; Linear Probe.”](https://dl.acm.org/doi/pdf/10.1145/108360.108446) CS MS Thesis, Shawn Becker, William A. Barrett &amp; Dan R. Olsen, ACM Transactions on Graphics, Vol. 10, No. 2, April 1991
+• Top Research Presentation – New Tech Research Conference - Brigham Young University – Provo, UT – March 1990
+• [“Fast Automated Object Detection Using Signature Parsing.”](https://www.spiedigitallibrary.org/conference-proceedings-of-spie/1192/1/Fast-Automated-Object-Detection-Using-Signature-Parsing/10.1117/12.969720.short) Tim Heaton; Shawn Becker; Kelley Anderson; William Barrett: Proceedings Volume 1192, Intelligent Robots &amp; Computer Vision VIII: Algorithms &amp; Techniques; (1990) https://doi.org/10.1117/12.969720
+• [“Probabilistic Segmentation of Myocardial Tissue by Deterministic Relaxation.”](https://scholarsarchive.byu.edu/cgi/viewcontent.cgi?article=1737&amp;context=facpub) Jerome A. Broekhuijsen, Shawn C. Becker, &amp; William A. Barrett: IEEE Proceedings of Computers in Cardiology, pp. 99-12, Jerusalem, September 1989.
+• [“Interactive Measurement of three-Dimensional Cardiac Morphology.”](https://scholarsarchive.byu.edu/cgi/viewcontent.cgi?article=1736&amp;context=facpub) Shawn C Becker, William A Barrett, October 1989, DOI: 10.1109/CIC.1989.130586, Conference: Computers in Cardiology.</t>
+  </si>
+  <si>
+    <t>•	Doctor of Philosopy degree, Massachusetts Institute of Technology, Cambridge, Massachusettes
+•	Media Laboratory, Media Arts and Sciences
+•	Took courses in machine vision, signals and systems, digital signal processing, and stochastics.
+•	Helped build the operating system for the [Cheops multi-processor system](http://alumni.media.mit.edu/~wad/cheops_CSVT/cheops.html) used for digital video research and for holographic video
+•	[“Vision-assisted modeling for model-based video representations”](https://dspace.mit.edu/handle/1721.1/29123), (Ph.D. Dissertation) MIT, Program in Media Arts &amp; Sciences, 1997
+•	[“Semiautomatic 3-D Model Extraction from Uncalibrated 2-D Camera Views.”](https://www.media.mit.edu/publications/semiautomatic-3-d-model-extraction-from-uncalibrated-2-d-camera-views-2/) S. Becker &amp; V. M. Bove, Jr., Proc. SPIE Image Synthesis, 2410, 1995, pp. 447-461.
+•	“Semiautomatic Scene Modeling From 2-D Views with Partially Known Structure.” Shawn Becker, MIT Media Lab Reports, 1995
+•	“Semiautomatic Camera Lens Calibration from Partially Known Structure”, Shawn Becker, MIT Media Lab Reports, 1994
+•	[“Formulating a scene probability equation to differentiate the effects of shape &amp; albedo on image brightness.”](https://www.researchgate.net/publication/2668457_Formulating_a_Scene_Probability_Equation_to_Differentiate_the_Effects_of_Shape_and_Albedo_on_Image_Brightness) Shawn Becker, MIT Media Lab Reports, 1994
+•	“Computation of some projective-chirplet-transform &amp; metaplectic-chirplet-transform subspaces, with applications in image processing.” Steve Mann &amp; Shawn Becker, DSP World Symposium, Boston, Massachusetts, November 1992.</t>
+  </si>
+  <si>
+    <t>• As lead software developer, built a CD-ROM-based home design application for selecting premium home design products for previewing in the context of images of any household rooms. 
+• Built the prototype using Adobe Photoshop and [Macromedia Director](https://macromedia.fandom.com/wiki/Macromedia_Director).
+• Built the actual application using using Java5 and [Marimba Bongo](https://www.thriftbooks.com/w/official-marimba-guide-to-bongo_danny-goodman/2574616/#edition=58026223&amp;idiq=42367912) widget layout tool.
+• Updates for the self-updating application were delivered over the internet using [Mariba Castanet](https://www.infoworld.com/article/2076707/marimba-launches-new-castanet-with-a-less-java-centric-focus.html) push-technology.</t>
+  </si>
+  <si>
     <t>• As co-founder and CTO, designed and led the development of a public website used by discerning home designers and builders called HomePortfolio.com. 
 • Hired a staff of   10 software and databases developers. 
 • Worked with data acquisition team to scan and tag over 700,000 premium home design products from over 2,000 manufactures and vendors.
 • Designed datamodel and data entry tools for category-specific product attribution. 
 • Helped extended the business model to provide online product selection tools for participating vendors and manufacturers.
 • Instrumental in raising over $70M in venture capital. 
-• Used [Oracle IIi](url), [ATG Dyanamo](url), [Java 8](url), [Akamai](url), [WebTrends](url), [FileMakerPro](url), [ImageMagik](url), and [Omnigraph](url) for data modeling and workflow designs.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lead Software Developer </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BuildingBlocks LLC </t>
-  </si>
-  <si>
-    <t>#008b8b</t>
-  </si>
-  <si>
-    <t>• As lead software developer, built a CD-ROM-based home design application for selecting premium home design products for previewing in the context of images of any household rooms. 
-• Built the prototype using [Adobe Photoshop](url) and [Macromedia Director](url).
-• Built the actual application using using [Java5](url) and [Marimba Bongo](url) widget layout tool.
-• Updates for the self-updating application were delivered over the internet using [Mariba Castanet](url) push-technology.</t>
-  </si>
-  <si>
-    <t>Ph.D. Media Arts &amp; Science</t>
-  </si>
-  <si>
-    <t>MIT Media Lab</t>
-  </si>
-  <si>
-    <t>•	Doctor of Philosopy degree, Massachusetts Institute of Technology, Cambridge, Massachusettes
-•	Media Laboratory, Media Arts and Sciences
-•	Took courses in machine vision, signals and systems, digital signal processing, and stochastics.
-•	Helped build the operating system for the Cheops multi-processor system used for digital video research and for holographic video
-•	“Vision-assisted modeling for model-based video representations”, (Ph.D. Dissertation) MIT, Program in Media Arts &amp; Sciences, 1997
-•	“Semiautomatic 3-D Model Extraction from Uncalibrated 2-D Camera Views.” S. Becker &amp; V. M. Bove, Jr., Proc. SPIE Image Synthesis, 2410, 1995, pp. 447-461.
-•	“Semiautomatic Scene Modeling From 2-D Views with Partially Known Structure.” Shawn Becker, MIT Media Lab Reports, 1995
-•	“Semiautomatic Camera Lens Calibration from Partially Known Structure”, Shawn Becker, MIT Media Lab Reports, 1994
-•	“Formulating a scene probability equation to differentiate the effects of shape &amp; albedo on image brightness.” Shawn Becker, MIT Media Lab Reports, 1994
-•	“Computation of some projective-chirplet-transform &amp; metaplectic-chirplet-transform subspaces, with applications in image processing.” Steve Mann &amp; Shawn Becker, DSP World Symposium, Boston, Massachusetts, November 1992.</t>
-  </si>
-  <si>
-    <t>MS Computer Science</t>
-  </si>
-  <si>
-    <t>BYU</t>
-  </si>
-  <si>
-    <t>#0000cd</t>
-  </si>
-  <si>
-    <t>• Masters of Science degree, Brigham Young University, Provo, Utah
-Took all courses required for both bachelors and masters degrees in Computer Science
-• Thesis project “Interactive Measurement of Three-Dimensional Objects Using a Depth Buffer &amp; Linear Probe.” (CS MS Thesis) Shawn Becker, William A. Barrett &amp; Dan R. Olsen, ACM Transactions on Graphics, Vol. 10, No. 2, April 1991
-• Top Research Presentation – New Tech Research Conference - Brigham Young University – Provo, UT – March 1990
-• “Fast Automated Object Detection Using Signature Parsing.” Tim Heaton; Shawn Becker; Kelley Anderson; William Barrett: Proceedings Volume 1192, Intelligent Robots &amp; Computer Vision VIII: Algorithms &amp; Techniques; (1990) https://doi.org/10.1117/12.969720
-• “Probabilistic Segmentation of Myocardial Tissue by Deterministic Relaxation.” Jerome A. Broekhuijsen, Shawn C. Becker, &amp; William A. Barrett: IEEE Proceedings of Computers in Cardiology, pp. 99-12, Jerusalem, September 1989.
-• “Interactive Measurement of three-Dimensional Cardiac Morphology.” Shawn C Becker, William A Barrett, October 1989, DOI: 10.1109/CIC.1989.130586, Conference: Computers in Cardiology.</t>
-  </si>
-  <si>
-    <t>Software Developer</t>
-  </si>
-  <si>
-    <t>Cimmetrix LLC</t>
-  </si>
-  <si>
-    <t>• Front-end software developer of a reverse kinametics path planning system for multi-axis industrial robots.
-• Technologies used include C, [Borne shell](url), [X11 Window System](url), [Xt toolkit intrinsics](url), [Silicon Graphics Irix](url), and [HP-UX](url).</t>
-  </si>
-  <si>
-    <t>BS Design Engineering Technology</t>
-  </si>
-  <si>
-    <t>• Completed bachelor degree in Design Engineering Technologies
-• Drafting, CAD/CAM, machine design, fluid dynamics, ferrous metallurgy, static load bearing mathematics.</t>
-  </si>
-  <si>
-    <t>Call Center Reservationist</t>
-  </si>
-  <si>
-    <t>Dell Webb Properties</t>
-  </si>
-  <si>
-    <t>• Worked as a reservations agent for Dell Webb [resorts](url) nnd rentals for [skiboats](url) and [houseboats](url) at the various [marinas](url) on [Lake Powell](uirl) in Utah.
-• Made occasional visits in [small aircraft](url).</t>
-  </si>
-  <si>
-    <t>Missonary</t>
-  </si>
-  <si>
-    <t>Taiwan Taibei Mission</t>
-  </si>
-  <si>
-    <t>• Served as a missionary for the Church of Jesus Christ of Latter-day Saints in the Taiwan Taibei mission.
-• Served as branch president in the town Yuli in the Hualien County on the east coast of Taiwan.</t>
-  </si>
-  <si>
-    <t>BS GED</t>
-  </si>
-  <si>
-    <t>• Majored in mathematics, took general education required classes as well as design and oil painting.</t>
-  </si>
-  <si>
-    <t>Data Processing</t>
-  </si>
-  <si>
-    <t>Greyhound Corp</t>
-  </si>
-  <si>
-    <t>• Worked as an intern in the Pension Department at Greyhound Corporaate.
-• Manully sorted thousands of pension checks and doing handwriting comparisons to find fraudulent cashing of checks for deceased pensioners.</t>
-  </si>
-  <si>
-    <t>Newspaper Delivery</t>
-  </si>
-  <si>
-    <t>Arizona Republic</t>
-  </si>
-  <si>
-    <t>gold</t>
-  </si>
-  <si>
-    <t>#ffd700</t>
-  </si>
-  <si>
-    <t>• Seven-day paper delivery for the Arizona Republic Newspaper.
-• Weekly collections
-• Used [Schwinn banana seat](url), [Schwinn 10 speed](url).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Project Manager / Technical Lead </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MSC </t>
-  </si>
-  <si>
-    <t>yellow</t>
-  </si>
-  <si>
-    <t>#ffff00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• MSC, now called [OneCall](url), is a leading workers compensation services company. 
-• As project manager and technical lead for this Sierra Vista Group project, I presented fixed schedule-fixed budget project proposals to C-level executives to add features to their legacy call center system used by 10 different healthcare divisions. 
-• Interviewed stakeholders to create functional requirements and technical spefications for each stage of development.
-• Worked with development team to create work plan, assign tasks.
-• Oversaw quality assurance and customer approval testing.
-• Used the [MS Office](url) suite of business apps a well as [Visio](url). </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Consulting Architect </t>
-  </si>
-  <si>
-    <t>Eleven LLC</t>
-  </si>
-  <si>
-    <t>lime</t>
-  </si>
-  <si>
-    <t>#00ff00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• [Eleven LLC](url) built mobile apps used by beverage industry distributors to help manage placement  of their products in the shelves and coolers in retail locations. The work done by the Sierra Vista Group was instrumental in their company being acquired by [Trimble Mobile Solutions](url). 
-• As the consulting architect and team lead, we used [Java 5](url) and  [JBoss](url) message-oriented middleware platform, [Sybase Anywhere](url) for the client/server based database, and [Windows Mobile 5](url) running on ruggedized mobile devices. </t>
-  </si>
-  <si>
-    <t>Consulting Architect</t>
-  </si>
-  <si>
-    <t>Intrusic LLC</t>
-  </si>
-  <si>
-    <t>limegreen</t>
-  </si>
-  <si>
-    <t>#32cd32</t>
-  </si>
-  <si>
-    <t>• [Intrusic LLC](url) built real-time network monitoring systems that identified external and internal network intrusion attempts
-• As a Sierra Vista Group consulting architech, I helped design and develop an approach for buffering live streaming network traffic for asynchronous package processing. 
-• Used [Debian Linux](url), [C](url), and [Visio](url).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Consulting Architect / Technical Lead </t>
-  </si>
-  <si>
-    <t xml:space="preserve">AMI Entertainment </t>
-  </si>
-  <si>
-    <t>olivedrab</t>
-  </si>
-  <si>
-    <t>#6b8e23</t>
-  </si>
-  <si>
-    <t>•  AMI (America Music Incorporated) was the internet-music distribution incarnation of Rowe International.  
-•  As a Sierra Vista Group consulting architect and technical lead, I helped design and implement their system for making monthly ACH royalty payments to music copyright owners for mechanical and performance licensing rights.
-•  Used [FileMaker Pro](url} and [Visio](url).</t>
-  </si>
-  <si>
-    <t>Rowe International</t>
-  </si>
-  <si>
-    <t>forestgreen</t>
-  </si>
-  <si>
-    <t>#228b22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">•  Rowe International was the leading manufacturer of music jukeboxes. 
-•  Sierra Vista Group was consulted to assess their available technologies and create a plan to build their back-end systems to let them become a leading provider of internet-based music.
-•  As consulting architect and technical lead created the project plan and led the development of a full-stack web application used by  jukebox owners and Rowe sales and marketing.
-•  Used [Java](url), [ObjectDesign](url), [JavaScript ES3](url), [MySQL 4](url), and [Adobe Photoshop v5.0](url). 
-</t>
-  </si>
-  <si>
-    <t>#FFFFFF</t>
-  </si>
-  <si>
-    <t>#000000</t>
-  </si>
-  <si>
-    <t>CURRENT_DATE</t>
-  </si>
-  <si>
-    <t>• As a consulting data engineer in the analytics team of [Warner Brothers Interactive Entertainment](url) Division, I implemented high-volume pipeline integrations shuffling game telemetry and [user PII data](URL) between WB-distributed consumer games and [marketing service platforms](URL) via [Segment customer data platform](url) using [Kafka](url), [Redshift](url), and [Airflow](url). 
-• Employed [Python](url), [Amazon Glue](url) and [Apache Airflow](url) for external [3rd-party integrations](url) and internal [dev-ops integrations](url) with [Jenkins](url), [DataDog](url), and [ZenDesk](url) 
-• Integrated with [Google BigQuery](url) [data warehouse](url) and [AWS-managed services](url) [Airflow](url), [S3](url), [Glue](url), and [Redshift warehouse](url).</t>
-  </si>
-  <si>
-    <t>• As a consulting data engineer for Greenseed Tech, an internet company that provides daily lead reports for independent real-estage agents world-wide, I  [containerized](url) legacy web applications using [Docker](url) and [AWS Secrets Manager](url). 
-• Documented existing data architecture as [ERDs](url) using [DBeaver Enterprise](url). 
-• Used [Selenium](url) and [Python](url) to [screem scrape](url) publicly available data from selected websites.</t>
-  </si>
-  <si>
-    <t>• As a consulting front-end software developer for NuSkin, an international company known for its excellent  skin and beauty products I created new [Vue](url), [Nuxt](url), and [Vuetify](url) components using [NodeJS](url) and [SCSS](url).  
-• [Internationalized](url) content using [Adobe Experience Cloud](url).</t>
-  </si>
-  <si>
-    <t>• As a consulting back-end software developer I sed [AWS microservices](url) for custom voice-based [natural language processing](url) applications.
-• Used [ActiveMQ](url), [Swagger](url), [JSON](url), [Jackson](url), [AOP](url), [Eclipse](url), [Maven](url), [Git](url), [Jira](url), and [Jenkins CI/CD](url).
-• [Java 8](url), [J2EE](url), [Servlets](url), [Spring](url), [SpringBoot](url), [JAX-RS](url), [JUnit](url), [JMeter](url), and [JProfile](url)</t>
+• Used Oracle IIi, [ATG Dyanamo]( https://docs.oracle.com/cd/E24152_01/Platform.10-1/ATGPersBusinessGuide/html/s0102dynamoapplicationframework01.html), Java 8, [Akamai](https://www.akamai.com/), [WebTrends](https://www.webtrends.com/), [FileMakerPro], [ImageMagik](https://imagemagick.org/index.php), and [Omnigraffle](https://www.omnigroup.com/omnigraffle) for data modeling and workflow designs.</t>
+  </si>
+  <si>
+    <t>• Co-founded a company that envisioned building a web destination where users could easily record and share their favorite pieces of content like facts, authored stories, quotes, articles, chapters, or personal thoughts, as a way of concretely defining their personal mindset.
+• Implemented [fuzzy matching](https://nanonets.com/blog/fuzzy-matching-fuzzy-logic/), word clustering](https://www.ilc.cnr.it/EAGLES96/rep2/node37.html#:~:text=Word%20clustering%20is%20a%20technique,to%20information%20retrieval%20and%20filtering.), [semantic similarity scores](https://towardsdatascience.com/semantic-similarity-using-transformers-8f3cb5bf66d6), and collaborative filtering](https://www.hindawi.com/journals/aai/2009/421425/) to help users find content that matched or differed from thieir own mindset.
+• Launched a novel SaaS] using [Amazon Web Services] that let individuals and content creators search and share [mindsets].
+• Conceptualized patented technology by designing and implementing a fuil-stack consumer-facing content management system that supported tuned matching among selected attributes.
+• [Java 8], [JSP], [Servlets], [Spring], [AWS services], [JavaScript], [JQuery], [HTML5], [CSS], [JUnit], [JMeter], JProfile.
+• Utilized [REST], [Swagger], [Apache Shiro](https://shiro.apache.org/), [Eclipse IDE], [Maven], [Ant], [Git], [Hibernate], [AWS SimpleDB](https://aws.amazon.com/simpledb/), [CentOS Linux](https://www.centos.org/), [Apache Tomcat](https://tomcat.apache.org/), [Jetty](https://projects.eclipse.org/projects/rt.jetty), and [Spring MVC](https://docs.spring.io/spring-framework/reference/web/webmvc.html).
+• Served as co-founder and co-authored [four patents].</t>
+  </si>
+  <si>
+    <t>• As a consulting back-end software developer I sed [AWS microservices] for custom voice-based [natural language processing] applications.
+• Used [Apache ActiveMQ](https://activemq.apache.org/), [Swagger](https://swagger.io/), [JSON], [Jackson](url), [AOP](https://www.baeldung.com/spring-aop), [Eclipse], [Maven], [Git], [Jira], and [Jenkins CI/CD].
+• [Java 8], [J2EE], [Servlets], [Spring], [SpringBoot], [JAX-RS], [JUnit], [JMeter], and [JProfile]</t>
+  </si>
+  <si>
+    <t>• As a senior data engineer for SeniorLink a homeservices support platform, helped create [ETL](https://aws.amazon.com/what-is/etl/) processes using [AWS Kinesis], [Python], [PySpark](https://spark.apache.org/), and AWS Data Pipeline](https://docs.aws.amazon.com/datapipeline/latest/DeveloperGuide/what-is-datapipeline.html) to load structured event data from [PostgreSQL] databases into a centralized [Redshift warehouse]. 
+• Saved data as [self-describing data assets] in [S3] using [AWS Kinesis](https://aws.amazon.com/kinesis/) and [AWS Lambda](https://docs.aws.amazon.com/lambda/) to aggregate event data into [schema-on-read] file formats, [Apache Avro](https://avro.apache.org/), and [Apache Parquet](https://parquet.apache.org/).
+• Steered efforts in creating a [Data Lake](url) using [PostgreSQL](url) and [FlyWay](url) with [Python](url) and [PySpark](url) pre-processing on [EC2 instances](url) with [AWS EFS](url), [EBS](url), and [S3](url) storage.
+• Used streaming event messages queued in [RabbitMQ](https://docs.aws.amazon.com/amazon-mq/latest/developer-guide/working-with-rabbitmq.html) and [AWS Kinesis](url) to build [type-2 slowly changing dimensions]](url) and accumulative facts tables. 
+• Designed and implemented a custom [star-schema warehouse](url) and [ETL](url) processes to [de-normalize](url) and load data into an [AWS Redshift](https://aws.amazon.com/redshift/) data warehouse for BI reporting using [Tableau](https://www.tableau.com/).
+• [Test-driven development] using [Python], [PyCharm], [PyTest], [GitHub], [Jira], and [Jenkins CI/CD](https://www.jenkins.io/).</t>
+  </si>
+  <si>
+    <t>• As a consulting front-end software developer for [NuSkin](https://www.nuskin.com/us/en/, an international company known for its excellent  skin and beauty products I created new [Vue.js](https://vuejs.org/), [Nuxt](https://nuxt.com/), and [Vuetify](https://vuetifyjs.com/en/) components using [NodeJS] and [SCSS].  
+• Internationalized content using [Adobe Experience Cloud](https://business.adobe.com/).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• As a consulting data engineer for Greenseed Tech, an internet company that provides daily lead reports for independent real-estage agents world-wide, I  [containerized](url) legacy web applications using [Docker](https://www.docker.com/) and [AWS Secrets Manager](https://aws.amazon.com/secrets-manager/). 
+• Documented existing data architecture as [ERDs] using [DBeaver Enterprise](https://dbeaver.com/dbeaver-enterprise/). </t>
   </si>
   <si>
     <t>• As a consulting data engineer for [Angel Studios](https://www.angel.com/home], a streaming media service that offers family-friendly entertainment that amplifies light, with titles including The Chosen, Dry Bar Comedy, and Tuttle Twins.
-• Used Python, [Pandas](url]), [Numpy](url), [Keras](url), and [Jupyter](url) to build and tune [hyperparameters](url) of a [convolutional neural network](url) with [supervised learning](url) on [AWS Sagemaker](https://aws.amazon.com/pm/sagemaker/) to classify movie frames from episodic programs stored in [S3](url). 
-• Built web client apps using [Python](url) with [Postman](url) that made [RESTful API](url) requests to pull monthly usage data from various web marketing partners like [FaceBook](url), [Google Play](url), and [Vimeo](url). 
-• Worked with [Segment customer data platform](https://segment.com/customer-data-platform/), [Excel](url), and [Tableau](url) to create scheduled [reports] for the company's sales and finance teams.</t>
-  </si>
-  <si>
-    <t>• As a consulting data engineer in the data cyber security team of the [Cigna Group](https://www.thecignagroup.com/) created a [REST API](url) using [Postman](https://www.postman.com/) and [OpenAP](https://openapi-generator.tech/)I for pulling credentials from the [CyberArk identity security platform](https://www.cyberark.com/) using [mutual TLS SSL authentication](https://docs.solace.com/Security/Two-Way-SSL-Authentication.htm) with [AWS API Gateway](https://docs.aws.amazon.com/apigateway/). 
-•  Migrated a suite of legacy data pipeline elements running on the [Unity IoC platform](http://unitycontainer.org/articles/introduction.html) to pull credentials from the CyberArk service at runtime rather than using [Fernet](https://cryptography.io/en/latest/fernet/) encrypted local files. 
-•  Upgraded GitHub apps to use [CloudBees/Jenkins](https://docs.aws.amazon.com/apigateway/) CI/CD pipeline for build, applying sofware and cyber-secutity code checks, and on-prem server installation.</t>
-  </si>
-  <si>
-    <t>SeniorLink</t>
+• Used Python, [Pandas], [Numpy], [Keras], and [Jupyter](https://jupyter.org/) to build and tune hyperparameters of a [convolutional neural network](https://towardsdatascience.com/a-comprehensive-guide-to-convolutional-neural-networks-the-eli5-way-3bd2b1164a53) with [supervised learning] on [AWS Sagemaker](https://aws.amazon.com/pm/sagemaker/) to classify movie frames from episodic programs stored in [S3]. 
+• Built web client apps using [Python] with [Postman](https://www.postman.com/) that made [RESTful API] requests to pull monthly usage data from various web marketing partners like [FaceBook], [Google Play] , and [Vimeo](https://vimeo.com/). 
+• Worked with [Segment customer data platform](https://segment.com/customer-data-platform/), [Excel], and [Tableau] to create scheduled reports for the company's sales and finance teams.</t>
+  </si>
+  <si>
+    <t>• As a consulting data engineer in the analytics team of [Warner Brothers Interactive Entertainment](https://warnerbrosgames.com/) Division, I implemented high-volume pipeline integrations shuffling game telemetry and [user PII data] between WB-distributed consumer games and [marketing service platforms] via [Segment customer data platform](https://segment.com/customer-data-platform/) using [Kafka](https://aws.amazon.com/msk/), [Redshift](https://aws.amazon.com/redshift/), and [Apache Airflow](https://airflow.apache.org). 
+• Employed [Python], [Amazon Glue](https://aws.amazon.com/glue/) and [Apache Airflow](https://airflow.apache.org/) for external [3rd-party integrations] and internal [dev-ops integrations] with [Jenkins], [DataDog](https://www.datadoghq.com/), and [ZenDesk](https://zendesk.com) 
+• Integrated with [Google BigQuery data warehouse](https://cloud.google.com/bigquery) and [AWS-managed services] [Apache Airflow](https://aws.amazon.com/managed-workflows-for-apache-airflow/), [S3](url), [AWS Glue](https://docs.aws.amazon.com/glue/latest/dg/what-is-glue.htmlhttps://docs.aws.amazon.com/glue/latest/dg/what-is-glue.html), and [AWS Redshift warehouse](https://aws.amazon.com/redshift/).</t>
   </si>
 </sst>
 </file>
@@ -987,8 +985,8 @@
   </sheetPr>
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="201" zoomScaleNormal="201" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="201" zoomScaleNormal="201" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1046,7 +1044,7 @@
         <v>45047</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="E2" s="8">
         <v>3</v>
@@ -1059,13 +1057,13 @@
       </c>
       <c r="H2" s="9"/>
       <c r="I2" s="6" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="128" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="192" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>10</v>
       </c>
@@ -1089,13 +1087,13 @@
       </c>
       <c r="H3" s="11"/>
       <c r="I3" s="6" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="144" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="160" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
@@ -1119,10 +1117,10 @@
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="6" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="64" x14ac:dyDescent="0.2">
@@ -1149,13 +1147,13 @@
       </c>
       <c r="H5" s="13"/>
       <c r="I5" s="6" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>23</v>
       </c>
@@ -1179,18 +1177,18 @@
       </c>
       <c r="H6" s="14"/>
       <c r="I6" s="6" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="208" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="272" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="C7" s="7">
         <v>42795</v>
@@ -1209,18 +1207,18 @@
       </c>
       <c r="H7" s="15"/>
       <c r="I7" s="6" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="J7" s="10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="96" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+      <c r="B8" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="C8" s="7">
         <v>42705</v>
@@ -1232,25 +1230,25 @@
         <v>1</v>
       </c>
       <c r="F8" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>34</v>
       </c>
       <c r="H8" s="16"/>
       <c r="I8" s="6" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="224" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="288" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>36</v>
       </c>
       <c r="C9" s="7">
         <v>40575</v>
@@ -1262,25 +1260,25 @@
         <v>2</v>
       </c>
       <c r="F9" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="6" t="s">
         <v>37</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>38</v>
       </c>
       <c r="H9" s="17"/>
       <c r="I9" s="6" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>39</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="176" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C10" s="7">
         <v>37561</v>
@@ -1292,25 +1290,25 @@
         <v>1</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H10" s="18"/>
       <c r="I10" s="6" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="160" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="208" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C11" s="7">
         <v>35827</v>
@@ -1322,25 +1320,25 @@
         <v>1</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H11" s="19"/>
       <c r="I11" s="6" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="144" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C12" s="7">
         <v>35217</v>
@@ -1355,22 +1353,22 @@
         <v>12</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H12" s="9"/>
       <c r="I12" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="J12" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="J12" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="256" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:10" ht="304" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C13" s="7">
         <v>33117</v>
@@ -1389,18 +1387,18 @@
       </c>
       <c r="H13" s="11"/>
       <c r="I13" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="J13" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="J13" s="10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="192" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:10" ht="256" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C14" s="7">
         <v>32021</v>
@@ -1415,22 +1413,22 @@
         <v>18</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="H14" s="12"/>
       <c r="I14" s="6" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C15" s="7">
         <v>32295</v>
@@ -1449,18 +1447,18 @@
       </c>
       <c r="H15" s="13"/>
       <c r="I15" s="6" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>61</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C16" s="7">
         <v>30926</v>
@@ -1479,18 +1477,18 @@
       </c>
       <c r="H16" s="14"/>
       <c r="I16" s="6" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C17" s="7">
         <v>30682</v>
@@ -1509,18 +1507,18 @@
       </c>
       <c r="H17" s="15"/>
       <c r="I17" s="6" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C18" s="7">
         <v>30133</v>
@@ -1532,25 +1530,25 @@
         <v>3</v>
       </c>
       <c r="F18" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G18" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>34</v>
       </c>
       <c r="H18" s="16"/>
       <c r="I18" s="6" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>69</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C19" s="7">
         <v>29830</v>
@@ -1562,25 +1560,25 @@
         <v>2</v>
       </c>
       <c r="F19" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G19" s="6" t="s">
         <v>37</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>38</v>
       </c>
       <c r="H19" s="17"/>
       <c r="I19" s="6" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C20" s="7">
         <v>29677</v>
@@ -1592,25 +1590,25 @@
         <v>1</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H20" s="18"/>
       <c r="I20" s="6" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C21" s="7">
         <v>28369</v>
@@ -1622,25 +1620,25 @@
         <v>1</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="H21" s="20"/>
       <c r="I21" s="6" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="112" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C22" s="7">
         <v>39417</v>
@@ -1652,25 +1650,25 @@
         <v>2</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="H22" s="21"/>
       <c r="I22" s="6" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="J22" s="22" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="128" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C23" s="7">
         <v>38749</v>
@@ -1682,25 +1680,25 @@
         <v>2</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="H23" s="23"/>
       <c r="I23" s="6" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="J23" s="10" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="C24" s="7">
         <v>38384</v>
@@ -1712,25 +1710,25 @@
         <v>2</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="H24" s="24"/>
       <c r="I24" s="6" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="C25" s="7">
         <v>38018</v>
@@ -1742,25 +1740,25 @@
         <v>2</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="H25" s="25"/>
       <c r="I25" s="6" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="J25" s="10" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="112" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="144" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="C26" s="7">
         <v>37681</v>
@@ -1772,17 +1770,17 @@
         <v>2</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="H26" s="26"/>
       <c r="I26" s="6" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
geo and img icons on newline when added to cardivs and in-line when added to cardDivLineItems, and icon color set to match parent element
</commit_message>
<xml_diff>
--- a/static_content/jobs/jobs.xlsx
+++ b/static_content/jobs/jobs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbecker11/workspace-parallax/flock-of-postcards/static_content/jobs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB784541-B0DD-1B49-B546-0F5C13E472DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8343E8F-4FC6-9245-95C1-496A02EFE131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35080" yWindow="4080" windowWidth="28960" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-50480" yWindow="7120" windowWidth="28960" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="jobs" sheetId="1" r:id="rId1"/>
@@ -310,11 +310,6 @@
     <t>CURRENT_DATE</t>
   </si>
   <si>
-    <t>• As a consulting data engineer in the data cyber security team of the [Cigna Group](https://www.thecignagroup.com/) created a [REST API](url) using [Postman](https://www.postman.com/) and [OpenAP](https://openapi-generator.tech/)I for pulling credentials from the [CyberArk identity security platform](https://www.cyberark.com/) using [mutual TLS SSL authentication](https://docs.solace.com/Security/Two-Way-SSL-Authentication.htm) with [AWS API Gateway](https://docs.aws.amazon.com/apigateway/). 
-•  Migrated a suite of legacy data pipeline elements running on the [Unity IoC platform](http://unitycontainer.org/articles/introduction.html) to pull credentials from the CyberArk service at runtime rather than using [Fernet](https://cryptography.io/en/latest/fernet/) encrypted local files. 
-•  Upgraded GitHub apps to use [CloudBees/Jenkins](https://docs.aws.amazon.com/apigateway/) CI/CD pipeline for build, applying sofware and cyber-secutity code checks, and on-prem server installation.</t>
-  </si>
-  <si>
     <t>SeniorLink</t>
   </si>
   <si>
@@ -394,15 +389,6 @@
 • Used Oracle IIi, [ATG Dyanamo]( https://docs.oracle.com/cd/E24152_01/Platform.10-1/ATGPersBusinessGuide/html/s0102dynamoapplicationframework01.html), Java 8, [Akamai](https://www.akamai.com/), [WebTrends](https://www.webtrends.com/), [FileMakerPro], [ImageMagik](https://imagemagick.org/index.php), and [Omnigraffle](https://www.omnigroup.com/omnigraffle) for data modeling and workflow designs.</t>
   </si>
   <si>
-    <t>• Co-founded a company that envisioned building a web destination where users could easily record and share their favorite pieces of content like facts, authored stories, quotes, articles, chapters, or personal thoughts, as a way of concretely defining their personal mindset.
-• Implemented [fuzzy matching](https://nanonets.com/blog/fuzzy-matching-fuzzy-logic/), word clustering](https://www.ilc.cnr.it/EAGLES96/rep2/node37.html#:~:text=Word%20clustering%20is%20a%20technique,to%20information%20retrieval%20and%20filtering.), [semantic similarity scores](https://towardsdatascience.com/semantic-similarity-using-transformers-8f3cb5bf66d6), and collaborative filtering](https://www.hindawi.com/journals/aai/2009/421425/) to help users find content that matched or differed from thieir own mindset.
-• Launched a novel SaaS] using [Amazon Web Services] that let individuals and content creators search and share [mindsets].
-• Conceptualized patented technology by designing and implementing a fuil-stack consumer-facing content management system that supported tuned matching among selected attributes.
-• [Java 8], [JSP], [Servlets], [Spring], [AWS services], [JavaScript], [JQuery], [HTML5], [CSS], [JUnit], [JMeter], JProfile.
-• Utilized [REST], [Swagger], [Apache Shiro](https://shiro.apache.org/), [Eclipse IDE], [Maven], [Ant], [Git], [Hibernate], [AWS SimpleDB](https://aws.amazon.com/simpledb/), [CentOS Linux](https://www.centos.org/), [Apache Tomcat](https://tomcat.apache.org/), [Jetty](https://projects.eclipse.org/projects/rt.jetty), and [Spring MVC](https://docs.spring.io/spring-framework/reference/web/webmvc.html).
-• Served as co-founder and co-authored [four patents].</t>
-  </si>
-  <si>
     <t>• As a consulting back-end software developer I sed [AWS microservices] for custom voice-based [natural language processing] applications.
 • Used [Apache ActiveMQ](https://activemq.apache.org/), [Swagger](https://swagger.io/), [JSON], [Jackson](url), [AOP](https://www.baeldung.com/spring-aop), [Eclipse], [Maven], [Git], [Jira], and [Jenkins CI/CD].
 • [Java 8], [J2EE], [Servlets], [Spring], [SpringBoot], [JAX-RS], [JUnit], [JMeter], and [JProfile]</t>
@@ -433,6 +419,20 @@
     <t>• As a consulting data engineer in the analytics team of [Warner Brothers Interactive Entertainment](https://warnerbrosgames.com/) Division, I implemented high-volume pipeline integrations shuffling game telemetry and [user PII data] between WB-distributed consumer games and [marketing service platforms] via [Segment customer data platform](https://segment.com/customer-data-platform/) using [Kafka](https://aws.amazon.com/msk/), [Redshift](https://aws.amazon.com/redshift/), and [Apache Airflow](https://airflow.apache.org). 
 • Employed [Python], [Amazon Glue](https://aws.amazon.com/glue/) and [Apache Airflow](https://airflow.apache.org/) for external [3rd-party integrations] and internal [dev-ops integrations] with [Jenkins], [DataDog](https://www.datadoghq.com/), and [ZenDesk](https://zendesk.com) 
 • Integrated with [Google BigQuery data warehouse](https://cloud.google.com/bigquery) and [AWS-managed services] [Apache Airflow](https://aws.amazon.com/managed-workflows-for-apache-airflow/), [S3](url), [AWS Glue](https://docs.aws.amazon.com/glue/latest/dg/what-is-glue.htmlhttps://docs.aws.amazon.com/glue/latest/dg/what-is-glue.html), and [AWS Redshift warehouse](https://aws.amazon.com/redshift/).</t>
+  </si>
+  <si>
+    <t>• As a consulting data engineer in the data cyber security team of the [Cigna Group](https://www.thecignagroup.com/) created a [REST API](url) using [Postman](https://www.postman.com/) and [OpenAP](https://openapi-generator.tech/) for pulling credentials from the [CyberArk identity security platform](https://www.cyberark.com/) using [mutual TLS SSL authentication](https://docs.solace.com/Security/Two-Way-SSL-Authentication.htm) with [AWS API Gateway](https://docs.aws.amazon.com/apigateway/). 
+•  Migrated a suite of legacy data pipeline elements running on the [Unity IoC platform](http://unitycontainer.org/articles/introduction.html) to pull credentials from the CyberArk service at runtime rather than using [Fernet](https://cryptography.io/en/latest/fernet/) encrypted local files. 
+•  Upgraded GitHub apps to use [CloudBees/Jenkins](https://docs.aws.amazon.com/apigateway/) CI/CD pipeline for build, applying sofware and cyber-secutity code checks, and on-prem server installation.</t>
+  </si>
+  <si>
+    <t>• Co-founded a company that envisioned building a web destination where users could easily record and share their favorite pieces of content like facts, authored stories, quotes, articles, chapters, or personal thoughts, as a way of concretely defining their personal mindset.
+• Implemented [fuzzy matching](https://nanonets.com/blog/fuzzy-matching-fuzzy-logic/), [word clustering](https://www.ilc.cnr.it/EAGLES96/rep2/node37.html#:~:text=Word%20clustering%20is%20a%20technique,to%20information%20retrieval%20and%20filtering.), [semantic similarity scores](https://towardsdatascience.com/semantic-similarity-using-transformers-8f3cb5bf66d6), and [collaborative filtering](https://www.hindawi.com/journals/aai/2009/421425/) to help users find content that matched or differed from thieir own mindset.
+• Launched a novel [SaaS] using [Amazon Web Services] that let individuals and content creators search and share [mindsets].
+• Conceptualized patented technology by designing and implementing a fuil-stack consumer-facing content management system that supported tuned matching among selected attributes.
+• [Java 8], [JSP], [Servlets], [Spring], [AWS services], [JavaScript], [JQuery], [HTML5], [CSS], [JUnit], [JMeter], [JProfile].
+• Utilized [REST], [Swagger], [Apache Shiro](https://shiro.apache.org/), [Eclipse IDE], [Maven], [Ant], [Git], [Hibernate], [AWS SimpleDB](https://aws.amazon.com/simpledb/), [CentOS Linux](https://www.centos.org/), [Apache Tomcat](https://tomcat.apache.org/), [Jetty](https://projects.eclipse.org/projects/rt.jetty), and [Spring MVC](https://docs.spring.io/spring-framework/reference/web/webmvc.html).
+• Served as co-founder and co-authored [four patents].</t>
   </si>
 </sst>
 </file>
@@ -985,8 +985,8 @@
   </sheetPr>
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="201" zoomScaleNormal="201" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="I8" zoomScale="201" zoomScaleNormal="201" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1060,7 +1060,7 @@
         <v>90</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>93</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="192" x14ac:dyDescent="0.2">
@@ -1090,7 +1090,7 @@
         <v>90</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="160" x14ac:dyDescent="0.2">
@@ -1120,7 +1120,7 @@
         <v>90</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="64" x14ac:dyDescent="0.2">
@@ -1150,7 +1150,7 @@
         <v>90</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="64" x14ac:dyDescent="0.2">
@@ -1180,7 +1180,7 @@
         <v>90</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="272" x14ac:dyDescent="0.2">
@@ -1188,7 +1188,7 @@
         <v>27</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C7" s="7">
         <v>42795</v>
@@ -1210,7 +1210,7 @@
         <v>90</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="80" x14ac:dyDescent="0.2">
@@ -1240,7 +1240,7 @@
         <v>90</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="288" x14ac:dyDescent="0.2">
@@ -1270,7 +1270,7 @@
         <v>91</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="176" x14ac:dyDescent="0.2">
@@ -1330,7 +1330,7 @@
         <v>91</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="144" x14ac:dyDescent="0.2">
@@ -1360,7 +1360,7 @@
         <v>91</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="304" x14ac:dyDescent="0.2">
@@ -1390,7 +1390,7 @@
         <v>90</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="256" x14ac:dyDescent="0.2">
@@ -1420,7 +1420,7 @@
         <v>90</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="64" x14ac:dyDescent="0.2">
@@ -1450,7 +1450,7 @@
         <v>91</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="32" x14ac:dyDescent="0.2">
@@ -1510,7 +1510,7 @@
         <v>90</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="64" x14ac:dyDescent="0.2">
@@ -1540,7 +1540,7 @@
         <v>90</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -1660,7 +1660,7 @@
         <v>91</v>
       </c>
       <c r="J22" s="22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="128" x14ac:dyDescent="0.2">
@@ -1690,7 +1690,7 @@
         <v>91</v>
       </c>
       <c r="J23" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="96" x14ac:dyDescent="0.2">
@@ -1720,7 +1720,7 @@
         <v>91</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="80" x14ac:dyDescent="0.2">
@@ -1750,7 +1750,7 @@
         <v>91</v>
       </c>
       <c r="J25" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="144" x14ac:dyDescent="0.2">
@@ -1780,7 +1780,7 @@
         <v>91</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
icons still wrong colors
</commit_message>
<xml_diff>
--- a/static_content/jobs/jobs.xlsx
+++ b/static_content/jobs/jobs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbecker11/workspace-parallax/flock-of-postcards/static_content/jobs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90786B78-D38F-A44A-80C2-9429D6EF1314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28DAFEB7-841F-B44A-B581-545A41BF9123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-50600" yWindow="7060" windowWidth="28960" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-45560" yWindow="7320" windowWidth="28960" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="jobs" sheetId="1" r:id="rId1"/>
@@ -215,10 +215,6 @@
     <t>Greyhound Corp</t>
   </si>
   <si>
-    <t>• Worked as an intern in the Pension Department at Greyhound Corporaate.
-• Manully sorted thousands of pension checks and doing handwriting comparisons to find fraudulent cashing of checks for deceased pensioners.</t>
-  </si>
-  <si>
     <t>Newspaper Delivery</t>
   </si>
   <si>
@@ -229,11 +225,6 @@
   </si>
   <si>
     <t>#ffd700</t>
-  </si>
-  <si>
-    <t>• Seven-day paper delivery for the Arizona Republic Newspaper.
-• Weekly collections
-• Used [Schwinn banana seat](url), [Schwinn 10 speed](url).</t>
   </si>
   <si>
     <t xml:space="preserve">Project Manager / Technical Lead </t>
@@ -333,19 +324,59 @@
 • Served as branch president in the town [Yuli](https://en.wikivoyage.org/wiki/Yuli) in the Hualien County on the east coast of Taiwan.</t>
   </si>
   <si>
-    <t>• Worked as a reservations agent for Dell Webb resorts and [houseboat rentals](https://www.lake-powell-country.com/lake-powell-houseboat-history.html) at the various marinas url on [Lake Powell](https://www.lakepowell.com/) in Utah</t>
-  </si>
-  <si>
-    <t>• Masters of Science degree, Brigham Young University, Provo, Utah
-Took all courses required for both bachelors and masters degrees in Computer Science
-• Thesis project [“Interactive Measurement of Three-Dimensional Objects Using a Depth Buffer &amp; Linear Probe.”](https://dl.acm.org/doi/pdf/10.1145/108360.108446) CS MS Thesis, Shawn Becker, William A. Barrett &amp; Dan R. Olsen, ACM Transactions on Graphics, Vol. 10, No. 2, April 1991
-• Top Research Presentation – New Tech Research Conference - Brigham Young University – Provo, UT – March 1990
-• [“Fast Automated Object Detection Using Signature Parsing.”](https://www.spiedigitallibrary.org/conference-proceedings-of-spie/1192/1/Fast-Automated-Object-Detection-Using-Signature-Parsing/10.1117/12.969720.short) Tim Heaton; Shawn Becker; Kelley Anderson; William Barrett: Proceedings Volume 1192, Intelligent Robots &amp; Computer Vision VIII: Algorithms &amp; Techniques; (1990) https://doi.org/10.1117/12.969720
-• [“Probabilistic Segmentation of Myocardial Tissue by Deterministic Relaxation.”](https://scholarsarchive.byu.edu/cgi/viewcontent.cgi?article=1737&amp;context=facpub) Jerome A. Broekhuijsen, Shawn C. Becker, &amp; William A. Barrett: IEEE Proceedings of Computers in Cardiology, pp. 99-12, Jerusalem, September 1989.
-• [“Interactive Measurement of three-Dimensional Cardiac Morphology.”](https://scholarsarchive.byu.edu/cgi/viewcontent.cgi?article=1736&amp;context=facpub) Shawn C Becker, William A Barrett, October 1989, DOI: 10.1109/CIC.1989.130586, Conference: Computers in Cardiology.</t>
-  </si>
-  <si>
-    <t>•	Doctor of Philosopy degree, Massachusetts Institute of Technology, Cambridge, Massachusettes
+    <t>• As lead software developer, built a CD-ROM-based home design application for selecting premium home design products for previewing in the context of images of any household rooms. 
+• Built the prototype using Adobe Photoshop and [Macromedia Director](https://macromedia.fandom.com/wiki/Macromedia_Director).
+• Built the actual application using using Java5 and [Marimba Bongo](https://www.thriftbooks.com/w/official-marimba-guide-to-bongo_danny-goodman/2574616/#edition=58026223&amp;idiq=42367912) widget layout tool.
+• Updates for the self-updating application were delivered over the internet using [Mariba Castanet](https://www.infoworld.com/article/2076707/marimba-launches-new-castanet-with-a-less-java-centric-focus.html) push-technology.</t>
+  </si>
+  <si>
+    <t>• As a consulting front-end software developer for [NuSkin](https://www.nuskin.com/us/en/, an international company known for its excellent  skin and beauty products I created new [Vue.js](https://vuejs.org/), [Nuxt](https://nuxt.com/), and [Vuetify](https://vuetifyjs.com/en/) components using [NodeJS] and [SCSS].  
+• Internationalized content using [Adobe Experience Cloud](https://business.adobe.com/).</t>
+  </si>
+  <si>
+    <t>• As a consulting data engineer in the data cyber security team of the [Cigna Group](https://www.thecignagroup.com/) created a [REST API](url) using [Postman](https://www.postman.com/) and [OpenAP](https://openapi-generator.tech/) for pulling credentials from the [CyberArk identity security platform](https://www.cyberark.com/) using [mutual TLS SSL authentication](https://docs.solace.com/Security/Two-Way-SSL-Authentication.htm) with [AWS API Gateway](https://docs.aws.amazon.com/apigateway/). 
+•  Migrated a suite of legacy data pipeline elements running on the [Unity IoC platform](http://unitycontainer.org/articles/introduction.html) to pull credentials from the CyberArk service at runtime rather than using [Fernet](https://cryptography.io/en/latest/fernet/) encrypted local files. 
+•  Upgraded GitHub apps to use [CloudBees/Jenkins](https://docs.aws.amazon.com/apigateway/) CI/CD pipeline for build, applying sofware and cyber-secutity code checks, and on-prem server installation.</t>
+  </si>
+  <si>
+    <t>• [Intrusic LLC](https://www.crunchbase.com/organization/intrusic) built real-time network monitoring systems that identified external and internal network intrusion attempts
+• As a Sierra Vista Group consulting architech, I helped design and develop an approach for buffering live streaming network traffic for asynchronous package processing. 
+• Used [Debian Linux](https://www.debian.org/), [C programming language](https://www.cprogramming.com/books/ritchie.html), and [Visio](https://www.microsoft.com/en-us/microsoft-365/visio/flowchart-software).</t>
+  </si>
+  <si>
+    <t>• As a consulting data engineer in the analytics team of [Warner Brothers Interactive Entertainment](https://warnerbrosgames.com/) Division, I implemented high-volume pipeline integrations shuffling game telemetry and [user PII data] between WB-distributed consumer games and [marketing service platforms] via [Segment customer data platform](https://segment.com/customer-data-platform/) using [Kafka](https://aws.amazon.com/msk/), [Redshift](https://aws.amazon.com/redshift/), and [Apache Airflow](https://airflow.apache.org). 
+• Employed [Python], [Amazon Glue](https://aws.amazon.com/glue/) and [Apache Airflow](https://airflow.apache.org/) for external [3rd-party integrations] and internal [dev-ops integrations] with [Jenkins], [DataDog](https://www.datadoghq.com/), and [ZenDesk](https://zendesk.com) 
+• Integrated with [Google BigQuery data warehouse](https://cloud.google.com/bigquery) and [AWS-managed services] [Apache Airflow](https://aws.amazon.com/managed-workflows-for-apache-airflow/), [S3], [AWS Glue](https://towardsdatascience.com/extract-transform-load-etl-aws-glue-edd383218cfd), and [AWS Redshift warehouse](https://aws.amazon.com/redshift/).</t>
+  </si>
+  <si>
+    <t>• As a consulting data engineer for [Angel Studios](https://www.angel.com/home], a streaming media service that offers family-friendly entertainment that amplifies light, with titles including The Chosen, Dry Bar Comedy, and Tuttle Twins.
+• Used Python, [Pandas], [Numpy], [Keras], and [Jupyter](https://jupyter.org/) to build and tune hyperparameters of a [convolutional neural network](https://towardsdatascience.com/a-comprehensive-guide-to-convolutional-neural-networks-the-eli5-way-3bd2b1164a53) with [supervised learning] on [AWS Sagemaker](https://aws.amazon.com/pm/sagemaker/) to classify movie frames from episodic programs stored in [Amazon S3](https://aws.amazon.com/s3/storage-classes). 
+• Built web client apps using [Python] with [Postman](https://www.postman.com/) that made [RESTful API] requests to pull monthly usage data from various web marketing partners like [FaceBook Marketing](https://www.quora.com/What-is-Facebook-Marketing-1), [Google Play](https://play.google/howplayworks/) , and [Vimeo](https://vimeo.com/). 
+• Worked with [Segment customer data platform](https://segment.com/customer-data-platform/), [Excel], and [Tableau] to create scheduled reports for the company's sales and finance teams.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• As a consulting data engineer for Greenseed Tech, an internet company that provides daily lead reports for independent real-estage agents world-wide, I  [containerized] legacy web applications using [Docker](https://www.docker.com/) and [AWS Secrets Manager](https://aws.amazon.com/secrets-manager/). 
+• Documented existing data architecture as [ERDs](https://www.lucidchart.com/pages/er-diagrams) using [DBeaver Enterprise](https://dbeaver.com/dbeaver-enterprise/). </t>
+  </si>
+  <si>
+    <t>• Co-founded a finance and technology boutique called [Sierra Vista Group](https://6sense.com/company/sierra-vista-group-llc/5ba8a5247c8666394376fc4f) that delivered support in planning and proposing effective IT strategies for key clients in several industries. 
+• Performed various services, including system and architecture assessment and solutions design, to ensure the smooth running of technical projects.
+• Managed project schedules and technical specifications to match business requirements within contractual budget constraints. 
+• Identified opportunities for potential clients requiring expertise in product development, software engineering, and data modeling. Negotiated and communicated with c-level client management regarding project milestone agreements.
+• Increased ROI for each client’s project by hiring and managing contractors to deliver custom software solutions.
+• Delivered high-level leadership and guidance to a team of software engineering consultants for several projects to accelerate operational excellence.</t>
+  </si>
+  <si>
+    <t>• As co-founder and CTO, designed and led the development of a public website used by discerning home designers and builders called [HomePortfolio.com](https://homeportfolio.com/). 
+• Hired a staff of   10 software and databases developers. 
+• Worked with data acquisition team to scan and tag over 700,000 premium home design products from over 2,000 manufactures and vendors.
+• Designed datamodel and data entry tools for category-specific product attribution. 
+• Helped extended the business model to provide online product selection tools for participating vendors and manufacturers.
+• Instrumental in raising over $70M in venture capital. 
+• Used Oracle IIi, [ATG Dyanamo]( https://docs.oracle.com/cd/E24152_01/Platform.10-1/ATGPersBusinessGuide/html/s0102dynamoapplicationframework01.html), Java 8, [Akamai]{https://www.hiclipart.com/free-transparent-background-png-clipart-zkmsn}(https://www.akamai.com/), [WebTrends](https://www.webtrends.com/), [FileMakerPro], [ImageMagik](https://imagemagick.org/index.php), and [Omnigraffle](https://www.omnigroup.com/omnigraffle) for data modeling and workflow designs.</t>
+  </si>
+  <si>
+    <t>•	Doctor of Philosopy degree, [Massachusetts Institute of Technology]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/MIT-logo.png}, Cambridge, Massachusettes
 •	Media Laboratory, Media Arts and Sciences
 •	Took courses in machine vision, signals and systems, digital signal processing, and stochastics.
 •	Helped build the operating system for the [Cheops multi-processor system](http://alumni.media.mit.edu/~wad/cheops_CSVT/cheops.html) used for digital video research and for holographic video
@@ -357,47 +388,33 @@
 •	“Computation of some projective-chirplet-transform &amp; metaplectic-chirplet-transform subspaces, with applications in image processing.” Steve Mann &amp; Shawn Becker, DSP World Symposium, Boston, Massachusetts, November 1992.</t>
   </si>
   <si>
-    <t>• As lead software developer, built a CD-ROM-based home design application for selecting premium home design products for previewing in the context of images of any household rooms. 
-• Built the prototype using Adobe Photoshop and [Macromedia Director](https://macromedia.fandom.com/wiki/Macromedia_Director).
-• Built the actual application using using Java5 and [Marimba Bongo](https://www.thriftbooks.com/w/official-marimba-guide-to-bongo_danny-goodman/2574616/#edition=58026223&amp;idiq=42367912) widget layout tool.
-• Updates for the self-updating application were delivered over the internet using [Mariba Castanet](https://www.infoworld.com/article/2076707/marimba-launches-new-castanet-with-a-less-java-centric-focus.html) push-technology.</t>
-  </si>
-  <si>
-    <t>• As a consulting back-end software developer I sed [AWS microservices] for custom voice-based [natural language processing] applications.
+    <t>• Front-end software developer of a reverse kinametics path planning system for multi-axis industrial robots for [Cimmetrix]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/Cimetrix-PDF-combined-logo-150x100.png}.
+• Technologies used include [C programming language], [Borne shell](https://en.wikipedia.org/wiki/Bourne_shell), X11 Window System, [Xt toolkit intrinsics](https://en.wikipedia.org/wiki/X_Toolkit_Intrinsics), [Silicon Graphics Irix](https://en.wikipedia.org/wiki/Silicon_Graphics), and [HP-UX](https://en.wikipedia.org/wiki/HP-UX).</t>
+  </si>
+  <si>
+    <t>• Masters of Science degree, [Brigham Young University]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/BYU-entrance-150x150.jpg}, Provo, Utah
+Took all courses required for both bachelors and masters degrees in Computer Science
+• Thesis project [“Interactive Measurement of Three-Dimensional Objects Using a Depth Buffer &amp; Linear Probe.”](https://dl.acm.org/doi/pdf/10.1145/108360.108446) CS MS Thesis, Shawn Becker, William A. Barrett &amp; Dan R. Olsen, ACM Transactions on Graphics, Vol. 10, No. 2, April 1991
+• Top Research Presentation – New Tech Research Conference - Brigham Young University – Provo, UT – March 1990
+• [“Fast Automated Object Detection Using Signature Parsing.”](https://www.spiedigitallibrary.org/conference-proceedings-of-spie/1192/1/Fast-Automated-Object-Detection-Using-Signature-Parsing/10.1117/12.969720.short) Tim Heaton; Shawn Becker; Kelley Anderson; William Barrett: Proceedings Volume 1192, Intelligent Robots &amp; Computer Vision VIII: Algorithms &amp; Techniques; (1990) https://doi.org/10.1117/12.969720
+• [“Probabilistic Segmentation of Myocardial Tissue by Deterministic Relaxation.”](https://scholarsarchive.byu.edu/cgi/viewcontent.cgi?article=1737&amp;context=facpub) Jerome A. Broekhuijsen, Shawn C. Becker, &amp; William A. Barrett: IEEE Proceedings of Computers in Cardiology, pp. 99-12, Jerusalem, September 1989.
+• [“Interactive Measurement of three-Dimensional Cardiac Morphology.”]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/BYU-MS-CS-Skull-Cross-Section-1.jpeg}(https://scholarsarchive.byu.edu/cgi/viewcontent.cgi?article=1736&amp;context=facpub) Shawn C Becker, William A Barrett, October 1989, DOI: 10.1109/CIC.1989.130586, Conference: Computers in Cardiology.</t>
+  </si>
+  <si>
+    <t>• Worked as a reservations agent for Dell Webb resorts and [houseboat rentals]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/Del-Webb-Reservations-150x115.png}(https://www.lake-powell-country.com/lake-powell-houseboat-history.html) at the various marinas url on [Lake Powell](https://www.lakepowell.com/) in Utah</t>
+  </si>
+  <si>
+    <t>• Seven-day paper delivery for the [Arizona Republic Newspaper]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/AZ-Republic-newspaper-150x150.jpg}.
+• Weekly collections
+• Used [purple Schwinn banana seat]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/AZ-Republic-paper-delivery-vehical-150x150.png}, [Schwinn 10 speed](url).</t>
+  </si>
+  <si>
+    <t>• As a consulting back-end software developer at [BigR.io]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/Bigr.io_-150x106.png} I used [AWS microservices] for custom voice-based [natural language processing] applications.
 • Used [Apache ActiveMQ](https://activemq.apache.org/), [Swagger](https://swagger.io/), [JSON], [Jackson](url), [AOP](https://www.baeldung.com/spring-aop), [Eclipse], [Maven], [Git], [Jira], and [Jenkins CI/CD].
 • [Java 8], [J2EE], [Servlets], [Spring], [SpringBoot], [JAX-RS], [JUnit], [JMeter], and [JProfile]</t>
   </si>
   <si>
-    <t>• As a consulting front-end software developer for [NuSkin](https://www.nuskin.com/us/en/, an international company known for its excellent  skin and beauty products I created new [Vue.js](https://vuejs.org/), [Nuxt](https://nuxt.com/), and [Vuetify](https://vuetifyjs.com/en/) components using [NodeJS] and [SCSS].  
-• Internationalized content using [Adobe Experience Cloud](https://business.adobe.com/).</t>
-  </si>
-  <si>
-    <t>• As a consulting data engineer in the data cyber security team of the [Cigna Group](https://www.thecignagroup.com/) created a [REST API](url) using [Postman](https://www.postman.com/) and [OpenAP](https://openapi-generator.tech/) for pulling credentials from the [CyberArk identity security platform](https://www.cyberark.com/) using [mutual TLS SSL authentication](https://docs.solace.com/Security/Two-Way-SSL-Authentication.htm) with [AWS API Gateway](https://docs.aws.amazon.com/apigateway/). 
-•  Migrated a suite of legacy data pipeline elements running on the [Unity IoC platform](http://unitycontainer.org/articles/introduction.html) to pull credentials from the CyberArk service at runtime rather than using [Fernet](https://cryptography.io/en/latest/fernet/) encrypted local files. 
-•  Upgraded GitHub apps to use [CloudBees/Jenkins](https://docs.aws.amazon.com/apigateway/) CI/CD pipeline for build, applying sofware and cyber-secutity code checks, and on-prem server installation.</t>
-  </si>
-  <si>
-    <t>• [Intrusic LLC](https://www.crunchbase.com/organization/intrusic) built real-time network monitoring systems that identified external and internal network intrusion attempts
-• As a Sierra Vista Group consulting architech, I helped design and develop an approach for buffering live streaming network traffic for asynchronous package processing. 
-• Used [Debian Linux](https://www.debian.org/), [C programming language](https://www.cprogramming.com/books/ritchie.html), and [Visio](https://www.microsoft.com/en-us/microsoft-365/visio/flowchart-software).</t>
-  </si>
-  <si>
-    <t>• As a consulting data engineer in the analytics team of [Warner Brothers Interactive Entertainment](https://warnerbrosgames.com/) Division, I implemented high-volume pipeline integrations shuffling game telemetry and [user PII data] between WB-distributed consumer games and [marketing service platforms] via [Segment customer data platform](https://segment.com/customer-data-platform/) using [Kafka](https://aws.amazon.com/msk/), [Redshift](https://aws.amazon.com/redshift/), and [Apache Airflow](https://airflow.apache.org). 
-• Employed [Python], [Amazon Glue](https://aws.amazon.com/glue/) and [Apache Airflow](https://airflow.apache.org/) for external [3rd-party integrations] and internal [dev-ops integrations] with [Jenkins], [DataDog](https://www.datadoghq.com/), and [ZenDesk](https://zendesk.com) 
-• Integrated with [Google BigQuery data warehouse](https://cloud.google.com/bigquery) and [AWS-managed services] [Apache Airflow](https://aws.amazon.com/managed-workflows-for-apache-airflow/), [S3], [AWS Glue](https://towardsdatascience.com/extract-transform-load-etl-aws-glue-edd383218cfd), and [AWS Redshift warehouse](https://aws.amazon.com/redshift/).</t>
-  </si>
-  <si>
-    <t>• As a consulting data engineer for [Angel Studios](https://www.angel.com/home], a streaming media service that offers family-friendly entertainment that amplifies light, with titles including The Chosen, Dry Bar Comedy, and Tuttle Twins.
-• Used Python, [Pandas], [Numpy], [Keras], and [Jupyter](https://jupyter.org/) to build and tune hyperparameters of a [convolutional neural network](https://towardsdatascience.com/a-comprehensive-guide-to-convolutional-neural-networks-the-eli5-way-3bd2b1164a53) with [supervised learning] on [AWS Sagemaker](https://aws.amazon.com/pm/sagemaker/) to classify movie frames from episodic programs stored in [Amazon S3](https://aws.amazon.com/s3/storage-classes). 
-• Built web client apps using [Python] with [Postman](https://www.postman.com/) that made [RESTful API] requests to pull monthly usage data from various web marketing partners like [FaceBook Marketing](https://www.quora.com/What-is-Facebook-Marketing-1), [Google Play](https://play.google/howplayworks/) , and [Vimeo](https://vimeo.com/). 
-• Worked with [Segment customer data platform](https://segment.com/customer-data-platform/), [Excel], and [Tableau] to create scheduled reports for the company's sales and finance teams.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• As a consulting data engineer for Greenseed Tech, an internet company that provides daily lead reports for independent real-estage agents world-wide, I  [containerized] legacy web applications using [Docker](https://www.docker.com/) and [AWS Secrets Manager](https://aws.amazon.com/secrets-manager/). 
-• Documented existing data architecture as [ERDs](https://www.lucidchart.com/pages/er-diagrams) using [DBeaver Enterprise](https://dbeaver.com/dbeaver-enterprise/). </t>
-  </si>
-  <si>
-    <t>• As a senior data engineer for SeniorLink a homeservices support platform, helped create [ETL](https://aws.amazon.com/what-is/etl/) processes using [AWS Kinesis](https://aws.amazon.com/pm/kinesis/), [Python], [PySpark](https://spark.apache.org/), and [AWS Data Pipeline](https://docs.aws.amazon.com/datapipeline/latest/DeveloperGuide/what-is-datapipeline.html) to load structured event data from [PostgreSQL] databases into a centralized [Redshift warehouse](https://aws.amazon.com/pm/redshift/). 
+    <t>• As a senior data engineer for SeniorLink's [Vela project]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/Vela-150x126.png} a homeservices support platform, helped create [ETL](https://aws.amazon.com/what-is/etl/) processes using [AWS Kinesis](https://aws.amazon.com/pm/kinesis/), [Python], [PySpark](https://spark.apache.org/), and [AWS Data Pipeline](https://docs.aws.amazon.com/datapipeline/latest/DeveloperGuide/what-is-datapipeline.html) to load structured event data from [PostgreSQL] databases into a centralized [Redshift warehouse](https://aws.amazon.com/pm/redshift/). 
 • Saved data as [self-describing data assets] in [S3] using [AWS Kinesis] and [AWS Lambda](https://docs.aws.amazon.com/lambda/) to aggregate event data into [schema-on-read] file formats, [Apache Avro](https://avro.apache.org/), and [Apache Parquet](https://parquet.apache.org/).
 • Steered efforts in creating a [Data Lake](https://aws.amazon.com/big-data/datalakes-and-analytics/datalakes/) using [PostgreSQL](url) and [FlyWay](https://flywaydb.org/) with [Python](url) and [PySpark](https://spark.apache.org/docs/latest/api/python/index.html) pre-processing on [EC2 instances](url) with [AWS EFS](https://zesty.co/blog/ebs-vs-efs-which-is-right), [EBS], and [S3] storage.
 • Used streaming event messages queued in [RabbitMQ](https://docs.aws.amazon.com/amazon-mq/latest/developer-guide/working-with-rabbitmq.html) and [AWS Kinesis] to build [type-2 slowly changing dimensions]](url) and accumulative facts tables. 
@@ -405,34 +422,17 @@
 • [Test-driven development](https://www.pluralsight.com/blog/software-development/tdd-vs-bdd) using [Python], [PyCharm], [PyTest], [Unit-test], [GitHub], [Jira], and [Jenkins CI/CD](https://www.jenkins.io/).</t>
   </si>
   <si>
-    <t>• Co-founded a finance and technology boutique called [Sierra Vista Group](https://6sense.com/company/sierra-vista-group-llc/5ba8a5247c8666394376fc4f) that delivered support in planning and proposing effective IT strategies for key clients in several industries. 
-• Performed various services, including system and architecture assessment and solutions design, to ensure the smooth running of technical projects.
-• Managed project schedules and technical specifications to match business requirements within contractual budget constraints. 
-• Identified opportunities for potential clients requiring expertise in product development, software engineering, and data modeling. Negotiated and communicated with c-level client management regarding project milestone agreements.
-• Increased ROI for each client’s project by hiring and managing contractors to deliver custom software solutions.
-• Delivered high-level leadership and guidance to a team of software engineering consultants for several projects to accelerate operational excellence.</t>
-  </si>
-  <si>
-    <t>• As co-founder and CTO, designed and led the development of a public website used by discerning home designers and builders called [HomePortfolio.com](https://homeportfolio.com/). 
-• Hired a staff of   10 software and databases developers. 
-• Worked with data acquisition team to scan and tag over 700,000 premium home design products from over 2,000 manufactures and vendors.
-• Designed datamodel and data entry tools for category-specific product attribution. 
-• Helped extended the business model to provide online product selection tools for participating vendors and manufacturers.
-• Instrumental in raising over $70M in venture capital. 
-• Used Oracle IIi, [ATG Dyanamo]( https://docs.oracle.com/cd/E24152_01/Platform.10-1/ATGPersBusinessGuide/html/s0102dynamoapplicationframework01.html), Java 8, [Akamai](https://www.akamai.com/), [WebTrends](https://www.webtrends.com/), [FileMakerPro], [ImageMagik](https://imagemagick.org/index.php), and [Omnigraffle](https://www.omnigroup.com/omnigraffle) for data modeling and workflow designs.</t>
-  </si>
-  <si>
-    <t>• Co-founded [ClipFile], a company that envisioned building a web destination where users could easily record and share their favorite pieces of content like facts, authored stories, quotes, articles, chapters, or personal thoughts, as a way of concretely defining their personal mindset.
+    <t>• Worked as an intern in the Pension Department at [Greyhound Corporate]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/Greyhound-Corporation-Phoenix-Downtown-circa-1970-150x150.png}.
+• Manully sorted thousands of pension checks and doing handwriting comparisons to find fraudulent cashing of checks for deceased pensioners.</t>
+  </si>
+  <si>
+    <t>• Co-founded [ClipFile]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/clipfile-infrastructure-150x150.png}, a company that envisioned building a web destination where users could easily record and share their favorite pieces of content like facts, authored stories, quotes, articles, chapters, or personal thoughts, as a way of concretely defining their personal [mindset]{https://sourcesofinsight.com/wp-content/uploads/2014/04/Mindset-768x505.jpg}(https://sourcesofinsight.com/what-is-mindset/).
 • Implemented [fuzzy matching](https://nanonets.com/blog/fuzzy-matching-fuzzy-logic/), [word clustering](https://www.ilc.cnr.it/EAGLES96/rep2/node37.html#:~:text=Word%20clustering%20is%20a%20technique,to%20information%20retrieval%20and%20filtering.), [semantic similarity scores](https://towardsdatascience.com/semantic-similarity-using-transformers-8f3cb5bf66d6), and [collaborative filtering](https://www.hindawi.com/journals/aai/2009/421425/) to help users find content that matched or differed from thieir own mindset.
 • Launched a novel [SaaS] using [Amazon Web Services] that let individuals and content creators search and share [mindsets].
 • Conceptualized patented technology by designing and implementing a fuil-stack consumer-facing content management system that supported tuned matching among selected attributes.
 • [Java 8], [JSP], [Servlets], [Spring], [AWS services], [JavaScript], [JQuery], [HTML5], [CSS], [JUnit], [JMeter], [JProfile].
 • Utilized [REST], [Swagger], [Apache Shiro](https://shiro.apache.org/), [Eclipse IDE](https://www.eclipse.org/home/whatis/), [Apache Maven](https://maven.apache.org/what-is-maven.html), [Apache Ant](https://ant.apache.org/), [Git], [Hibernate], [AWS SimpleDB](https://aws.amazon.com/simpledb/), [CentOS Linux](https://www.centos.org/), [Apache Tomcat](https://tomcat.apache.org/), [Jetty](https://projects.eclipse.org/projects/rt.jetty), and [Spring MVC](https://docs.spring.io/spring-framework/reference/web/webmvc.html).
 • Served as co-founder and co-authored [four patents](https://www.freepatentsonline.com/y2013/0325870.html).</t>
-  </si>
-  <si>
-    <t>• Front-end software developer of a reverse kinametics path planning system for multi-axis industrial robots.
-• Technologies used include [C programming language], [Borne shell](https://en.wikipedia.org/wiki/Bourne_shell), X11 Window System, [Xt toolkit intrinsics](https://en.wikipedia.org/wiki/X_Toolkit_Intrinsics), [Silicon Graphics Irix](https://en.wikipedia.org/wiki/Silicon_Graphics), and [HP-UX](https://en.wikipedia.org/wiki/HP-UX).</t>
   </si>
 </sst>
 </file>
@@ -985,8 +985,8 @@
   </sheetPr>
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I14" zoomScale="201" zoomScaleNormal="201" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="H9" zoomScale="201" zoomScaleNormal="201" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1044,7 +1044,7 @@
         <v>45047</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E2" s="8">
         <v>3</v>
@@ -1057,10 +1057,10 @@
       </c>
       <c r="H2" s="9"/>
       <c r="I2" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="192" x14ac:dyDescent="0.2">
@@ -1087,10 +1087,10 @@
       </c>
       <c r="H3" s="11"/>
       <c r="I3" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="176" x14ac:dyDescent="0.2">
@@ -1117,10 +1117,10 @@
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="80" x14ac:dyDescent="0.2">
@@ -1147,10 +1147,10 @@
       </c>
       <c r="H5" s="13"/>
       <c r="I5" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="64" x14ac:dyDescent="0.2">
@@ -1177,18 +1177,18 @@
       </c>
       <c r="H6" s="14"/>
       <c r="I6" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="320" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="335" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C7" s="7">
         <v>42795</v>
@@ -1207,13 +1207,13 @@
       </c>
       <c r="H7" s="15"/>
       <c r="I7" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>30</v>
       </c>
@@ -1237,13 +1237,13 @@
       </c>
       <c r="H8" s="16"/>
       <c r="I8" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="304" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="335" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>34</v>
       </c>
@@ -1267,10 +1267,10 @@
       </c>
       <c r="H9" s="17"/>
       <c r="I9" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="192" x14ac:dyDescent="0.2">
@@ -1297,13 +1297,13 @@
       </c>
       <c r="H10" s="18"/>
       <c r="I10" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="208" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="224" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>34</v>
       </c>
@@ -1327,10 +1327,10 @@
       </c>
       <c r="H11" s="19"/>
       <c r="I11" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="144" x14ac:dyDescent="0.2">
@@ -1357,13 +1357,13 @@
       </c>
       <c r="H12" s="9"/>
       <c r="I12" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="304" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="320" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>47</v>
       </c>
@@ -1387,13 +1387,13 @@
       </c>
       <c r="H13" s="11"/>
       <c r="I13" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="256" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="288" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>49</v>
       </c>
@@ -1417,13 +1417,13 @@
       </c>
       <c r="H14" s="12"/>
       <c r="I14" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>52</v>
       </c>
@@ -1447,10 +1447,10 @@
       </c>
       <c r="H15" s="13"/>
       <c r="I15" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="32" x14ac:dyDescent="0.2">
@@ -1477,13 +1477,13 @@
       </c>
       <c r="H16" s="14"/>
       <c r="I16" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J16" s="10" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>56</v>
       </c>
@@ -1507,10 +1507,10 @@
       </c>
       <c r="H17" s="15"/>
       <c r="I17" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="64" x14ac:dyDescent="0.2">
@@ -1537,10 +1537,10 @@
       </c>
       <c r="H18" s="16"/>
       <c r="I18" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -1567,13 +1567,13 @@
       </c>
       <c r="H19" s="17"/>
       <c r="I19" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J19" s="10" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>62</v>
       </c>
@@ -1597,18 +1597,18 @@
       </c>
       <c r="H20" s="18"/>
       <c r="I20" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J20" s="10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" ht="48" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
+      <c r="B21" s="6" t="s">
         <v>65</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>66</v>
       </c>
       <c r="C21" s="7">
         <v>28369</v>
@@ -1620,25 +1620,25 @@
         <v>1</v>
       </c>
       <c r="F21" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G21" s="6" t="s">
         <v>67</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>68</v>
       </c>
       <c r="H21" s="20"/>
       <c r="I21" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>69</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="112" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C22" s="7">
         <v>39417</v>
@@ -1650,25 +1650,25 @@
         <v>2</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H22" s="21"/>
       <c r="I22" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J22" s="22" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="128" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C23" s="7">
         <v>38749</v>
@@ -1680,25 +1680,25 @@
         <v>2</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H23" s="23"/>
       <c r="I23" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J23" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="112" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C24" s="7">
         <v>38384</v>
@@ -1710,25 +1710,25 @@
         <v>2</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H24" s="24"/>
       <c r="I24" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C25" s="7">
         <v>38018</v>
@@ -1740,25 +1740,25 @@
         <v>2</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H25" s="25"/>
       <c r="I25" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J25" s="10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="144" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C26" s="7">
         <v>37681</v>
@@ -1770,17 +1770,17 @@
         <v>2</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H26" s="26"/>
       <c r="I26" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed monocolor issues, renamed ICON_TYPES and icon filenames
</commit_message>
<xml_diff>
--- a/static_content/jobs/jobs.xlsx
+++ b/static_content/jobs/jobs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbecker11/workspace-parallax/flock-of-postcards/static_content/jobs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E28DE26-379E-C74E-AFFF-69A7D70D0007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E08119FD-2A06-034A-9003-435380700CFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23160" yWindow="500" windowWidth="28960" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="640" yWindow="2560" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="jobs" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="95">
   <si>
     <t>role</t>
   </si>
@@ -52,9 +52,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t xml:space="preserve">Consulting Data Engineer </t>
-  </si>
-  <si>
     <t>The Cigna Group</t>
   </si>
   <si>
@@ -91,9 +88,6 @@
     <t>#8a2be2</t>
   </si>
   <si>
-    <t xml:space="preserve">Consulting Full-Stack Developer </t>
-  </si>
-  <si>
     <t>NuSkin</t>
   </si>
   <si>
@@ -112,9 +106,6 @@
     <t>#800000</t>
   </si>
   <si>
-    <t xml:space="preserve">Consulting Back-End Engineer </t>
-  </si>
-  <si>
     <t>BigR.io</t>
   </si>
   <si>
@@ -124,9 +115,6 @@
     <t>#dc143c</t>
   </si>
   <si>
-    <t xml:space="preserve">Software Architect / Co-Founder </t>
-  </si>
-  <si>
     <t>ClipFile LLC</t>
   </si>
   <si>
@@ -178,55 +166,9 @@
     <t>#0000cd</t>
   </si>
   <si>
-    <t>Software Developer</t>
-  </si>
-  <si>
     <t>Cimmetrix LLC</t>
   </si>
   <si>
-    <t>BS Design Engineering Technology</t>
-  </si>
-  <si>
-    <t>• Completed bachelor degree in Design Engineering Technologies
-• Drafting, CAD/CAM, machine design, fluid dynamics, ferrous metallurgy, static load bearing mathematics.</t>
-  </si>
-  <si>
-    <t>Call Center Reservationist</t>
-  </si>
-  <si>
-    <t>Dell Webb Properties</t>
-  </si>
-  <si>
-    <t>Missonary</t>
-  </si>
-  <si>
-    <t>Taiwan Taibei Mission</t>
-  </si>
-  <si>
-    <t>BS GED</t>
-  </si>
-  <si>
-    <t>• Majored in mathematics, took general education required classes as well as design and oil painting.</t>
-  </si>
-  <si>
-    <t>Data Processing</t>
-  </si>
-  <si>
-    <t>Greyhound Corp</t>
-  </si>
-  <si>
-    <t>Newspaper Delivery</t>
-  </si>
-  <si>
-    <t>Arizona Republic</t>
-  </si>
-  <si>
-    <t>gold</t>
-  </si>
-  <si>
-    <t>#ffd700</t>
-  </si>
-  <si>
     <t xml:space="preserve">Project Manager / Technical Lead </t>
   </si>
   <si>
@@ -239,9 +181,6 @@
     <t>#ffff00</t>
   </si>
   <si>
-    <t xml:space="preserve">Consulting Architect </t>
-  </si>
-  <si>
     <t>Eleven LLC</t>
   </si>
   <si>
@@ -251,9 +190,6 @@
     <t>#00ff00</t>
   </si>
   <si>
-    <t>Consulting Architect</t>
-  </si>
-  <si>
     <t>Intrusic LLC</t>
   </si>
   <si>
@@ -261,9 +197,6 @@
   </si>
   <si>
     <t>#32cd32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Consulting Architect / Technical Lead </t>
   </si>
   <si>
     <t xml:space="preserve">AMI Entertainment </t>
@@ -304,15 +237,6 @@
 • Used the MS Office suite of business apps a well as MS Visio. </t>
   </si>
   <si>
-    <t>• Served as a missionary for the Church of Jesus Christ of Latter-day Saints in the [Taiwan Taibei mission](https://www.mymission.com/lds-missions/taiwan-taipei-mission).
-• Served as branch president in the town [Yuli](https://en.wikivoyage.org/wiki/Yuli) in the Hualien County on the east coast of Taiwan.</t>
-  </si>
-  <si>
-    <t>• [Intrusic LLC](https://www.crunchbase.com/organization/intrusic) built real-time network monitoring systems that identified external and internal network intrusion attempts
-• As a Sierra Vista Group consulting architech, I helped design and develop an approach for buffering live streaming network traffic for asynchronous package processing. 
-• Used [Debian Linux](https://www.debian.org/), [C programming language](https://www.cprogramming.com/books/ritchie.html), and [Visio](https://www.microsoft.com/en-us/microsoft-365/visio/flowchart-software).</t>
-  </si>
-  <si>
     <t>• Co-founded a finance and technology boutique called [Sierra Vista Group](https://6sense.com/company/sierra-vista-group-llc/5ba8a5247c8666394376fc4f) that delivered support in planning and proposing effective IT strategies for key clients in several industries. 
 • Performed various services, including system and architecture assessment and solutions design, to ensure the smooth running of technical projects.
 • Managed project schedules and technical specifications to match business requirements within contractual budget constraints. 
@@ -321,89 +245,30 @@
 • Delivered high-level leadership and guidance to a team of software engineering consultants for several projects to accelerate operational excellence.</t>
   </si>
   <si>
-    <t>• Worked as a reservations agent for Dell Webb resorts and [houseboat rentals]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/Del-Webb-Reservations-150x115.png}(https://www.lake-powell-country.com/lake-powell-houseboat-history.html) at the various marinas url on [Lake Powell](https://www.lakepowell.com/) in Utah</t>
-  </si>
-  <si>
-    <t>• Seven-day paper delivery for the [Arizona Republic Newspaper]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/AZ-Republic-newspaper-150x150.jpg}.
-• Weekly collections
-• Used [purple Schwinn banana seat]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/AZ-Republic-paper-delivery-vehical-150x150.png}, [Schwinn 10 speed](url).</t>
-  </si>
-  <si>
-    <t>• Worked as an intern in the Pension Department at [Greyhound Corporate]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/Greyhound-Corporation-Phoenix-Downtown-circa-1970-150x150.png}.
-• Manully sorted thousands of pension checks and doing handwriting comparisons to find fraudulent cashing of checks for deceased pensioners.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• As a consulting data engineer for Greenseed Tech, an internet company that provides daily lead reports for independent real-estage agents world-wide, I  [containerized] legacy web applications using [Linux], [Docker](https://www.docker.com/) and [AWS Secrets Manager](https://aws.amazon.com/secrets-manager/). 
-• Documented existing data architecture as [ERDs](https://www.lucidchart.com/pages/er-diagrams) using [DBeaver Enterprise](https://dbeaver.com/dbeaver-enterprise/). </t>
-  </si>
-  <si>
-    <t>• As a consulting data engineer for [Angel Studios](https://www.angel.com/home], a streaming media service that offers family-friendly entertainment that amplifies light, with titles including The Chosen, Dry Bar Comedy, and Tuttle Twins.
-• Used [Python], [Pandas], [Numpy], [Keras], [Linux], and [Jupyter](https://jupyter.org/) to build and tune hyperparameters of a [convolutional neural network](https://towardsdatascience.com/a-comprehensive-guide-to-convolutional-neural-networks-the-eli5-way-3bd2b1164a53) with [supervised learning] on [AWS Sagemaker](https://aws.amazon.com/pm/sagemaker/) to classify movie frames from episodic programs stored in [Amazon S3](https://aws.amazon.com/s3/storage-classes). 
-• Built web client apps using [Python] with [Postman](https://www.postman.com/) that made [RESTful API] requests to pull monthly usage data from various web marketing partners like [FaceBook Marketing](https://www.quora.com/What-is-Facebook-Marketing-1), [Google Play](https://play.google/howplayworks/) , and [Vimeo](https://vimeo.com/). 
-• Worked with [Segment customer data platform](https://segment.com/customer-data-platform/), [Excel], and [Tableau] to create scheduled reports for the company's sales and finance teams.</t>
-  </si>
-  <si>
-    <t>• As a consulting data engineer in the analytics team of [Warner Brothers Interactive Entertainment](https://warnerbrosgames.com/) Division, I implemented high-volume pipeline integrations shuffling game telemetry and [user PII data] between WB-distributed consumer games and [marketing service platforms] via [Segment customer data platform](https://segment.com/customer-data-platform/) using [Kafka](https://aws.amazon.com/msk/), [Redshift](https://aws.amazon.com/redshift/), and [Apache Airflow](https://airflow.apache.org). 
-• Employed [Python], [Linux], [Amazon Glue](https://aws.amazon.com/glue/) and [Apache Airflow](https://airflow.apache.org/) for external [3rd-party integrations] and internal [dev-ops integrations] with [Jenkins], [DataDog](https://www.datadoghq.com/), and [ZenDesk](https://zendesk.com) 
-• Integrated with [Google BigQuery data warehouse](https://cloud.google.com/bigquery) and [AWS-managed services] [Apache Airflow](https://aws.amazon.com/managed-workflows-for-apache-airflow/), [S3], [AWS Glue](https://towardsdatascience.com/extract-transform-load-etl-aws-glue-edd383218cfd), and [AWS Redshift warehouse](https://aws.amazon.com/redshift/).</t>
-  </si>
-  <si>
-    <t>• As a consulting data engineer in the data cyber security team of the [Cigna Group](https://www.thecignagroup.com/) created a [REST API](url) using [Postman](https://www.postman.com/), [Linux], and [OpenAPI](https://openapi-generator.tech/) for pulling credentials from the [CyberArk identity security platform](https://www.cyberark.com/) using [mutual TLS SSL authentication](https://docs.solace.com/Security/Two-Way-SSL-Authentication.htm) with [AWS API Gateway](https://docs.aws.amazon.com/apigateway/). 
-•  Migrated a suite of legacy data pipeline [Python] elements running on the [Unity IoC platform](http://unitycontainer.org/articles/introduction.html) to pull credentials from the CyberArk service at runtime rather than using [Fernet](https://cryptography.io/en/latest/fernet/) encrypted local files. 
-•  Upgraded [GitHub] apps to use [CloudBees/Jenkins](https://docs.aws.amazon.com/apigateway/) CI/CD pipeline for build, applying sofware and cyber-secutity code checks, and on-prem server installation.</t>
-  </si>
-  <si>
-    <t>• As a consulting front-end software developer for [NuSkin](https://www.nuskin.com/us/en/, an international company known for its excellent  skin and beauty products I created new [Vue.js](https://vuejs.org/), [Nuxt](https://nuxt.com/), and [Vuetify](https://vuetifyjs.com/en/) components using [Linux], [NodeJS] and [SCSS].  
-• Internationalized content using [Adobe Experience Cloud](https://business.adobe.com/).</t>
-  </si>
-  <si>
-    <t>• As a senior data engineer for SeniorLink's [Vela project]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/Vela-150x126.png} a homeservices support platform, helped create [ETL](https://aws.amazon.com/what-is/etl/) processes using [AWS Kinesis](https://aws.amazon.com/pm/kinesis/), [Python], [PySpark](https://spark.apache.org/), and [AWS Data Pipeline](https://docs.aws.amazon.com/datapipeline/latest/DeveloperGuide/what-is-datapipeline.html) to load structured event data from [PostgreSQL] databases into a centralized [Redshift warehouse](https://aws.amazon.com/pm/redshift/). 
-• Saved data as [self-describing data assets] in [S3] using [AWS Kinesis] and [AWS Lambda](https://docs.aws.amazon.com/lambda/) to aggregate event data into [schema-on-read] file formats, [Apache Avro](https://avro.apache.org/), and [Apache Parquet](https://parquet.apache.org/).
-• Steered efforts in creating a [Data Lake](https://aws.amazon.com/big-data/datalakes-and-analytics/datalakes/) using [PostgreSQL](url) and [FlyWay](https://flywaydb.org/) with [Python](url) and [PySpark](https://spark.apache.org/docs/latest/api/python/index.html) pre-processing on [EC2 instances](url) with [AWS EFS](https://zesty.co/blog/ebs-vs-efs-which-is-right), [EBS], and [S3] storage.
-• Used streaming event messages queued in [RabbitMQ](https://docs.aws.amazon.com/amazon-mq/latest/developer-guide/working-with-rabbitmq.html) and [AWS Kinesis] to build [type-2 slowly changing dimensions]](url) and accumulative facts tables. 
-• Designed and implemented a custom [star-schema warehouse](https://www.databricks.com/glossary/star-schema) and [ETL] processes to [de-normalize](https://en.wikipedia.org/wiki/Denormalization) and load data into an [AWS Redshift](https://aws.amazon.com/redshift/) data warehouse for BI reporting using [Tableau](https://www.tableau.com/).
-• [Test-driven development](https://www.pluralsight.com/blog/software-development/tdd-vs-bdd) using [Linux], [Python], [PyCharm], [PyTest], [Unit-test], [GitHub], [Jira], and [Jenkins CI/CD](https://www.jenkins.io/).</t>
-  </si>
-  <si>
-    <t>•  AMI (https://amientertainment.com/) was the internet-music distribution incarnation of Rowe International.  
-•  As a Sierra Vista Group consulting architect and technical lead, I helped design and implement their system for making monthly ACH royalty payments to music copyright owners for mechanical and performance licensing rights.
-•  Used [FileMaker Pro](https://www.claris.com/filemaker/), [Linux], [Java5], and [Visio](https://www.microsoft.com/en-us/microsoft-365/visio/flowchart-software).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">•  [Rowe International](https://pitchbook.com/profiles/company/13178-08) was the leading manufacturer of music jukeboxes. 
-•  Sierra Vista Group was consulted to assess their available technologies and create a plan to build their back-end systems to let them become a leading provider of internet-based music.
-•  As consulting architect and technical lead created the project plan and led the development of a full-stack web application used by  jukebox owners and Rowe sales and marketing.
-•  Used [Java], [Linux], [ObjectDesign](https://object.design/), JavaScript , [MySQL](https://www.mysql.com/), and [Adobe Photoshop](https://www.adobe.com/products/photoshop.html). 
-</t>
-  </si>
-  <si>
-    <t>• As lead software developer, built a CD-ROM-based home design application for selecting premium home design products for previewing in the context of images of any household rooms. 
-• Built the prototype using Adobe Photoshop and [Macromedia Director](https://macromedia.fandom.com/wiki/Macromedia_Director).
-• Built the actual application using using [Linux], [Java] and [Marimba Bongo](https://www.thriftbooks.com/w/official-marimba-guide-to-bongo_danny-goodman/2574616/#edition=58026223&amp;idiq=42367912) widget layout tool.
-• Updates for the self-updating application were delivered over the internet using [Mariba Castanet](https://www.infoworld.com/article/2076707/marimba-launches-new-castanet-with-a-less-java-centric-focus.html) push-technology.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• [Eleven LLC](https://www.eleven.net/) built mobile apps used by beverage industry distributors to help manage placement  of their products in the shelves and coolers in retail locations. The work done by the Sierra Vista Group was instrumental in their company being acquired by [Trimble Mobile Solutions](https://help.trimblegeospatial.com/TMM/Home.htm). 
-• As the consulting architect and team lead, we used [Java], [Linix], and  [JBoss](https://developers.redhat.com/products/eap/overview) message-oriented middleware platform, [Sybase Anywhere](https://texas.gs.shi.com/Product/30451452/Sybase-SQL-Anywhere-Advanced-Edition) for the client/server based database, and [Windows Mobile 5](https://en.wikipedia.org/wiki/Windows_Mobile_5.0) running on ruggedized mobile devices. </t>
-  </si>
-  <si>
-    <t>• As a consulting back-end software developer at [BigR.io]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/Bigr.io_-150x106.png} I used [AWS microservices] for custom voice-based [natural language processing] applications.
-• Used [Apache ActiveMQ](https://activemq.apache.org/), [Swagger](https://swagger.io/), [JSON], [Jackson](url), [AOP](https://www.baeldung.com/spring-aop), [Eclipse], [Maven], [Git], [Jira], and [Jenkins CI/CD].
-• [Java], [J2EE], [Servlets], [Spring], [SpringBoot], [JAX-RS], [Linux], [JUnit], [JMeter], and [JProfile]</t>
-  </si>
-  <si>
-    <t>• Front-end software developer of a reverse kinametics path planning system for multi-axis industrial robots for [Cimmetrix]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/Cimetrix-PDF-combined-logo-150x100.png}.
-• Technologies used include [Linux], [C programming language], [Borne shell](https://en.wikipedia.org/wiki/Bourne_shell), [X11] , [Xt toolkit intrinsics](https://en.wikipedia.org/wiki/X_Toolkit_Intrinsics), [Silicon Graphics Irix](https://en.wikipedia.org/wiki/Silicon_Graphics), and [HP-UX](https://en.wikipedia.org/wiki/HP-UX).</t>
-  </si>
-  <si>
-    <t>• Masters of Science degree, [Brigham Young University]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/BYU-entrance-150x150.jpg}, Provo, Utah
-Took all courses required for both bachelors and masters degrees in Computer Science
-• Thesis project [“Interactive Measurement of Three-Dimensional Objects Using a Depth Buffer &amp; Linear Probe.”](https://dl.acm.org/doi/pdf/10.1145/108360.108446) CS MS Thesis, Shawn Becker, William A. Barrett &amp; Dan R. Olsen, ACM Transactions on Graphics, Vol. 10, No. 2, April 1991
-• Top Research Presentation – New Tech Research Conference - Brigham Young University – Provo, UT – March 1990
-• [“Fast Automated Object Detection Using Signature Parsing.”](https://www.spiedigitallibrary.org/conference-proceedings-of-spie/1192/1/Fast-Automated-Object-Detection-Using-Signature-Parsing/10.1117/12.969720.short) Tim Heaton; Shawn Becker; Kelley Anderson; William Barrett: Proceedings Volume 1192, Intelligent Robots &amp; Computer Vision VIII: Algorithms &amp; Techniques; (1990) https://doi.org/10.1117/12.969720
-• [“Probabilistic Segmentation of Myocardial Tissue by Deterministic Relaxation.”](https://scholarsarchive.byu.edu/cgi/viewcontent.cgi?article=1737&amp;context=facpub) Jerome A. Broekhuijsen, Shawn C. Becker, &amp; William A. Barrett: IEEE Proceedings of Computers in Cardiology, pp. 99-12, Jerusalem, September 1989.
-• [“Interactive Measurement of three-Dimensional Cardiac Morphology.”]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/BYU-MS-CS-Skull-Cross-Section-1.jpeg}(https://scholarsarchive.byu.edu/cgi/viewcontent.cgi?article=1736&amp;context=facpub) Shawn C Becker, William A Barrett, October 1989, DOI: 10.1109/CIC.1989.130586, Conference: Computers in Cardiology.
-• [C programming language], [Linux], [XMotif], and [X11].</t>
+    <t xml:space="preserve">Senior Full-Stack Developer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Senior Back-End Engineer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Senior Architect </t>
+  </si>
+  <si>
+    <t>Senior Architect</t>
+  </si>
+  <si>
+    <t>Full Stack Developer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Technical Lead / Co-Founder </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lead Solutions Architect / Co-Founder </t>
+  </si>
+  <si>
+    <t>• [Intrusic LLC](https://www.crunchbase.com/organization/intrusic) built real-time network monitoring systems that identified external and internal network intrusion attempts
+• As a Sierra Vista Group architech, I helped design and develop an approach for buffering live streaming network traffic for asynchronous package processing. 
+• Used [Debian Linux](https://www.debian.org/), [C programming language](https://www.cprogramming.com/books/ritchie.html), and [Visio](https://www.microsoft.com/en-us/microsoft-365/visio/flowchart-software).</t>
   </si>
   <si>
     <t>•	Doctor of Philosopy degree, [Massachusetts Institute of Technology]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/MIT-logo.png}, Cambridge, Massachusettes
@@ -416,7 +281,11 @@
 •	“Semiautomatic Camera Lens Calibration from Partially Known Structure”, Shawn Becker, MIT Media Lab Reports, 1994
 •	[“Formulating a scene probability equation to differentiate the effects of shape &amp; albedo on image brightness.”](https://www.researchgate.net/publication/2668457_Formulating_a_Scene_Probability_Equation_to_Differentiate_the_Effects_of_Shape_and_Albedo_on_Image_Brightness) Shawn Becker, MIT Media Lab Reports, 1994
 •	“Computation of some projective-chirplet-transform &amp; metaplectic-chirplet-transform subspaces, with applications in image processing.” Steve Mann &amp; Shawn Becker, DSP World Symposium, Boston, Massachusetts, November 1992.
-• [C programming language], [TclTk], [X11], [XMotif], [Linux]</t>
+• [C programming language], [TclTk], [X11], [HTML], [JavaScript],[CSS],[XMotif], [bash], [Linux]</t>
+  </si>
+  <si>
+    <t>• As a senior full stack developer for [NuSkin](https://www.nuskin.com/us/en/, an international company known for its excellent  skin and beauty products I created new [Vue.js](https://vuejs.org/), [Nuxt](https://nuxt.com/), and [Vuetify](https://vuetifyjs.com/en/) components using [bash], [Linux], [GitHub], [NodeJS], [HTML] and [CSS].  
+• Internationalized content using [Adobe Experience Cloud](https://business.adobe.com/).</t>
   </si>
   <si>
     <t>• As co-founder and CTO, designed and led the development of a public website used by discerning home designers and builders called [HomePortfolio.com](https://homeportfolio.com/). 
@@ -425,16 +294,86 @@
 • Designed datamodel and data entry tools for category-specific product attribution. 
 • Helped extended the business model to provide online product selection tools for participating vendors and manufacturers.
 • Instrumental in raising over $70M in venture capital. 
-• Used [Oracle], [ATG Dyanamo]( https://docs.oracle.com/cd/E24152_01/Platform.10-1/ATGPersBusinessGuide/html/s0102dynamoapplicationframework01.html), [Java], [Akamai]{https://www.hiclipart.com/free-transparent-background-png-clipart-zkmsn}(https://www.akamai.com/), [WebTrends](https://www.webtrends.com/), [FileMakerPro], [ImageMagik](https://imagemagick.org/index.php), [Linux], and [Omnigraffle](https://www.omnigroup.com/omnigraffle) for data modeling and workflow designs.</t>
+• Used [Oracle], [ATG Dyanamo]( https://docs.oracle.com/cd/E24152_01/Platform.10-1/ATGPersBusinessGuide/html/s0102dynamoapplicationframework01.html), [Java], [Akamai]{https://www.hiclipart.com/free-transparent-background-png-clipart-zkmsn}(https://www.akamai.com/), [WebTrends](https://www.webtrends.com/), [FileMakerPro], [ImageMagik](https://imagemagick.org/index.php), [bash], [Linux], [HTML], [JavaScript], [CSS], and [Omnigraffle](https://www.omnigroup.com/omnigraffle) for data modeling and workflow designs.</t>
+  </si>
+  <si>
+    <t>• As lead software developer, built a CD-ROM-based home design application for selecting premium home design products for previewing in the context of images of any household rooms. 
+• Built the prototype using Adobe Photoshop and [Macromedia Director](https://macromedia.fandom.com/wiki/Macromedia_Director).
+• Built the actual application using using [bash], [Linux], [Java] and [Marimba Bongo](https://www.thriftbooks.com/w/official-marimba-guide-to-bongo_danny-goodman/2574616/#edition=58026223&amp;idiq=42367912) widget layout tool.
+• Updates for the self-updating application were delivered over the internet using [Marimba Castanet](https://www.infoworld.com/article/2076707/marimba-launches-new-castanet-with-a-less-java-centric-focus.html) push-technology.</t>
+  </si>
+  <si>
+    <t>• Masters of Science degree, [Brigham Young University]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/BYU-entrance-150x150.jpg}, Provo, Utah
+Took all courses required for both bachelors and masters degrees in Computer Science
+• Thesis project [“Interactive Measurement of Three-Dimensional Objects Using a Depth Buffer &amp; Linear Probe.”](https://dl.acm.org/doi/pdf/10.1145/108360.108446) CS MS Thesis, Shawn Becker, William A. Barrett &amp; Dan R. Olsen, ACM Transactions on Graphics, Vol. 10, No. 2, April 1991
+• Top Research Presentation – New Tech Research Conference - Brigham Young University – Provo, UT – March 1990
+• [“Fast Automated Object Detection Using Signature Parsing.”](https://www.spiedigitallibrary.org/conference-proceedings-of-spie/1192/1/Fast-Automated-Object-Detection-Using-Signature-Parsing/10.1117/12.969720.short) Tim Heaton; Shawn Becker; Kelley Anderson; William Barrett: Proceedings Volume 1192, Intelligent Robots &amp; Computer Vision VIII: Algorithms &amp; Techniques; (1990) https://doi.org/10.1117/12.969720
+• [“Probabilistic Segmentation of Myocardial Tissue by Deterministic Relaxation.”](https://scholarsarchive.byu.edu/cgi/viewcontent.cgi?article=1737&amp;context=facpub) Jerome A. Broekhuijsen, Shawn C. Becker, &amp; William A. Barrett: IEEE Proceedings of Computers in Cardiology, pp. 99-12, Jerusalem, September 1989.
+• [“Interactive Measurement of three-Dimensional Cardiac Morphology.”]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/BYU-MS-CS-Skull-Cross-Section-1.jpeg}(https://scholarsarchive.byu.edu/cgi/viewcontent.cgi?article=1736&amp;context=facpub) Shawn C Becker, William A Barrett, October 1989, DOI: 10.1109/CIC.1989.130586, Conference: Computers in Cardiology.
+• [C programming language], [bash], [Linux], [XMotif], and [X11].</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• [Eleven LLC](https://www.eleven.net/) built mobile apps used by beverage industry distributors to help manage placement  of their products in the shelves and coolers in retail locations. The work done by the Sierra Vista Group was instrumental in their company being acquired by [Trimble Mobile Solutions](https://help.trimblegeospatial.com/TMM/Home.htm). 
+• As the architect and team lead, we used [Java], [bash], [GitHub], [Linix], and  [JBoss](https://developers.redhat.com/products/eap/overview) message-oriented middleware platform, [Sybase Anywhere](https://texas.gs.shi.com/Product/30451452/Sybase-SQL-Anywhere-Advanced-Edition) for the client/server based database, and [Windows Mobile](https://en.wikipedia.org/wiki/Windows_Mobile_5.0) running on ruggedized mobile devices. </t>
+  </si>
+  <si>
+    <t>•  AMI (https://amientertainment.com/) was the internet-music distribution incarnation of Rowe International.  
+•  As a Sierra Vista Group project manager and technical lead, I helped design and implement their system for making monthly ACH royalty payments to music copyright owners for mechanical and performance licensing rights.
+•  Used [FileMaker Pro](https://www.claris.com/filemaker/), [bash], [Linux], [HTML], [CSS], [JavaScript], [Java], and [Visio](https://www.microsoft.com/en-us/microsoft-365/visio/flowchart-software).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">•  [Rowe International](https://pitchbook.com/profiles/company/13178-08) was the leading manufacturer of music jukeboxes. 
+•  Sierra Vista Group was consulted to assess their available technologies and create a plan to build their back-end systems to let them become a leading provider of internet-based music.
+•  As project manager and technical lead created the project plan and led the development of a full-stack web application used by  jukebox owners and Rowe sales and marketing.
+•  Used [Java], [bash], [Linux], [HTML], [CSS], [JavaScript], [ObjectDesign](https://object.design/), [MySQL](https://www.mysql.com/), and [Adobe Photoshop](https://www.adobe.com/products/photoshop.html). 
+</t>
+  </si>
+  <si>
+    <t>• As a senior software engineer at [BigR.io]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/Bigr.io_-150x106.png} I used [Amazon microservices] for custom voice-based [natural language processing] applications.
+• Used [Apache ActiveMQ](https://activemq.apache.org/), [Swagger](https://swagger.io/), [JSON], [Jackson](url), [AOP](https://www.baeldung.com/spring-aop), [Eclipse], [Maven], [GitHub], [Jira], and [Jenkins].
+• [Java], [J2EE], [Servlets], [Spring], [SpringBoot], [JAX-RS], [bash], [Linux], [JUnit], [JMeter], and [JProfile]</t>
+  </si>
+  <si>
+    <t>• As a senior data engineer in the data cyber security team of the [Cigna Group](https://www.thecignagroup.com/) created a [REST API](url) using [Postman](https://www.postman.com/), [bash], [Linux], and [OpenAPI](https://openapi-generator.tech/) for pulling credentials from the [CyberArk identity security platform](https://www.cyberark.com/) using [mutual TLS SSL authentication](https://docs.solace.com/Security/Two-Way-SSL-Authentication.htm) with [Amazon API Gateway](https://docs.aws.amazon.com/apigateway/). 
+•  Migrated a suite of legacy data pipeline [Python] elements running on the [Unity IoC platform](http://unitycontainer.org/articles/introduction.html) to pull credentials from the CyberArk service at runtime rather than using [Fernet](https://cryptography.io/en/latest/fernet/) encrypted local files. 
+•  Upgraded [GitHub] apps to use [Jenkins](https://docs.aws.amazon.com/apigateway/) CI/CD pipeline for build, applying sofware and cyber-secutity code checks, and on-prem server installation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• As a senior software engineer for Greenseed Tech, an internet company that provides daily lead reports for independent real-estage agents world-wide, I  [containerized] legacy web applications using [bash], [Linux], [GitHub], [Docker](https://www.docker.com/) and [Amazon Secrets Manager](https://aws.amazon.com/secrets-manager/). 
+• Updated legacy web apps using [bash], [Linux], [HTML], [CSS], [JavaScript], [NGINX], and [OpenSSL].
+• Documented existing data architecture as [ERDs](https://www.lucidchart.com/pages/er-diagrams) using [DBeaver Enterprise](https://dbeaver.com/dbeaver-enterprise/). </t>
   </si>
   <si>
     <t>• Co-founded [ClipFile]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/clipfile-infrastructure-150x150.png}, a company that envisioned building a web destination where users could easily record and share their favorite pieces of content like facts, authored stories, quotes, articles, chapters, or personal thoughts, as a way of concretely defining their personal [mindset]{https://sourcesofinsight.com/wp-content/uploads/2014/04/Mindset-768x505.jpg}(https://sourcesofinsight.com/what-is-mindset/).
 • Implemented [fuzzy matching](https://nanonets.com/blog/fuzzy-matching-fuzzy-logic/), [word clustering](https://www.ilc.cnr.it/EAGLES96/rep2/node37.html#:~:text=Word%20clustering%20is%20a%20technique,to%20information%20retrieval%20and%20filtering.), [semantic similarity scores](https://towardsdatascience.com/semantic-similarity-using-transformers-8f3cb5bf66d6), and [collaborative filtering](https://www.hindawi.com/journals/aai/2009/421425/) to help users find content that matched or differed from thieir own mindset.
-• Launched a novel [SaaS] using [Amazon Web Services] that let individuals and content creators search and share [mindsets].
+• Launched a novel [SaaS] using [Amazon Web Services] that let individuals and content creators search and share mindsets.
 • Conceptualized patented technology by designing and implementing a fuil-stack consumer-facing content management system that supported tuned matching among selected attributes.
-• [Java], [J2EE], [JSP], [Servlets], [Spring], [AWS services], [JavaScript], [JQuery], [HTML5], [CSS], [JUnit], [JMeter], [JProfile].
-• Utilized [REST], [Swagger], [Apache Shiro](https://shiro.apache.org/), [Eclipse IDE](https://www.eclipse.org/home/whatis/), [Apache Maven](https://maven.apache.org/what-is-maven.html), [Apache Ant](https://ant.apache.org/), [Git], [Hibernate], [AWS SimpleDB](https://aws.amazon.com/simpledb/), [CentOS Linux](https://www.centos.org/), [Apache Tomcat](https://tomcat.apache.org/), [Linux], [Jetty](https://projects.eclipse.org/projects/rt.jetty), and [Spring MVC](https://docs.spring.io/spring-framework/reference/web/webmvc.html).
+• [Java], [J2EE], [JSP], [Servlets], [Spring], [Amazon services], [JavaScript], [JQuery], [HTML], [CSS], [JUnit], [JMeter], [JProfile].
+• Utilized [REST API], [Swagger], [Apache Shiro](https://shiro.apache.org/), [Eclipse IDE](https://www.eclipse.org/home/whatis/), [Apache Maven](https://maven.apache.org/what-is-maven.html), [Apache Ant](https://ant.apache.org/), [GitHub], [Hibernate], [Amazon SimpleDB](https://aws.amazon.com/simpledb/), [CentOS Linux](https://www.centos.org/), [Apache Tomcat](https://tomcat.apache.org/), [bash], [Linux], [Jetty](https://projects.eclipse.org/projects/rt.jetty), and [Spring MVC](https://docs.spring.io/spring-framework/reference/web/webmvc.html).
 • Served as co-founder and co-authored [four patents](https://www.freepatentsonline.com/y2013/0325870.html).</t>
+  </si>
+  <si>
+    <t>• As a senior data engineer in the analytics team of [Warner Brothers Interactive Entertainment](https://warnerbrosgames.com/) Division, I implemented high-volume pipeline integrations shuffling game telemetry and [user PII data] between WB-distributed consumer games and [marketing service platforms] via [Segment customer data platform](https://segment.com/customer-data-platform/) using [Kafka](https://aws.amazon.com/msk/), [Amazon Redshift](https://aws.amazon.com/redshift/), and [Apache Airflow](https://airflow.apache.org). 
+• Employed [Python], [GitHub], [bash], [Linux], [Amazon Glue](https://aws.amazon.com/glue/) and [Apache Airflow](https://airflow.apache.org/) for external 3rd-party integrations and internal dev-ops integrations with [Jenkins], [DataDog](https://www.datadoghq.com/), and [ZenDesk](https://zendesk.com) 
+• Integrated with [Google BigQuery data warehouse](https://cloud.google.com/bigquery using  [Apache Airflow](https://aws.amazon.com/managed-workflows-for-apache-airflow/), [Amazon S3], and [Amazon Redshift](https://aws.amazon.com/redshift/).</t>
+  </si>
+  <si>
+    <t>• Front-end software developer of a reverse kinametics path planning system for multi-axis industrial robots for [Cimmetrix]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/Cimetrix-PDF-combined-logo-150x100.png}.
+• Technologies used include [bash], [Linux], [C programming language], [bash](https://en.wikipedia.org/wiki/Bourne_shell), [X11] , [Xt toolkit intrinsics](https://en.wikipedia.org/wiki/X_Toolkit_Intrinsics), [Silicon Graphics Irix](https://en.wikipedia.org/wiki/Silicon_Graphics), and [HP-UX](https://en.wikipedia.org/wiki/HP-UX).</t>
+  </si>
+  <si>
+    <t>• As a senior data engineer for [Angel Studios](https://www.angel.com/home), a streaming media service that offers family-friendly entertainment that amplifies light, with titles including The Chosen, Dry Bar Comedy, and Tuttle Twins.
+• Used [Python], [GitHub], [Pandas], [Numpy], [Keras], [bash], [Linux], and [Jupyter](https://jupyter.org/) to build and tune hyperparameters of a [convolutional neural network](https://towardsdatascience.com/a-comprehensive-guide-to-convolutional-neural-networks-the-eli5-way-3bd2b1164a53) with [supervised learning] on [Amazon Sagemaker](https://aws.amazon.com/pm/sagemaker/) to classify movie frames from episodic programs stored in [Amazon S3](https://aws.amazon.com/s3/storage-classes). 
+• Built web client apps using [Python] with [Postman](https://www.postman.com/) that made [REST API] requests to pull monthly usage data from various web marketing partners like [FaceBook Marketing](https://www.quora.com/What-is-Facebook-Marketing-1), [Google Play](https://play.google/howplayworks/) , and [Vimeo](https://vimeo.com/). 
+• Worked with [Segment customer data platform](https://segment.com/customer-data-platform/), [Excel], and [Tableau] to create scheduled reports for the company's sales and finance teams.</t>
+  </si>
+  <si>
+    <t>• As a senior data engineer for SeniorLink's [Vela project]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/Vela-150x126.png} a homeservices support platform, helped create [ETL](https://aws.amazon.com/what-is/etl/) processes using [Amazon Kinesis](https://aws.amazon.com/pm/kinesis/), [Python], [PySpark](https://spark.apache.org/), and [Amazon Data Pipeline](https://docs.aws.amazon.com/datapipeline/latest/DeveloperGuide/what-is-datapipeline.html) to load structured event data from [PostgreSQL] databases into [Amazon Redshift](https://aws.amazon.com/pm/redshift/). 
+• Saved data to [Amazon S3] using [Amazon Kinesis] and triggered [Amazon Lambda](https://docs.aws.amazon.com/lambda/) jobs to aggregate steaming event data into [schema-on-read] file formats, [Apache Avro](https://avro.apache.org/) and [Apache Parquet](https://parquet.apache.org/).
+• Steered efforts in creating a [Data Lake](https://aws.amazon.com/big-data/datalakes-and-analytics/datalakes/) using [PostgreSQL] and [FlyWay](https://flywaydb.org/) with [Python] and [PySpark](https://spark.apache.org/docs/latest/api/python/index.html) pre-processing on [EC2 instances] using shared [Amazon EFS](https://zesty.co/blog/ebs-vs-efs-which-is-right) for staged storage.
+• Used streaming event messages queued in [RabbitMQ](https://docs.aws.amazon.com/amazon-mq/latest/developer-guide/working-with-rabbitmq.html) and [Amazon Kinesis] to build [type-2 slowly changing dimensions] and accumulative facts tables. 
+• Designed and implemented a custom [star-schema warehouse](https://www.databricks.com/glossary/star-schema) and [ETL] processes to [de-normalize](https://en.wikipedia.org/wiki/Denormalization) and load data into [Amazon Redshift](https://aws.amazon.com/redshift/) data warehouse for BI reporting using [Tableau](https://www.tableau.com/).
+• [Test-driven development](https://www.pluralsight.com/blog/software-development/tdd-vs-bdd) using [bash], [Linux], [Python], [PyCharm], [PyTest], [Unit-test], [GitHub], [Jira], and [Jenkins](https://www.jenkins.io/).</t>
   </si>
 </sst>
 </file>
@@ -466,7 +405,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -521,11 +460,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF008080"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFD700"/>
       </patternFill>
     </fill>
     <fill>
@@ -588,7 +522,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -650,12 +584,12 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -663,9 +597,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -985,21 +916,21 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="201" zoomScaleNormal="201" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="400" zoomScaleNormal="201" workbookViewId="0">
+      <selection activeCell="C3" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.1640625" style="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" style="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13" style="28" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="10.83203125" style="27" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="96" style="30" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.1640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" style="27" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="28" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="10.83203125" style="26" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="96" style="29" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -1037,40 +968,40 @@
     </row>
     <row r="2" spans="1:10" ht="160" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>10</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>11</v>
       </c>
       <c r="C2" s="7">
         <v>45047</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="E2" s="8">
         <v>3</v>
       </c>
       <c r="F2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>13</v>
       </c>
       <c r="H2" s="9"/>
       <c r="I2" s="6" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="192" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="176" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="7">
         <v>44805</v>
@@ -1082,25 +1013,25 @@
         <v>2</v>
       </c>
       <c r="F3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>16</v>
       </c>
       <c r="H3" s="11"/>
       <c r="I3" s="6" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="192" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="7">
         <v>44501</v>
@@ -1112,25 +1043,25 @@
         <v>1</v>
       </c>
       <c r="F4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>18</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>19</v>
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="6" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" s="7">
         <v>44136</v>
@@ -1142,25 +1073,25 @@
         <v>2</v>
       </c>
       <c r="F5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>22</v>
       </c>
       <c r="H5" s="13"/>
       <c r="I5" s="6" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C6" s="7">
         <v>43770</v>
@@ -1172,25 +1103,25 @@
         <v>1</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H6" s="14"/>
       <c r="I6" s="6" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="335" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="320" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="C7" s="7">
         <v>42795</v>
@@ -1202,25 +1133,25 @@
         <v>2</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H7" s="15"/>
       <c r="I7" s="6" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>30</v>
+        <v>72</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C8" s="7">
         <v>42705</v>
@@ -1232,25 +1163,25 @@
         <v>1</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H8" s="16"/>
       <c r="I8" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="J8" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="J8" s="10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="335" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:10" ht="350" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>34</v>
+        <v>76</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C9" s="7">
         <v>40575</v>
@@ -1262,25 +1193,25 @@
         <v>2</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="H9" s="17"/>
       <c r="I9" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="192" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>34</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>38</v>
       </c>
       <c r="C10" s="7">
         <v>37561</v>
@@ -1292,25 +1223,25 @@
         <v>1</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H10" s="18"/>
       <c r="I10" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="224" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>34</v>
+        <v>76</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C11" s="7">
         <v>35827</v>
@@ -1322,25 +1253,25 @@
         <v>1</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H11" s="19"/>
       <c r="I11" s="6" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>112</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="144" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C12" s="7">
         <v>35217</v>
@@ -1352,25 +1283,25 @@
         <v>1</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H12" s="9"/>
       <c r="I12" s="6" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>106</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="335" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C13" s="7">
         <v>33117</v>
@@ -1382,25 +1313,25 @@
         <v>2</v>
       </c>
       <c r="F13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>16</v>
       </c>
       <c r="H13" s="11"/>
       <c r="I13" s="6" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>111</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="304" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C14" s="7">
         <v>32021</v>
@@ -1412,25 +1343,25 @@
         <v>2</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H14" s="12"/>
       <c r="I14" s="6" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>110</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C15" s="7">
         <v>32295</v>
@@ -1442,347 +1373,167 @@
         <v>3</v>
       </c>
       <c r="F15" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>22</v>
       </c>
       <c r="H15" s="13"/>
       <c r="I15" s="6" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="112" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>50</v>
       </c>
       <c r="C16" s="7">
-        <v>30926</v>
+        <v>39417</v>
       </c>
       <c r="D16" s="7">
-        <v>32021</v>
+        <v>40391</v>
       </c>
       <c r="E16" s="8">
         <v>2</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="H16" s="14"/>
+        <v>52</v>
+      </c>
+      <c r="H16" s="20"/>
       <c r="I16" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="J16" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="J16" s="21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="128" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="7">
+        <v>38749</v>
+      </c>
+      <c r="D17" s="7">
+        <v>39417</v>
+      </c>
+      <c r="E17" s="8">
+        <v>2</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G17" s="6" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" ht="48" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
+      <c r="H17" s="22"/>
+      <c r="I17" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="J17" s="10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="112" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="C18" s="7">
+        <v>38384</v>
+      </c>
+      <c r="D18" s="7">
+        <v>38749</v>
+      </c>
+      <c r="E18" s="8">
+        <v>2</v>
+      </c>
+      <c r="F18" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="7">
-        <v>30682</v>
-      </c>
-      <c r="D17" s="7">
-        <v>30926</v>
-      </c>
-      <c r="E17" s="8">
-        <v>1</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="H17" s="15"/>
-      <c r="I17" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="J17" s="10" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="64" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
+      <c r="G18" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="H18" s="23"/>
+      <c r="I18" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="J18" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="7">
-        <v>30133</v>
-      </c>
-      <c r="D18" s="7">
-        <v>30682</v>
-      </c>
-      <c r="E18" s="8">
-        <v>3</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H18" s="16"/>
-      <c r="I18" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="J18" s="10" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>50</v>
-      </c>
       <c r="C19" s="7">
-        <v>29830</v>
+        <v>38018</v>
       </c>
       <c r="D19" s="7">
-        <v>30133</v>
+        <v>38384</v>
       </c>
       <c r="E19" s="8">
         <v>2</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="H19" s="17"/>
+        <v>61</v>
+      </c>
+      <c r="H19" s="24"/>
       <c r="I19" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="144" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="C20" s="7">
+        <v>37681</v>
+      </c>
+      <c r="D20" s="7">
+        <v>38018</v>
+      </c>
+      <c r="E20" s="8">
+        <v>2</v>
+      </c>
+      <c r="F20" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="7">
-        <v>29677</v>
-      </c>
-      <c r="D20" s="7">
-        <v>29830</v>
-      </c>
-      <c r="E20" s="8">
-        <v>1</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>39</v>
-      </c>
       <c r="G20" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="H20" s="18"/>
+        <v>64</v>
+      </c>
+      <c r="H20" s="25"/>
       <c r="I20" s="6" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="80" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C21" s="7">
-        <v>28369</v>
-      </c>
-      <c r="D21" s="7">
-        <v>29677</v>
-      </c>
-      <c r="E21" s="8">
-        <v>1</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="H21" s="20"/>
-      <c r="I21" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="J21" s="10" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="112" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C22" s="7">
-        <v>39417</v>
-      </c>
-      <c r="D22" s="7">
-        <v>40391</v>
-      </c>
-      <c r="E22" s="8">
-        <v>2</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="H22" s="21"/>
-      <c r="I22" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="J22" s="22" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="128" x14ac:dyDescent="0.2">
-      <c r="A23" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C23" s="7">
-        <v>38749</v>
-      </c>
-      <c r="D23" s="7">
-        <v>39417</v>
-      </c>
-      <c r="E23" s="8">
-        <v>2</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="H23" s="23"/>
-      <c r="I23" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="J23" s="10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="112" x14ac:dyDescent="0.2">
-      <c r="A24" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C24" s="7">
-        <v>38384</v>
-      </c>
-      <c r="D24" s="7">
-        <v>38749</v>
-      </c>
-      <c r="E24" s="8">
-        <v>2</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="H24" s="24"/>
-      <c r="I24" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="J24" s="10" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="80" x14ac:dyDescent="0.2">
-      <c r="A25" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C25" s="7">
-        <v>38018</v>
-      </c>
-      <c r="D25" s="7">
-        <v>38384</v>
-      </c>
-      <c r="E25" s="8">
-        <v>2</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="H25" s="25"/>
-      <c r="I25" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="J25" s="10" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="144" x14ac:dyDescent="0.2">
-      <c r="A26" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C26" s="7">
-        <v>37681</v>
-      </c>
-      <c r="D26" s="7">
-        <v>38018</v>
-      </c>
-      <c r="E26" s="8">
-        <v>2</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="G26" s="6" t="s">
         <v>86</v>
-      </c>
-      <c r="H26" s="26"/>
-      <c r="I26" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="J26" s="10" t="s">
-        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
index.html confirmIconTags, fixed bizcard jobStart/EndStrs, logAllBizcardDivs uniques sorted, keeps, ignores, sankey diagram, dateSortedBizcards, welcomeAlert widened and centered, jobs.xlsx trimmed and normalized
</commit_message>
<xml_diff>
--- a/static_content/jobs/jobs.xlsx
+++ b/static_content/jobs/jobs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbecker11/workspace-parallax/flock-of-postcards/static_content/jobs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E08119FD-2A06-034A-9003-435380700CFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EF515D2-9D53-444D-B085-7027FFF1656B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="2560" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-65380" yWindow="4260" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="jobs" sheetId="1" r:id="rId1"/>
@@ -61,9 +61,6 @@
     <t>#006688</t>
   </si>
   <si>
-    <t>Warner Brothers Interactive Entertainment</t>
-  </si>
-  <si>
     <t>blue</t>
   </si>
   <si>
@@ -77,9 +74,6 @@
   </si>
   <si>
     <t>#4400cd</t>
-  </si>
-  <si>
-    <t>Greenseed Tech</t>
   </si>
   <si>
     <t>blueviolet</t>
@@ -268,10 +262,59 @@
   <si>
     <t>• [Intrusic LLC](https://www.crunchbase.com/organization/intrusic) built real-time network monitoring systems that identified external and internal network intrusion attempts
 • As a Sierra Vista Group architech, I helped design and develop an approach for buffering live streaming network traffic for asynchronous package processing. 
-• Used [Debian Linux](https://www.debian.org/), [C programming language](https://www.cprogramming.com/books/ritchie.html), and [Visio](https://www.microsoft.com/en-us/microsoft-365/visio/flowchart-software).</t>
-  </si>
-  <si>
-    <t>•	Doctor of Philosopy degree, [Massachusetts Institute of Technology]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/MIT-logo.png}, Cambridge, Massachusettes
+• Used [Linux](https://www.debian.org/), [C programming language](https://www.cprogramming.com/books/ritchie.html), and [Visio](https://www.microsoft.com/en-us/microsoft-365/visio/flowchart-software).</t>
+  </si>
+  <si>
+    <t>Warner Brothers</t>
+  </si>
+  <si>
+    <t>Data Laboratory</t>
+  </si>
+  <si>
+    <t>• As a senior full stack developer for [NuSkin](https://www.nuskin.com/us/en/, an international company known for its excellent  skin and beauty products I created new [Vue.js](https://vuejs.org/), [Nuxt](https://nuxt.com/), and [Vuetify](https://vuetifyjs.com/en/) components using [Bash], [Linux], [GitHub], [NodeJS], [HTML] and [CSS].  
+• Internationalized content using [Adobe Experience Cloud](https://business.adobe.com/).</t>
+  </si>
+  <si>
+    <t>• As a senior data engineer for SeniorLink's [Vela project]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/Vela-150x126.png} a homeservices support platform, helped create [ETL](https://aws.amazon.com/what-is/etl/) processes using [Amazon Kinesis](https://aws.amazon.com/pm/kinesis/), [Python], [PySpark](https://spark.apache.org/), and [Amazon Data Pipeline](https://docs.aws.amazon.com/datapipeline/latest/DeveloperGuide/what-is-datapipeline.html) to load structured event data from [PostgreSQL] databases into [Redshift](https://aws.amazon.com/pm/redshift/). 
+• Saved data to [Amazon S3] using [Amazon Kinesis] and triggered [Amazon Lambda](https://docs.aws.amazon.com/lambda/) jobs to aggregate steaming event data into [schema-on-read] file formats, [Apache Avro](https://avro.apache.org/) and [Apache Parquet](https://parquet.apache.org/).
+• Steered efforts in creating a [Data Lake](https://aws.amazon.com/big-data/datalakes-and-analytics/datalakes/) using [PostgreSQL] and [FlyWay](https://flywaydb.org/) with [Python] and [PySpark](https://spark.apache.org/docs/latest/api/python/index.html) pre-processing on [EC2 instances] using shared [Amazon EFS](https://zesty.co/blog/ebs-vs-efs-which-is-right) for staged storage.
+• Used streaming event messages queued in [RabbitMQ](https://docs.aws.amazon.com/amazon-mq/latest/developer-guide/working-with-rabbitmq.html) and [Amazon Kinesis] to build [type-2 slowly changing dimensions] and accumulative facts tables. 
+• Designed and implemented a custom [star-schema warehouse](https://www.databricks.com/glossary/star-schema) and [ETL] processes to [de-normalize](https://en.wikipedia.org/wiki/Denormalization) and load data into [Redshift](https://aws.amazon.com/redshift/) data warehouse for BI reporting using [Tableau](https://www.tableau.com/).
+• [Test-driven development](https://www.pluralsight.com/blog/software-development/tdd-vs-bdd) using [Bash], [Linux], [Python], [PyCharm], [PyTest], [Unit-test], [GitHub], [Jira], and [Jenkins](https://www.jenkins.io/).</t>
+  </si>
+  <si>
+    <t>• Co-founded [ClipFile]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/clipfile-infrastructure-150x150.png}, a company that envisioned building a web destination where users could easily record and share their favorite pieces of content like facts, authored stories, quotes, articles, chapters, or personal thoughts, as a way of concretely defining their personal [mindset]{https://sourcesofinsight.com/wp-content/uploads/2014/04/Mindset-768x505.jpg}(https://sourcesofinsight.com/what-is-mindset/).
+• Implemented [fuzzy matching](https://nanonets.com/blog/fuzzy-matching-fuzzy-logic/), [word clustering](https://www.ilc.cnr.it/EAGLES96/rep2/node37.html#:~:text=Word%20clustering%20is%20a%20technique,to%20information%20retrieval%20and%20filtering.), [semantic similarity scores](https://towardsdatascience.com/semantic-similarity-using-transformers-8f3cb5bf66d6), and [collaborative filtering](https://www.hindawi.com/journals/aai/2009/421425/) to help users find content that matched or differed from thieir own mindset.
+• Launched a novel [SaaS] using [Amazon Web Services] that let individuals and content creators search and share mindsets.
+• Conceptualized patented technology by designing and implementing a fuil-stack consumer-facing content management system that supported tuned matching among selected attributes.
+• [Java], [J2EE], [JSP], [Servlets], [Spring], [Amazon services], [JavaScript], [JQuery], [HTML], [CSS], [JUnit], [JMeter], [JProfile].
+• Utilized [REST], [Swagger], [Apache Shiro](https://shiro.apache.org/), [Eclipse IDE](https://www.eclipse.org/home/whatis/), [Apache Maven](https://maven.apache.org/what-is-maven.html), [Apache Ant](https://ant.apache.org/), [GitHub], [Hibernate], [Amazon SimpleDB](https://aws.amazon.com/simpledb/), [Linux](https://www.centos.org/), [Apache Tomcat](https://tomcat.apache.org/), [Bash], [Linux], [Jetty](https://projects.eclipse.org/projects/rt.jetty), and [Spring MVC](https://docs.spring.io/spring-framework/reference/web/webmvc.html).
+• Served as co-founder and co-authored [four patents](https://www.freepatentsonline.com/y2013/0325870.html).</t>
+  </si>
+  <si>
+    <t>• As lead software developer, built a CD-ROM-based home design application for selecting premium home design products for previewing in the context of images of any household rooms. 
+• Built the prototype using Adobe Photoshop and [Macromedia Director](https://macromedia.fandom.com/wiki/Macromedia_Director).
+• Built the actual application using using [Bash], [Linux], [Java] and [Marimba Bongo](https://www.thriftbooks.com/w/official-marimba-guide-to-bongo_danny-goodman/2574616/#edition=58026223&amp;idiq=42367912) widget layout tool.
+• Updates for the self-updating application were delivered over the internet using [Marimba Castanet](https://www.infoworld.com/article/2076707/marimba-launches-new-castanet-with-a-less-java-centric-focus.html) push-technology.</t>
+  </si>
+  <si>
+    <t>• Front-end software developer of a reverse kinametics path planning system for multi-axis industrial robots for [Cimmetrix]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/Cimetrix-PDF-combined-logo-150x100.png}.
+• Technologies used include [Bash], [Linux], [C programming language], [Bash](https://en.wikipedia.org/wiki/Bourne_shell), [X11] , [Xt toolkit intrinsics](https://en.wikipedia.org/wiki/X_Toolkit_Intrinsics), [Silicon Graphics Irix](https://en.wikipedia.org/wiki/Silicon_Graphics), and [HP-UX](https://en.wikipedia.org/wiki/HP-UX).</t>
+  </si>
+  <si>
+    <t>•  AMI (https://amientertainment.com/) was the internet-music distribution incarnation of Rowe International.  
+•  As a Sierra Vista Group project manager and technical lead, I helped design and implement their system for making monthly ACH royalty payments to music copyright owners for mechanical and performance licensing rights.
+•  Used [FileMaker Pro](https://www.claris.com/filemaker/), [Bash], [Linux], [HTML], [CSS], [JavaScript], [Java], and [Visio](https://www.microsoft.com/en-us/microsoft-365/visio/flowchart-software).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">•  [Rowe International](https://pitchbook.com/profiles/company/13178-08) was the leading manufacturer of music jukeboxes. 
+•  Sierra Vista Group was consulted to assess their available technologies and create a plan to build their back-end systems to let them become a leading provider of internet-based music.
+•  As project manager and technical lead created the project plan and led the development of a full-stack web application used by  jukebox owners and Rowe sales and marketing.
+•  Used [Java], [Bash], [Linux], [HTML], [CSS], [JavaScript], [ObjectDesign](https://object.design/), [MySQL](https://www.mysql.com/), and [Adobe Photoshop](https://www.adobe.com/products/photoshop.html). 
+</t>
+  </si>
+  <si>
+    <t>•	Doctor of Philosopy degree, [MIT]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/MIT-logo.png}, Cambridge, Massachusettes
 •	Media Laboratory, Media Arts and Sciences
 •	Took courses in machine vision, signals and systems, digital signal processing, and stochastics.
 •	Helped build the operating system for the [Cheops multi-processor system](http://alumni.media.mit.edu/~wad/cheops_CSVT/cheops.html) used for digital video research and for holographic video
@@ -281,99 +324,56 @@
 •	“Semiautomatic Camera Lens Calibration from Partially Known Structure”, Shawn Becker, MIT Media Lab Reports, 1994
 •	[“Formulating a scene probability equation to differentiate the effects of shape &amp; albedo on image brightness.”](https://www.researchgate.net/publication/2668457_Formulating_a_Scene_Probability_Equation_to_Differentiate_the_Effects_of_Shape_and_Albedo_on_Image_Brightness) Shawn Becker, MIT Media Lab Reports, 1994
 •	“Computation of some projective-chirplet-transform &amp; metaplectic-chirplet-transform subspaces, with applications in image processing.” Steve Mann &amp; Shawn Becker, DSP World Symposium, Boston, Massachusetts, November 1992.
-• [C programming language], [TclTk], [X11], [HTML], [JavaScript],[CSS],[XMotif], [bash], [Linux]</t>
-  </si>
-  <si>
-    <t>• As a senior full stack developer for [NuSkin](https://www.nuskin.com/us/en/, an international company known for its excellent  skin and beauty products I created new [Vue.js](https://vuejs.org/), [Nuxt](https://nuxt.com/), and [Vuetify](https://vuetifyjs.com/en/) components using [bash], [Linux], [GitHub], [NodeJS], [HTML] and [CSS].  
-• Internationalized content using [Adobe Experience Cloud](https://business.adobe.com/).</t>
-  </si>
-  <si>
-    <t>• As co-founder and CTO, designed and led the development of a public website used by discerning home designers and builders called [HomePortfolio.com](https://homeportfolio.com/). 
+• [C programming language], [TclTk], [X11], [HTML], [JavaScript],[CSS],[XMotif], [Bash], [Linux]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• [Eleven LLC](https://www.eleven.net/) built mobile apps used by beverage industry distributors to help manage placement  of their products in the shelves and coolers in retail locations. The work done by the Sierra Vista Group was instrumental in their company being acquired by [Trimble](https://help.trimblegeospatial.com/TMM/Home.htm). 
+• As the architect and team lead, we used [Java], [Bash], [GitHub], [Linux], and  [JBoss](https://developers.redhat.com/products/eap/overview) message-oriented middleware platform, [Sybase Anywhere](https://texas.gs.shi.com/Product/30451452/Sybase-SQL-Anywhere-Advanced-Edition) for the client/server based database, and [Windows Mobile](https://en.wikipedia.org/wiki/Windows_Mobile_5.0) running on ruggedized mobile devices. </t>
+  </si>
+  <si>
+    <t>• As co-founder and CTO, designed and led the development of a public website used by discerning home designers and builders called [HomePortfolio](https://HomePortfolio/). 
 • Hired a staff of  10 software and databases developers. 
 • Worked with data acquisition team to scan and tag over 700,000 premium home design products from over 2,000 manufactures and vendors.
 • Designed datamodel and data entry tools for category-specific product attribution. 
 • Helped extended the business model to provide online product selection tools for participating vendors and manufacturers.
 • Instrumental in raising over $70M in venture capital. 
-• Used [Oracle], [ATG Dyanamo]( https://docs.oracle.com/cd/E24152_01/Platform.10-1/ATGPersBusinessGuide/html/s0102dynamoapplicationframework01.html), [Java], [Akamai]{https://www.hiclipart.com/free-transparent-background-png-clipart-zkmsn}(https://www.akamai.com/), [WebTrends](https://www.webtrends.com/), [FileMakerPro], [ImageMagik](https://imagemagick.org/index.php), [bash], [Linux], [HTML], [JavaScript], [CSS], and [Omnigraffle](https://www.omnigroup.com/omnigraffle) for data modeling and workflow designs.</t>
-  </si>
-  <si>
-    <t>• As lead software developer, built a CD-ROM-based home design application for selecting premium home design products for previewing in the context of images of any household rooms. 
-• Built the prototype using Adobe Photoshop and [Macromedia Director](https://macromedia.fandom.com/wiki/Macromedia_Director).
-• Built the actual application using using [bash], [Linux], [Java] and [Marimba Bongo](https://www.thriftbooks.com/w/official-marimba-guide-to-bongo_danny-goodman/2574616/#edition=58026223&amp;idiq=42367912) widget layout tool.
-• Updates for the self-updating application were delivered over the internet using [Marimba Castanet](https://www.infoworld.com/article/2076707/marimba-launches-new-castanet-with-a-less-java-centric-focus.html) push-technology.</t>
-  </si>
-  <si>
-    <t>• Masters of Science degree, [Brigham Young University]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/BYU-entrance-150x150.jpg}, Provo, Utah
+• Used [Oracle], [ATG Dyanamo]( https://docs.oracle.com/cd/E24152_01/Platform.10-1/ATGPersBusinessGuide/html/s0102dynamoapplicationframework01.html), [Java], [Akamai]{https://www.hiclipart.com/free-transparent-background-png-clipart-zkmsn}(https://www.akamai.com/), [WebTrends](https://www.webtrends.com/), [FileMakerPro], [ImageMagik](https://imagemagick.org/index.php), [Bash], [Linux], [HTML], [JavaScript], [CSS], and [Omnigraffle](https://www.omnigroup.com/omnigraffle) for data modeling and workflow designs.</t>
+  </si>
+  <si>
+    <t>• Masters of Science degree, [BYU]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/BYU-entrance-150x150.jpg}, Provo, Utah
 Took all courses required for both bachelors and masters degrees in Computer Science
 • Thesis project [“Interactive Measurement of Three-Dimensional Objects Using a Depth Buffer &amp; Linear Probe.”](https://dl.acm.org/doi/pdf/10.1145/108360.108446) CS MS Thesis, Shawn Becker, William A. Barrett &amp; Dan R. Olsen, ACM Transactions on Graphics, Vol. 10, No. 2, April 1991
-• Top Research Presentation – New Tech Research Conference - Brigham Young University – Provo, UT – March 1990
+• Top Research Presentation – New Tech Research Conference - BYU – Provo, UT – March 1990
 • [“Fast Automated Object Detection Using Signature Parsing.”](https://www.spiedigitallibrary.org/conference-proceedings-of-spie/1192/1/Fast-Automated-Object-Detection-Using-Signature-Parsing/10.1117/12.969720.short) Tim Heaton; Shawn Becker; Kelley Anderson; William Barrett: Proceedings Volume 1192, Intelligent Robots &amp; Computer Vision VIII: Algorithms &amp; Techniques; (1990) https://doi.org/10.1117/12.969720
 • [“Probabilistic Segmentation of Myocardial Tissue by Deterministic Relaxation.”](https://scholarsarchive.byu.edu/cgi/viewcontent.cgi?article=1737&amp;context=facpub) Jerome A. Broekhuijsen, Shawn C. Becker, &amp; William A. Barrett: IEEE Proceedings of Computers in Cardiology, pp. 99-12, Jerusalem, September 1989.
 • [“Interactive Measurement of three-Dimensional Cardiac Morphology.”]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/BYU-MS-CS-Skull-Cross-Section-1.jpeg}(https://scholarsarchive.byu.edu/cgi/viewcontent.cgi?article=1736&amp;context=facpub) Shawn C Becker, William A Barrett, October 1989, DOI: 10.1109/CIC.1989.130586, Conference: Computers in Cardiology.
-• [C programming language], [bash], [Linux], [XMotif], and [X11].</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• [Eleven LLC](https://www.eleven.net/) built mobile apps used by beverage industry distributors to help manage placement  of their products in the shelves and coolers in retail locations. The work done by the Sierra Vista Group was instrumental in their company being acquired by [Trimble Mobile Solutions](https://help.trimblegeospatial.com/TMM/Home.htm). 
-• As the architect and team lead, we used [Java], [bash], [GitHub], [Linix], and  [JBoss](https://developers.redhat.com/products/eap/overview) message-oriented middleware platform, [Sybase Anywhere](https://texas.gs.shi.com/Product/30451452/Sybase-SQL-Anywhere-Advanced-Edition) for the client/server based database, and [Windows Mobile](https://en.wikipedia.org/wiki/Windows_Mobile_5.0) running on ruggedized mobile devices. </t>
-  </si>
-  <si>
-    <t>•  AMI (https://amientertainment.com/) was the internet-music distribution incarnation of Rowe International.  
-•  As a Sierra Vista Group project manager and technical lead, I helped design and implement their system for making monthly ACH royalty payments to music copyright owners for mechanical and performance licensing rights.
-•  Used [FileMaker Pro](https://www.claris.com/filemaker/), [bash], [Linux], [HTML], [CSS], [JavaScript], [Java], and [Visio](https://www.microsoft.com/en-us/microsoft-365/visio/flowchart-software).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">•  [Rowe International](https://pitchbook.com/profiles/company/13178-08) was the leading manufacturer of music jukeboxes. 
-•  Sierra Vista Group was consulted to assess their available technologies and create a plan to build their back-end systems to let them become a leading provider of internet-based music.
-•  As project manager and technical lead created the project plan and led the development of a full-stack web application used by  jukebox owners and Rowe sales and marketing.
-•  Used [Java], [bash], [Linux], [HTML], [CSS], [JavaScript], [ObjectDesign](https://object.design/), [MySQL](https://www.mysql.com/), and [Adobe Photoshop](https://www.adobe.com/products/photoshop.html). 
-</t>
+• [C programming language], [Bash], [Linux], [XMotif], and [X11].</t>
   </si>
   <si>
     <t>• As a senior software engineer at [BigR.io]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/Bigr.io_-150x106.png} I used [Amazon microservices] for custom voice-based [natural language processing] applications.
-• Used [Apache ActiveMQ](https://activemq.apache.org/), [Swagger](https://swagger.io/), [JSON], [Jackson](url), [AOP](https://www.baeldung.com/spring-aop), [Eclipse], [Maven], [GitHub], [Jira], and [Jenkins].
-• [Java], [J2EE], [Servlets], [Spring], [SpringBoot], [JAX-RS], [bash], [Linux], [JUnit], [JMeter], and [JProfile]</t>
-  </si>
-  <si>
-    <t>• As a senior data engineer in the data cyber security team of the [Cigna Group](https://www.thecignagroup.com/) created a [REST API](url) using [Postman](https://www.postman.com/), [bash], [Linux], and [OpenAPI](https://openapi-generator.tech/) for pulling credentials from the [CyberArk identity security platform](https://www.cyberark.com/) using [mutual TLS SSL authentication](https://docs.solace.com/Security/Two-Way-SSL-Authentication.htm) with [Amazon API Gateway](https://docs.aws.amazon.com/apigateway/). 
-•  Migrated a suite of legacy data pipeline [Python] elements running on the [Unity IoC platform](http://unitycontainer.org/articles/introduction.html) to pull credentials from the CyberArk service at runtime rather than using [Fernet](https://cryptography.io/en/latest/fernet/) encrypted local files. 
+• Used [Apache ActiveMQ](https://activemq.apache.org/), [Swagger](https://swagger.io/), [JSON], [Jackson](url), [AOP](https://www.baeldung.com/spring-aop), [Eclipse], [Maven], [GitHub], [Jira], [PostgreSQL], and [Jenkins].
+• [Java], [J2EE], [Servlets], [Spring], [SpringBoot], [JAX-RS], [Bash], [Linux], [JUnit], [JMeter], and [JProfile]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• As a senior software engineer for Data Laboratory, an internet company that provides daily lead reports for independent real-estage agents world-wide, I  [containerized] legacy web applications using [Bash], [Linux], [GitHub], [Docker](https://www.docker.com/) and [Amazon Secrets Manager](https://aws.amazon.com/secrets-manager/). 
+• Updated legacy web apps using [Bash], [Linux], [HTML], [CSS], [JavaScript], [PostgreSQL], [NGINX], and [OpenSSL].
+• Documented existing data architecture as [ERDs](https://www.lucidchart.com/pages/er-diagrams) using [DBeaver Enterprise](https://dbeaver.com/dbeaver-enterprise/). </t>
+  </si>
+  <si>
+    <t>• As a senior data engineer for [Angel Studios](https://www.angel.com/home), a streaming media service that offers family-friendly entertainment that amplifies light, with titles including The Chosen, Dry Bar Comedy, and Tuttle Twins.
+• Used [Python], [GitHub], [Pandas], [Numpy], [Keras], [Bash], [Linux], [PostgreSQL], and [Jupyter](https://jupyter.org/) to build and tune hyperparameters of a [convolutional neural network](https://towardsdatascience.com/a-comprehensive-guide-to-convolutional-neural-networks-the-eli5-way-3bd2b1164a53) with [supervised learning] on [Amazon Sagemaker](https://aws.amazon.com/pm/sagemaker/) to classify movie frames from episodic programs stored in [Amazon S3](https://aws.amazon.com/s3/storage-classes). 
+• Built web client apps using [Python] with [Postman](https://www.postman.com/) that made [REST] requests to pull monthly usage data from various web marketing partners like [FaceBook Marketing](https://www.quora.com/What-is-Facebook-Marketing-1), [Google Play](https://play.google/howplayworks/) , and [Vimeo](https://vimeo.com/). 
+• Worked with [Segment customer data platform](https://segment.com/customer-data-platform/), [Excel], and [Tableau] to create scheduled reports for the company's sales and finance teams.</t>
+  </si>
+  <si>
+    <t>• As a senior data engineer in the analytics team of [Warner Brothers](https://warnerbrosgames.com/) Division, I implemented high-volume pipeline integrations shuffling game telemetry and [user PII data] between WB-distributed consumer games and [marketing service platforms] via [Segment customer data platform](https://segment.com/customer-data-platform/) using [Kafka](https://aws.amazon.com/msk/), [Redshift](https://aws.amazon.com/redshift/), and [Apache Airflow](https://airflow.apache.org). 
+• Employed [Python], [GitHub], [Bash], [Linux], [Amazon Glue](https://aws.amazon.com/glue/) and [Apache Airflow](https://airflow.apache.org/) for external 3rd-party integrations and internal dev-ops integrations with [Jenkins], [PostgreSQL], [DataDog](https://www.datadoghq.com/), and [ZenDesk](https://zendesk.com) 
+• Integrated with [Google BigQuery data warehouse](https://cloud.google.com/bigquery using  [Apache Airflow](https://aws.amazon.com/managed-workflows-for-apache-airflow/), [Amazon S3], and [Redshift](https://aws.amazon.com/redshift/).</t>
+  </si>
+  <si>
+    <t>• As a senior data engineer in the data cyber security team of the [Cigna Group](https://www.thecignagroup.com/) created a [REST](url) using [Postman](https://www.postman.com/), [Bash], [Linux], and [OpenAPI](https://openapi-generator.tech/) for pulling credentials from the [CyberArk identity security platform](https://www.cyberark.com/) using [mutual TLS SSL authentication](https://docs.solace.com/Security/Two-Way-SSL-Authentication.htm) with [API Gateway](https://docs.aws.amazon.com/apigateway/). 
+•  Migrated a suite of legacy data pipeline [Python] elements running on the [Unity IoC platform](http://unitycontainer.org/articles/introduction.html) with [PostgreSQL] to pull credentials from the CyberArk service at runtime rather than using [Fernet](https://cryptography.io/en/latest/fernet/) encrypted local files. 
 •  Upgraded [GitHub] apps to use [Jenkins](https://docs.aws.amazon.com/apigateway/) CI/CD pipeline for build, applying sofware and cyber-secutity code checks, and on-prem server installation.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• As a senior software engineer for Greenseed Tech, an internet company that provides daily lead reports for independent real-estage agents world-wide, I  [containerized] legacy web applications using [bash], [Linux], [GitHub], [Docker](https://www.docker.com/) and [Amazon Secrets Manager](https://aws.amazon.com/secrets-manager/). 
-• Updated legacy web apps using [bash], [Linux], [HTML], [CSS], [JavaScript], [NGINX], and [OpenSSL].
-• Documented existing data architecture as [ERDs](https://www.lucidchart.com/pages/er-diagrams) using [DBeaver Enterprise](https://dbeaver.com/dbeaver-enterprise/). </t>
-  </si>
-  <si>
-    <t>• Co-founded [ClipFile]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/clipfile-infrastructure-150x150.png}, a company that envisioned building a web destination where users could easily record and share their favorite pieces of content like facts, authored stories, quotes, articles, chapters, or personal thoughts, as a way of concretely defining their personal [mindset]{https://sourcesofinsight.com/wp-content/uploads/2014/04/Mindset-768x505.jpg}(https://sourcesofinsight.com/what-is-mindset/).
-• Implemented [fuzzy matching](https://nanonets.com/blog/fuzzy-matching-fuzzy-logic/), [word clustering](https://www.ilc.cnr.it/EAGLES96/rep2/node37.html#:~:text=Word%20clustering%20is%20a%20technique,to%20information%20retrieval%20and%20filtering.), [semantic similarity scores](https://towardsdatascience.com/semantic-similarity-using-transformers-8f3cb5bf66d6), and [collaborative filtering](https://www.hindawi.com/journals/aai/2009/421425/) to help users find content that matched or differed from thieir own mindset.
-• Launched a novel [SaaS] using [Amazon Web Services] that let individuals and content creators search and share mindsets.
-• Conceptualized patented technology by designing and implementing a fuil-stack consumer-facing content management system that supported tuned matching among selected attributes.
-• [Java], [J2EE], [JSP], [Servlets], [Spring], [Amazon services], [JavaScript], [JQuery], [HTML], [CSS], [JUnit], [JMeter], [JProfile].
-• Utilized [REST API], [Swagger], [Apache Shiro](https://shiro.apache.org/), [Eclipse IDE](https://www.eclipse.org/home/whatis/), [Apache Maven](https://maven.apache.org/what-is-maven.html), [Apache Ant](https://ant.apache.org/), [GitHub], [Hibernate], [Amazon SimpleDB](https://aws.amazon.com/simpledb/), [CentOS Linux](https://www.centos.org/), [Apache Tomcat](https://tomcat.apache.org/), [bash], [Linux], [Jetty](https://projects.eclipse.org/projects/rt.jetty), and [Spring MVC](https://docs.spring.io/spring-framework/reference/web/webmvc.html).
-• Served as co-founder and co-authored [four patents](https://www.freepatentsonline.com/y2013/0325870.html).</t>
-  </si>
-  <si>
-    <t>• As a senior data engineer in the analytics team of [Warner Brothers Interactive Entertainment](https://warnerbrosgames.com/) Division, I implemented high-volume pipeline integrations shuffling game telemetry and [user PII data] between WB-distributed consumer games and [marketing service platforms] via [Segment customer data platform](https://segment.com/customer-data-platform/) using [Kafka](https://aws.amazon.com/msk/), [Amazon Redshift](https://aws.amazon.com/redshift/), and [Apache Airflow](https://airflow.apache.org). 
-• Employed [Python], [GitHub], [bash], [Linux], [Amazon Glue](https://aws.amazon.com/glue/) and [Apache Airflow](https://airflow.apache.org/) for external 3rd-party integrations and internal dev-ops integrations with [Jenkins], [DataDog](https://www.datadoghq.com/), and [ZenDesk](https://zendesk.com) 
-• Integrated with [Google BigQuery data warehouse](https://cloud.google.com/bigquery using  [Apache Airflow](https://aws.amazon.com/managed-workflows-for-apache-airflow/), [Amazon S3], and [Amazon Redshift](https://aws.amazon.com/redshift/).</t>
-  </si>
-  <si>
-    <t>• Front-end software developer of a reverse kinametics path planning system for multi-axis industrial robots for [Cimmetrix]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/Cimetrix-PDF-combined-logo-150x100.png}.
-• Technologies used include [bash], [Linux], [C programming language], [bash](https://en.wikipedia.org/wiki/Bourne_shell), [X11] , [Xt toolkit intrinsics](https://en.wikipedia.org/wiki/X_Toolkit_Intrinsics), [Silicon Graphics Irix](https://en.wikipedia.org/wiki/Silicon_Graphics), and [HP-UX](https://en.wikipedia.org/wiki/HP-UX).</t>
-  </si>
-  <si>
-    <t>• As a senior data engineer for [Angel Studios](https://www.angel.com/home), a streaming media service that offers family-friendly entertainment that amplifies light, with titles including The Chosen, Dry Bar Comedy, and Tuttle Twins.
-• Used [Python], [GitHub], [Pandas], [Numpy], [Keras], [bash], [Linux], and [Jupyter](https://jupyter.org/) to build and tune hyperparameters of a [convolutional neural network](https://towardsdatascience.com/a-comprehensive-guide-to-convolutional-neural-networks-the-eli5-way-3bd2b1164a53) with [supervised learning] on [Amazon Sagemaker](https://aws.amazon.com/pm/sagemaker/) to classify movie frames from episodic programs stored in [Amazon S3](https://aws.amazon.com/s3/storage-classes). 
-• Built web client apps using [Python] with [Postman](https://www.postman.com/) that made [REST API] requests to pull monthly usage data from various web marketing partners like [FaceBook Marketing](https://www.quora.com/What-is-Facebook-Marketing-1), [Google Play](https://play.google/howplayworks/) , and [Vimeo](https://vimeo.com/). 
-• Worked with [Segment customer data platform](https://segment.com/customer-data-platform/), [Excel], and [Tableau] to create scheduled reports for the company's sales and finance teams.</t>
-  </si>
-  <si>
-    <t>• As a senior data engineer for SeniorLink's [Vela project]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/Vela-150x126.png} a homeservices support platform, helped create [ETL](https://aws.amazon.com/what-is/etl/) processes using [Amazon Kinesis](https://aws.amazon.com/pm/kinesis/), [Python], [PySpark](https://spark.apache.org/), and [Amazon Data Pipeline](https://docs.aws.amazon.com/datapipeline/latest/DeveloperGuide/what-is-datapipeline.html) to load structured event data from [PostgreSQL] databases into [Amazon Redshift](https://aws.amazon.com/pm/redshift/). 
-• Saved data to [Amazon S3] using [Amazon Kinesis] and triggered [Amazon Lambda](https://docs.aws.amazon.com/lambda/) jobs to aggregate steaming event data into [schema-on-read] file formats, [Apache Avro](https://avro.apache.org/) and [Apache Parquet](https://parquet.apache.org/).
-• Steered efforts in creating a [Data Lake](https://aws.amazon.com/big-data/datalakes-and-analytics/datalakes/) using [PostgreSQL] and [FlyWay](https://flywaydb.org/) with [Python] and [PySpark](https://spark.apache.org/docs/latest/api/python/index.html) pre-processing on [EC2 instances] using shared [Amazon EFS](https://zesty.co/blog/ebs-vs-efs-which-is-right) for staged storage.
-• Used streaming event messages queued in [RabbitMQ](https://docs.aws.amazon.com/amazon-mq/latest/developer-guide/working-with-rabbitmq.html) and [Amazon Kinesis] to build [type-2 slowly changing dimensions] and accumulative facts tables. 
-• Designed and implemented a custom [star-schema warehouse](https://www.databricks.com/glossary/star-schema) and [ETL] processes to [de-normalize](https://en.wikipedia.org/wiki/Denormalization) and load data into [Amazon Redshift](https://aws.amazon.com/redshift/) data warehouse for BI reporting using [Tableau](https://www.tableau.com/).
-• [Test-driven development](https://www.pluralsight.com/blog/software-development/tdd-vs-bdd) using [bash], [Linux], [Python], [PyCharm], [PyTest], [Unit-test], [GitHub], [Jira], and [Jenkins](https://www.jenkins.io/).</t>
   </si>
 </sst>
 </file>
@@ -918,8 +918,8 @@
   </sheetPr>
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="400" zoomScaleNormal="201" workbookViewId="0">
-      <selection activeCell="C3" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="400" zoomScaleNormal="201" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -968,7 +968,7 @@
     </row>
     <row r="2" spans="1:10" ht="160" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>10</v>
@@ -977,7 +977,7 @@
         <v>45047</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E2" s="8">
         <v>3</v>
@@ -990,18 +990,18 @@
       </c>
       <c r="H2" s="9"/>
       <c r="I2" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="176" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="C3" s="7">
         <v>44805</v>
@@ -1013,25 +1013,25 @@
         <v>2</v>
       </c>
       <c r="F3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>15</v>
       </c>
       <c r="H3" s="11"/>
       <c r="I3" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="192" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="7">
         <v>44501</v>
@@ -1043,25 +1043,25 @@
         <v>1</v>
       </c>
       <c r="F4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>18</v>
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>19</v>
+        <v>78</v>
       </c>
       <c r="C5" s="7">
         <v>44136</v>
@@ -1073,25 +1073,25 @@
         <v>2</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H5" s="13"/>
       <c r="I5" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C6" s="7">
         <v>43770</v>
@@ -1103,25 +1103,25 @@
         <v>1</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H6" s="14"/>
       <c r="I6" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="320" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C7" s="7">
         <v>42795</v>
@@ -1133,25 +1133,25 @@
         <v>2</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H7" s="15"/>
       <c r="I7" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C8" s="7">
         <v>42705</v>
@@ -1163,25 +1163,25 @@
         <v>1</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H8" s="16"/>
       <c r="I8" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="350" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C9" s="7">
         <v>40575</v>
@@ -1193,25 +1193,25 @@
         <v>2</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H9" s="17"/>
       <c r="I9" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="192" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C10" s="7">
         <v>37561</v>
@@ -1223,25 +1223,25 @@
         <v>1</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H10" s="18"/>
       <c r="I10" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="224" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C11" s="7">
         <v>35827</v>
@@ -1253,25 +1253,25 @@
         <v>1</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H11" s="19"/>
       <c r="I11" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="144" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C12" s="7">
         <v>35217</v>
@@ -1286,11 +1286,11 @@
         <v>11</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H12" s="9"/>
       <c r="I12" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J12" s="10" t="s">
         <v>82</v>
@@ -1298,10 +1298,10 @@
     </row>
     <row r="13" spans="1:10" ht="335" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C13" s="7">
         <v>33117</v>
@@ -1313,25 +1313,25 @@
         <v>2</v>
       </c>
       <c r="F13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>15</v>
       </c>
       <c r="H13" s="11"/>
       <c r="I13" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="304" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C14" s="7">
         <v>32021</v>
@@ -1343,25 +1343,25 @@
         <v>2</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H14" s="12"/>
       <c r="I14" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C15" s="7">
         <v>32295</v>
@@ -1373,25 +1373,25 @@
         <v>3</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H15" s="13"/>
       <c r="I15" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="112" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C16" s="7">
         <v>39417</v>
@@ -1403,25 +1403,25 @@
         <v>2</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H16" s="20"/>
       <c r="I16" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J16" s="21" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="128" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="112" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C17" s="7">
         <v>38749</v>
@@ -1433,25 +1433,25 @@
         <v>2</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H17" s="22"/>
       <c r="I17" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="112" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C18" s="7">
         <v>38384</v>
@@ -1463,25 +1463,25 @@
         <v>2</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H18" s="23"/>
       <c r="I18" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C19" s="7">
         <v>38018</v>
@@ -1493,25 +1493,25 @@
         <v>2</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H19" s="24"/>
       <c r="I19" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="144" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C20" s="7">
         <v>37681</v>
@@ -1523,17 +1523,17 @@
         <v>2</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H20" s="25"/>
       <c r="I20" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
use first day of next month when job[end_year]='CURRENT_DATE'
</commit_message>
<xml_diff>
--- a/static_content/jobs/jobs.xlsx
+++ b/static_content/jobs/jobs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbecker11/workspace-parallax/flock-of-postcards/static_content/jobs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA857FE2-748A-BB42-A888-8FDC84289780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D6A0FD-33A2-2143-ACCB-51085389D7CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-56200" yWindow="280" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-60000" yWindow="-14480" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="jobs" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="99">
   <si>
     <t>role</t>
   </si>
@@ -357,20 +357,36 @@
 • Documented existing data architecture as [ERDs](https://www.lucidchart.com/pages/er-diagrams) using [DBeaver Enterprise](https://dbeaver.com/dbeaver-enterprise/). </t>
   </si>
   <si>
-    <t>• As a senior data engineer for [Angel Studios](https://www.angel.com/home), a streaming media service that offers family-friendly entertainment that amplifies light, with titles including The Chosen, Dry Bar Comedy, and Tuttle Twins.
+    <t>Fannie Mae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Senior Data / Machine Learning Engineer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Introductory phase in new role as senior data / machine learning engineer in the Risk &amp; Corporate Systems team at Fannie Mae GSE 
+</t>
+  </si>
+  <si>
+    <t>#006900</t>
+  </si>
+  <si>
+    <t>• Senior data engineer for [Angel Studios](https://www.angel.com/home), a streaming media service that offers family-friendly entertainment that amplifies light, with titles including The Chosen, Dry Bar Comedy, and Tuttle Twins.
 • Used [Python], [GitHub], [Pandas], [Numpy], [Keras], [Bash], [Linux], [PostgreSQL], and [Jupyter](https://jupyter.org/) to build and tune hyperparameters of a [convolutional neural network](https://towardsdatascience.com/a-comprehensive-guide-to-convolutional-neural-networks-the-eli5-way-3bd2b1164a53) with [supervised learning] on [Amazon Sagemaker](https://aws.amazon.com/pm/sagemaker/) to classify movie frames from episodic programs stored in [Amazon S3](https://aws.amazon.com/s3/storage-classes). 
 • Built web client apps using [Python] with [Postman](https://www.postman.com/) that made [REST] requests to pull monthly usage data from various web marketing partners like [FaceBook Marketing](https://www.quora.com/What-is-Facebook-Marketing-1), [Google Play](https://play.google/howplayworks/) , and [Vimeo](https://vimeo.com/). 
 • Worked with [Segment customer data platform](https://segment.com/customer-data-platform/), [Excel], and [Tableau] to create scheduled reports for the company's sales and finance teams.</t>
   </si>
   <si>
-    <t>• As a senior data engineer in the analytics team of [Warner Brothers](https://warnerbrosgames.com/) Division, I implemented high-volume pipeline integrations shuffling game telemetry and [user PII data] between WB-distributed consumer games and [marketing service platforms] via [Segment customer data platform](https://segment.com/customer-data-platform/) using [Kafka](https://aws.amazon.com/msk/), [Redshift](https://aws.amazon.com/redshift/), and [Apache Airflow](https://airflow.apache.org). 
-• Employed [Python], [GitHub], [Bash], [Linux], [Amazon Glue](https://aws.amazon.com/glue/) and [Apache Airflow](https://airflow.apache.org/) for external 3rd-party integrations and internal dev-ops integrations with [Jenkins], [PostgreSQL], [DataDog](https://www.datadoghq.com/), and [ZenDesk](https://zendesk.com) 
-• Integrated with [Google BigQuery data warehouse](https://cloud.google.com/bigquery using  [Apache Airflow](https://aws.amazon.com/managed-workflows-for-apache-airflow/), [Amazon S3], and [Redshift](https://aws.amazon.com/redshift/).</t>
-  </si>
-  <si>
-    <t>• As a senior data engineer in the data cyber security team of the [Cigna Group](https://www.thecignagroup.com/) created a [REST](url) using [Postman](https://www.postman.com/), [Bash], [Linux], and [OpenAPI](https://openapi-generator.tech/) for pulling credentials from the [CyberArk identity security platform](https://www.cyberark.com/) using [mutual TLS SSL authentication](https://docs.solace.com/Security/Two-Way-SSL-Authentication.htm) with [API Gateway](https://docs.aws.amazon.com/apigateway/). 
-•  Migrated a suite of legacy data pipeline [Python] elements running on the [Unity IoC platform](http://unitycontainer.org/articles/introduction.html) with [PostgreSQL] to pull credentials from the CyberArk service at runtime rather than using [Fernet](https://cryptography.io/en/latest/fernet/) encrypted local files. 
-•  Upgraded [GitHub] apps to use [Jenkins](https://docs.aws.amazon.com/apigateway/) CI/CD pipeline for build, applying sofware and cyber-secutity code checks, and on-prem server installation.</t>
+    <t>• As a senior data engineer in the data cyber security team of the [Cigna Group](https://www.thecignagroup.com/) created a [REST API] using [Postman], [Bash], [Linux], and [OpenAPI] for pulling credentials from [CyberArk](https://www.cyberark.com/) using [OpenSSL] with [mutual TLS SSL authentication](https://docs.solace.com/Security/Two-Way-SSL-Authentication.htm) via [API Gateway]. 
+•  Migrated a suite of legacy [ETL][data pipeline] [Python] elements running on the [Unity IoC platform] with [PostgreSQL] and [S3] to pull credentials from the [CyberArk] identity service at runtime rather than using [Fernet](https://cryptography.io/en/latest/fernet/) encrypted local files. 
+•  Upgraded [GitHub] apps to use [Jenkins](https://docs.aws.amazon.com/apigateway/) [CI/CD pipeline] for build, applying software and cyber-security code checks, and on-prem server installation.</t>
+  </si>
+  <si>
+    <t>• As a senior data engineer in the analytics team of [Warner Brothers](https://warnerbrosgames.com/) Division, implemented high-volume [ETL] [data pipeline] [integrations] transforming and sharing  game telemetry and [user PII data] between WB-distributed consumer games and [marketing service platforms] via [Segment customer data platform](https://segment.com/customer-data-platform/) using [Kafka](https://aws.amazon.com/msk/), [Amazon S3], [Redshift](https://aws.amazon.com/redshift/), and [Apache Airflow](https://airflow.apache.org). 
+• Employed [Python], [GitHub], [Bash], [Linux], [Amazon Glue](https://aws.amazon.com/glue/) and [Apache Airflow](https://airflow.apache.org/) for external [3rd-party integrations] and internal dev-ops integrations with [Jenkins], [PostgreSQL], [DataDog](https://www.datadoghq.com/),  [ZenDesk](https://zendesk.com). and [Tableau].
+• Integrated with [Google BigQuery](https://cloud.google.com/bigquery using  [Apache Airflow](https://aws.amazon.com/managed-workflows-for-apache-airflow/), [Amazon S3], and [Redshift](https://aws.amazon.com/redshift/).</t>
+  </si>
+  <si>
+    <t>CURRENT_DATE</t>
   </si>
 </sst>
 </file>
@@ -402,7 +418,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -482,6 +498,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF228B22"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF006900"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -519,7 +541,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -607,6 +629,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -614,6 +639,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF006900"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -913,10 +943,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="400" zoomScaleNormal="201" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -963,29 +993,29 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="160" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>23</v>
+        <v>92</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C2" s="7">
-        <v>45047</v>
-      </c>
-      <c r="D2" s="7">
-        <v>45277</v>
+        <v>45339</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>98</v>
       </c>
       <c r="E2" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="9"/>
+        <v>94</v>
+      </c>
+      <c r="H2" s="30"/>
       <c r="I2" s="6" t="s">
         <v>63</v>
       </c>
@@ -993,543 +1023,573 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="176" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="144" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>76</v>
+        <v>10</v>
       </c>
       <c r="C3" s="7">
-        <v>44805</v>
+        <v>45047</v>
       </c>
       <c r="D3" s="7">
-        <v>45047</v>
+        <v>45277</v>
       </c>
       <c r="E3" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="H3" s="9"/>
       <c r="I3" s="6" t="s">
         <v>63</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="192" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="176" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>15</v>
+        <v>76</v>
       </c>
       <c r="C4" s="7">
-        <v>44501</v>
+        <v>44805</v>
       </c>
       <c r="D4" s="7">
-        <v>44805</v>
+        <v>45047</v>
       </c>
       <c r="E4" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="H4" s="11"/>
       <c r="I4" s="6" t="s">
         <v>63</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="192" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>77</v>
+        <v>15</v>
       </c>
       <c r="C5" s="7">
-        <v>44136</v>
+        <v>44501</v>
       </c>
       <c r="D5" s="7">
-        <v>44501</v>
+        <v>44805</v>
       </c>
       <c r="E5" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="13"/>
+        <v>17</v>
+      </c>
+      <c r="H5" s="12"/>
       <c r="I5" s="6" t="s">
         <v>63</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>68</v>
+        <v>23</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>20</v>
+        <v>77</v>
       </c>
       <c r="C6" s="7">
-        <v>43770</v>
+        <v>44136</v>
       </c>
       <c r="D6" s="7">
-        <v>44136</v>
+        <v>44501</v>
       </c>
       <c r="E6" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" s="14"/>
+        <v>19</v>
+      </c>
+      <c r="H6" s="13"/>
       <c r="I6" s="6" t="s">
         <v>63</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="320" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>23</v>
+        <v>68</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>65</v>
+        <v>20</v>
       </c>
       <c r="C7" s="7">
-        <v>42795</v>
+        <v>43770</v>
       </c>
       <c r="D7" s="7">
-        <v>43770</v>
+        <v>44136</v>
       </c>
       <c r="E7" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" s="15"/>
+        <v>22</v>
+      </c>
+      <c r="H7" s="14"/>
       <c r="I7" s="6" t="s">
         <v>63</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="335" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>69</v>
+        <v>23</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="C8" s="7">
-        <v>42705</v>
+        <v>42795</v>
       </c>
       <c r="D8" s="7">
-        <v>42795</v>
+        <v>43770</v>
       </c>
       <c r="E8" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="H8" s="16"/>
+        <v>25</v>
+      </c>
+      <c r="H8" s="15"/>
       <c r="I8" s="6" t="s">
         <v>63</v>
       </c>
       <c r="J8" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="7">
+        <v>42705</v>
+      </c>
+      <c r="D9" s="7">
+        <v>42795</v>
+      </c>
+      <c r="E9" s="8">
+        <v>1</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" s="16"/>
+      <c r="I9" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="J9" s="10" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="335" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+    <row r="10" spans="1:10" ht="335" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B10" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C10" s="7">
         <v>40575</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D10" s="7">
         <v>42705</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E10" s="8">
         <v>2</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F10" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G10" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="17"/>
-      <c r="I9" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="J9" s="10" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="192" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="7">
-        <v>37561</v>
-      </c>
-      <c r="D10" s="7">
-        <v>40575</v>
-      </c>
-      <c r="E10" s="8">
-        <v>1</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H10" s="18"/>
+      <c r="H10" s="17"/>
       <c r="I10" s="6" t="s">
         <v>64</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="224" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="192" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C11" s="7">
-        <v>35827</v>
+        <v>37561</v>
       </c>
       <c r="D11" s="7">
-        <v>37561</v>
+        <v>40575</v>
       </c>
       <c r="E11" s="8">
         <v>1</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="H11" s="19"/>
+        <v>34</v>
+      </c>
+      <c r="H11" s="18"/>
       <c r="I11" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="144" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="224" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C12" s="7">
-        <v>35217</v>
+        <v>35827</v>
       </c>
       <c r="D12" s="7">
-        <v>35827</v>
+        <v>37561</v>
       </c>
       <c r="E12" s="8">
         <v>1</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="H12" s="9"/>
+        <v>37</v>
+      </c>
+      <c r="H12" s="19"/>
       <c r="I12" s="6" t="s">
         <v>63</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="335" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="144" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C13" s="7">
-        <v>33117</v>
+        <v>35217</v>
       </c>
       <c r="D13" s="7">
-        <v>35521</v>
+        <v>35827</v>
       </c>
       <c r="E13" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13" s="11"/>
+        <v>40</v>
+      </c>
+      <c r="H13" s="9"/>
       <c r="I13" s="6" t="s">
         <v>63</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="304" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="335" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C14" s="7">
-        <v>32021</v>
+        <v>33117</v>
       </c>
       <c r="D14" s="7">
-        <v>33117</v>
+        <v>35521</v>
       </c>
       <c r="E14" s="8">
         <v>2</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="H14" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="H14" s="11"/>
       <c r="I14" s="6" t="s">
         <v>63</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="304" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>72</v>
+        <v>43</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C15" s="7">
-        <v>32295</v>
+        <v>32021</v>
       </c>
       <c r="D15" s="7">
-        <v>32752</v>
+        <v>33117</v>
       </c>
       <c r="E15" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H15" s="13"/>
+        <v>45</v>
+      </c>
+      <c r="H15" s="12"/>
       <c r="I15" s="6" t="s">
         <v>63</v>
       </c>
       <c r="J15" s="10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="7">
+        <v>32295</v>
+      </c>
+      <c r="D16" s="7">
+        <v>32752</v>
+      </c>
+      <c r="E16" s="8">
+        <v>3</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" s="13"/>
+      <c r="I16" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="J16" s="10" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="112" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16" s="7">
-        <v>39417</v>
-      </c>
-      <c r="D16" s="7">
-        <v>40391</v>
-      </c>
-      <c r="E16" s="8">
-        <v>2</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="H16" s="20"/>
-      <c r="I16" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="J16" s="21" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="112" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C17" s="7">
-        <v>38749</v>
+        <v>39417</v>
       </c>
       <c r="D17" s="7">
-        <v>39417</v>
+        <v>40391</v>
       </c>
       <c r="E17" s="8">
         <v>2</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H17" s="22"/>
+        <v>50</v>
+      </c>
+      <c r="H17" s="20"/>
       <c r="I17" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="J17" s="10" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+      <c r="J17" s="21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="128" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C18" s="7">
-        <v>38384</v>
+        <v>38749</v>
       </c>
       <c r="D18" s="7">
-        <v>38749</v>
+        <v>39417</v>
       </c>
       <c r="E18" s="8">
         <v>2</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="H18" s="23"/>
+        <v>53</v>
+      </c>
+      <c r="H18" s="22"/>
       <c r="I18" s="6" t="s">
         <v>64</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C19" s="7">
-        <v>38018</v>
+        <v>38384</v>
       </c>
       <c r="D19" s="7">
-        <v>38384</v>
+        <v>38749</v>
       </c>
       <c r="E19" s="8">
         <v>2</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="H19" s="24"/>
+        <v>56</v>
+      </c>
+      <c r="H19" s="23"/>
       <c r="I19" s="6" t="s">
         <v>64</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="144" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>47</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C20" s="7">
-        <v>37681</v>
+        <v>38018</v>
       </c>
       <c r="D20" s="7">
-        <v>38018</v>
+        <v>38384</v>
       </c>
       <c r="E20" s="8">
         <v>2</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="H20" s="25"/>
+        <v>59</v>
+      </c>
+      <c r="H20" s="24"/>
       <c r="I20" s="6" t="s">
         <v>64</v>
       </c>
       <c r="J20" s="10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="144" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="7">
+        <v>37681</v>
+      </c>
+      <c r="D21" s="7">
+        <v>38018</v>
+      </c>
+      <c r="E21" s="8">
+        <v>2</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="H21" s="25"/>
+      <c r="I21" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="J21" s="10" t="s">
         <v>84</v>
       </c>
     </row>

</xml_diff>

<commit_message>
color updates / listAllCardDivs
</commit_message>
<xml_diff>
--- a/static_content/jobs/jobs.xlsx
+++ b/static_content/jobs/jobs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbecker11/workspace-parallax/flock-of-postcards/static_content/jobs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3380000E-DAA0-F848-B135-6D1C8C5AA972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D33AB650-C9A8-D444-BDB6-EC3DC7D7BD81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33600" yWindow="-12880" windowWidth="33600" windowHeight="15140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-49320" yWindow="-10680" windowWidth="33600" windowHeight="15140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="jobs" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="98">
   <si>
     <t>role</t>
   </si>
@@ -58,15 +58,6 @@
     <t>darkcyan</t>
   </si>
   <si>
-    <t>#006688</t>
-  </si>
-  <si>
-    <t>blue</t>
-  </si>
-  <si>
-    <t>#0000ff</t>
-  </si>
-  <si>
     <t xml:space="preserve">Angel Studios </t>
   </si>
   <si>
@@ -130,21 +121,9 @@
     <t xml:space="preserve">HomePorfolio LLC </t>
   </si>
   <si>
-    <t>teal</t>
-  </si>
-  <si>
-    <t>#008080</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lead Software Developer </t>
-  </si>
-  <si>
     <t xml:space="preserve">BuildingBlocks LLC </t>
   </si>
   <si>
-    <t>#008b8b</t>
-  </si>
-  <si>
     <t>Ph.D. Media Arts &amp; Science</t>
   </si>
   <si>
@@ -157,9 +136,6 @@
     <t>BYU</t>
   </si>
   <si>
-    <t>#0000cd</t>
-  </si>
-  <si>
     <t>Cimmetrix LLC</t>
   </si>
   <si>
@@ -170,9 +146,6 @@
   </si>
   <si>
     <t>yellow</t>
-  </si>
-  <si>
-    <t>#ffff00</t>
   </si>
   <si>
     <t>Eleven LLC</t>
@@ -251,12 +224,6 @@
     <t>Full Stack Developer</t>
   </si>
   <si>
-    <t xml:space="preserve">Technical Lead / Co-Founder </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lead Solutions Architect / Co-Founder </t>
-  </si>
-  <si>
     <t>• [Intrusic LLC](https://www.crunchbase.com/organization/intrusic) built real-time network monitoring systems that identified external and internal network intrusion attempts
 • As a Sierra Vista Group architech, I helped design and develop an approach for buffering live streaming network traffic for asynchronous package processing. 
 • Used [Linux](https://www.debian.org/), [C programming language](https://www.cprogramming.com/books/ritchie.html), and [Visio](https://www.microsoft.com/en-us/microsoft-365/visio/flowchart-software).</t>
@@ -270,15 +237,6 @@
   <si>
     <t>• As a senior full stack developer for [NuSkin](https://www.nuskin.com/us/en/, an international company known for its excellent  skin and beauty products I created new [Vue.js](https://vuejs.org/), [Nuxt](https://nuxt.com/), and [Vuetify](https://vuetifyjs.com/en/) components using [Bash], [Linux], [GitHub], [NodeJS], [HTML] and [CSS].  
 • Internationalized content using [Adobe Experience Cloud](https://business.adobe.com/).</t>
-  </si>
-  <si>
-    <t>• Co-founded [ClipFile]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/clipfile-infrastructure-150x150.png}, a company that envisioned building a web destination where users could easily record and share their favorite pieces of content like facts, authored stories, quotes, articles, chapters, or personal thoughts, as a way of concretely defining their personal [mindset]{https://sourcesofinsight.com/wp-content/uploads/2014/04/Mindset-768x505.jpg}(https://sourcesofinsight.com/what-is-mindset/).
-• Implemented [fuzzy matching](https://nanonets.com/blog/fuzzy-matching-fuzzy-logic/), [word clustering](https://www.ilc.cnr.it/EAGLES96/rep2/node37.html#:~:text=Word%20clustering%20is%20a%20technique,to%20information%20retrieval%20and%20filtering.), [semantic similarity scores](https://towardsdatascience.com/semantic-similarity-using-transformers-8f3cb5bf66d6), and [collaborative filtering](https://www.hindawi.com/journals/aai/2009/421425/) to help users find content that matched or differed from thieir own mindset.
-• Launched a novel [SaaS] using [Amazon Web Services] that let individuals and content creators search and share mindsets.
-• Conceptualized patented technology by designing and implementing a fuil-stack consumer-facing content management system that supported tuned matching among selected attributes.
-• [Java], [J2EE], [JSP], [Servlets], [Spring], [Amazon services], [JavaScript], [JQuery], [HTML], [CSS], [JUnit], [JMeter], [JProfile].
-• Utilized [REST], [Swagger], [Apache Shiro](https://shiro.apache.org/), [Eclipse IDE](https://www.eclipse.org/home/whatis/), [Apache Maven](https://maven.apache.org/what-is-maven.html), [Apache Ant](https://ant.apache.org/), [GitHub], [Hibernate], [Amazon SimpleDB](https://aws.amazon.com/simpledb/), [Linux](https://www.centos.org/), [Apache Tomcat](https://tomcat.apache.org/), [Bash], [Linux], [Jetty](https://projects.eclipse.org/projects/rt.jetty), and [Spring MVC](https://docs.spring.io/spring-framework/reference/web/webmvc.html).
-• Served as co-founder and co-authored [four patents](https://www.freepatentsonline.com/y2013/0325870.html).</t>
   </si>
   <si>
     <t>• As lead software developer, built a CD-ROM-based home design application for selecting premium home design products for previewing in the context of images of any household rooms. 
@@ -347,33 +305,15 @@
     <t>Fannie Mae</t>
   </si>
   <si>
-    <t>#006900</t>
-  </si>
-  <si>
     <t>CURRENT_DATE</t>
   </si>
   <si>
     <t>darkgreen</t>
-  </si>
-  <si>
-    <t>• Senior data engineer for [Angel Studios](https://www.angel.com/home), a streaming media service that offers family-friendly entertainment that amplifies light, with titles including The Chosen, Dry Bar Comedy, and Tuttle Twins.
-• Used [Python], [GitHub], [Pandas], [Numpy], [Keras], [Bash], [Linux], [PostgreSQL], and [Jupyter](https://jupyter.org/) to build and tune hyperparameters of a [convolutional neural network](https://towardsdatascience.com/a-comprehensive-guide-to-convolutional-neural-networks-the-eli5-way-3bd2b1164a53) with [supervised learning] on [Amazon Sagemaker](https://aws.amazon.com/pm/sagemaker/) to classify movie frames from episodic programs stored in [Amazon S3](https://aws.amazon.com/s3/storage-classes). 
-• Built web client apps using [Python] with [Postman](https://www.postman.com/) that made [REST] requests to pull monthly usage data from various web marketing partners like [FaceBook Marketing](https://www.quora.com/What-is-Facebook-Marketing-1), [Google Play](https://play.google/howplayworks/) , and [Vimeo](https://vimeo.com/). 
-• Worked with [ETL data pipeline] using the [Segment customer data platform](https://segment.com/customer-data-platform/), [Excel], and [Tableau] to create scheduled [business intelligence] reports for the company's sales and finance teams.</t>
   </si>
   <si>
     <t>• As a senior data engineer in the analytics team of [Warner Brothers](https://warnerbrosgames.com/) Division, implemented high-volume [ETL data pipeline] [integrations] transforming and sharing  game telemetry and [user PII data] between WB-distributed consumer games and [marketing service platforms] via [Segment customer data platform](https://segment.com/customer-data-platform/) using [Kafka](https://aws.amazon.com/msk/), [Amazon S3], [Amazon Redshift](https://aws.amazon.com/redshift/), and [Apache Airflow](https://airflow.apache.org). 
 • Employed [Python], [GitHub], [Bash], [Linux], [Amazon Glue](https://aws.amazon.com/glue/) and [Apache Airflow](https://airflow.apache.org/) for external [3rd-party integrations] and internal dev-ops integrations with [Jenkins], [PostgreSQL], [DataDog](https://www.datadoghq.com/),  [ZenDesk](https://zendesk.com). and [Tableau].
 • Integrated with [Google BigQuery](https://cloud.google.com/bigquery using  [Apache Airflow](https://aws.amazon.com/managed-workflows-for-apache-airflow/), [Amazon S3], and [Amazon Redshift](https://aws.amazon.com/redshift/) for [business intelligence] reporting.</t>
-  </si>
-  <si>
-    <t>• As a senior data engineer in the data cyber security team of the [Cigna Group](https://www.thecignagroup.com/) created a [REST API] using [Postman], [Bash], [Linux], and [OpenAPI] for pulling credentials from [CyberArk](https://www.cyberark.com/) using [OpenSSL] with [mutual TLS SSL authentication](https://docs.solace.com/Security/Two-Way-SSL-Authentication.htm) via [API Gateway]. 
-•  Migrated a suite of legacy [ETL data pipeline] [Python] elements running on the [Unity IoC platform] with [PostgreSQL] and [Amazon S3] to pull credentials from the [CyberArk] identity service at runtime rather than using [Fernet](https://cryptography.io/en/latest/fernet/) encrypted local files. 
-•  Upgraded [GitHub] apps to use [Jenkins](https://docs.aws.amazon.com/apigateway/) [CI/CD pipeline] for build, applying software and cyber-security code checks, and on-prem server installation.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• Senior data modeling engineer in the Risk &amp; Corporate Systems team at [datalake], and [business intelligence] reporting used for their mortgage financing services. Extensive use of [Amazon Redshift], [Amazon S3], [API Gateway], [Amazon Lambda], and [Amazon Glue].
-</t>
   </si>
   <si>
     <t>• As a senior software engineer for Data Laboratory, an internet company that provides daily lead reports for independent real-estage agents world-wide, I  [datalake].</t>
@@ -383,6 +323,63 @@
 • Used streaming event messages queued in [RabbitMQ](https://docs.aws.amazon.com/amazon-mq/latest/developer-guide/working-with-rabbitmq.html) and [Amazon Kinesis] to build [type-2 slowly changing dimensions] and accumulative facts tables. 
 • Designed and implemented a custom [star-schema warehouse](https://www.databricks.com/glossary/star-schema) and [ETL] processes to [de-normalize](https://en.wikipedia.org/wiki/Denormalization) and load data into [Amazon Redshift](https://aws.amazon.com/redshift/) data warehouse for scheduled [business intelligence] reports for the company's sales and finance team using [Tableau](https://www.tableau.com/).
 • [Test-driven development](https://www.pluralsight.com/blog/software-development/tdd-vs-bdd) using [Bash], [Linux], [Python], [PyCharm], [PyTest], [Unit-test], [GitHub], [Jira], and [Jenkins](https://www.jenkins.io/).</t>
+  </si>
+  <si>
+    <t>• Senior data engineer for [Angel Studios](https://www.angel.com/home), a streaming media service that offers family-friendly entertainment that amplifies light, with titles including The Chosen, Dry Bar Comedy, and Tuttle Twins.
+• Used [Python], [GitHub], [Pandas], [Numpy], [Keras], [Bash], [Linux], [PostgreSQL], and [Jupyter](https://jupyter.org/) to build and tune hyperparameters of a [convolutional neural network](https://towardsdatascience.com/a-comprehensive-guide-to-convolutional-neural-networks-the-eli5-way-3bd2b1164a53) with [supervised learning] on [Amazon Sagemaker](https://aws.amazon.com/pm/sagemaker/) to classify movie frames from episodic programs stored in [Amazon S3](https://aws.amazon.com/s3/storage-classes). 
+• Built web client apps using [Python] with [Postman](https://www.postman.com/) that made [REST API] requests to pull monthly usage data from various web marketing partners like [FaceBook Marketing](https://www.quora.com/What-is-Facebook-Marketing-1), [Google Play](https://play.google/howplayworks/) , and [Vimeo](https://vimeo.com/). 
+• Worked with [ETL data pipeline] using the [Segment customer data platform](https://segment.com/customer-data-platform/), [Excel], and [Tableau] to create scheduled [business intelligence] reports for the company's sales and finance teams.</t>
+  </si>
+  <si>
+    <t>• Co-founded [ClipFile]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/clipfile-infrastructure-150x150.png}, a company that envisioned building a web destination where users could easily record and share their favorite pieces of content like facts, authored stories, quotes, articles, chapters, or personal thoughts, as a way of concretely defining their personal [mindset]{https://sourcesofinsight.com/wp-content/uploads/2014/04/Mindset-768x505.jpg}(https://sourcesofinsight.com/what-is-mindset/).
+• Implemented [fuzzy matching](https://nanonets.com/blog/fuzzy-matching-fuzzy-logic/), [word clustering](https://www.ilc.cnr.it/EAGLES96/rep2/node37.html#:~:text=Word%20clustering%20is%20a%20technique,to%20information%20retrieval%20and%20filtering.), [semantic similarity scores](https://towardsdatascience.com/semantic-similarity-using-transformers-8f3cb5bf66d6), and [collaborative filtering](https://www.hindawi.com/journals/aai/2009/421425/) to help users find content that matched or differed from thieir own mindset.
+• Launched a novel [SaaS] using [Amazon Web Services] that let individuals and content creators search and share mindsets.
+• Conceptualized patented technology by designing and implementing a fuil-stack consumer-facing content management system that supported tuned matching among selected attributes.
+• [Java], [J2EE], [JSP], [Servlets], [Spring], [Amazon services], [JavaScript], [JQuery], [HTML], [CSS], [JUnit], [JMeter], [JProfile].
+• Utilized [REST API], [Swagger], [Apache Shiro](https://shiro.apache.org/), [Eclipse IDE](https://www.eclipse.org/home/whatis/), [Apache Maven](https://maven.apache.org/what-is-maven.html), [Apache Ant](https://ant.apache.org/), [GitHub], [Hibernate], [Amazon SimpleDB](https://aws.amazon.com/simpledb/), [Linux](https://www.centos.org/), [Apache Tomcat](https://tomcat.apache.org/), [Bash], [Linux], [Jetty](https://projects.eclipse.org/projects/rt.jetty), and [Spring MVC](https://docs.spring.io/spring-framework/reference/web/webmvc.html).
+• Served as co-founder and co-authored [four patents](https://www.freepatentsonline.com/y2013/0325870.html).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Senior data modeling engineer in the Risk &amp; Corporate Systems team at [datalake], and [business intelligence] reporting used for their mortgage financing services. Extensive use of [Amazon Redshift], [Amazon S3], [Amazon API Gateway], [Amazon Lambda], and [Amazon Glue].
+</t>
+  </si>
+  <si>
+    <t>• As a senior data engineer in the data cyber security team of the [Cigna Group](https://www.thecignagroup.com/) created a [REST API] using [Postman], [Bash], [Linux], and [OpenAPI] for pulling credentials from [CyberArk](https://www.cyberark.com/) using [OpenSSL] with [mutual TLS SSL authentication](https://docs.solace.com/Security/Two-Way-SSL-Authentication.htm) via [Amazon API Gateway]. 
+•  Migrated a suite of legacy [ETL data pipeline] [Python] elements running on the [Unity IoC platform] with [PostgreSQL] and [Amazon S3] to pull credentials from the [CyberArk] identity service at runtime rather than using [Fernet](https://cryptography.io/en/latest/fernet/) encrypted local files. 
+•  Upgraded [GitHub] apps to use [Jenkins](https://docs.aws.amazon.com/apigateway/) [CI/CD pipeline] for build, applying software and cyber-security code checks, and on-prem server installation.</t>
+  </si>
+  <si>
+    <t>#004500</t>
+  </si>
+  <si>
+    <t>#dddd44</t>
+  </si>
+  <si>
+    <t>#004466</t>
+  </si>
+  <si>
+    <t>Product Manager / Technical Lead / Co-Founder</t>
+  </si>
+  <si>
+    <t>#600080</t>
+  </si>
+  <si>
+    <t>#004040</t>
+  </si>
+  <si>
+    <t>darkteal</t>
+  </si>
+  <si>
+    <t>#4400bb</t>
+  </si>
+  <si>
+    <t>darkblue</t>
+  </si>
+  <si>
+    <t>#0000cc</t>
+  </si>
+  <si>
+    <t>#204480</t>
   </si>
 </sst>
 </file>
@@ -414,7 +411,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -468,11 +465,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF008080"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
@@ -499,6 +491,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF006900"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4E0090"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF004643"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF43008E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF204480"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -537,7 +553,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -596,12 +612,12 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -609,9 +625,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -626,7 +639,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -637,6 +662,12 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF204480"/>
+      <color rgb="FF43008E"/>
+      <color rgb="FF7900D1"/>
+      <color rgb="FF004643"/>
+      <color rgb="FF4E0090"/>
+      <color rgb="FF80008B"/>
       <color rgb="FF006900"/>
     </mruColors>
   </colors>
@@ -941,19 +972,19 @@
   </sheetPr>
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.1640625" style="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" style="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13" style="27" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="28" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="10.83203125" style="26" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="96" style="29" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.5" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" style="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" style="26" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="27" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="10.83203125" style="25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="96" style="28" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -991,37 +1022,37 @@
     </row>
     <row r="2" spans="1:10" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="C2" s="7">
         <v>45339</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="E2" s="8">
         <v>1</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="H2" s="30"/>
+        <v>87</v>
+      </c>
+      <c r="H2" s="29"/>
       <c r="I2" s="6" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="144" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>10</v>
@@ -1039,22 +1070,22 @@
         <v>11</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>12</v>
+        <v>89</v>
       </c>
       <c r="H3" s="9"/>
       <c r="I3" s="6" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="176" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="C4" s="7">
         <v>44805</v>
@@ -1066,25 +1097,25 @@
         <v>2</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="11"/>
+        <v>91</v>
+      </c>
+      <c r="H4" s="30"/>
       <c r="I4" s="6" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="208" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C5" s="7">
         <v>44501</v>
@@ -1096,25 +1127,25 @@
         <v>1</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H5" s="12"/>
       <c r="I5" s="6" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="112" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="C6" s="7">
         <v>44136</v>
@@ -1126,25 +1157,25 @@
         <v>2</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H6" s="13"/>
       <c r="I6" s="6" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C7" s="7">
         <v>43770</v>
@@ -1156,25 +1187,25 @@
         <v>1</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H7" s="14"/>
       <c r="I7" s="6" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="318" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C8" s="7">
         <v>42795</v>
@@ -1186,25 +1217,25 @@
         <v>2</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H8" s="15"/>
       <c r="I8" s="6" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C9" s="7">
         <v>42705</v>
@@ -1216,25 +1247,25 @@
         <v>1</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H9" s="16"/>
       <c r="I9" s="6" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="335" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="350" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C10" s="7">
         <v>40575</v>
@@ -1246,25 +1277,25 @@
         <v>2</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H10" s="17"/>
       <c r="I10" s="6" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="192" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C11" s="7">
         <v>37561</v>
@@ -1276,25 +1307,25 @@
         <v>1</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H11" s="18"/>
       <c r="I11" s="6" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="224" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="240" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C12" s="7">
         <v>35827</v>
@@ -1306,25 +1337,25 @@
         <v>1</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="H12" s="19"/>
+        <v>92</v>
+      </c>
+      <c r="H12" s="31"/>
       <c r="I12" s="6" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="144" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="160" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>38</v>
+        <v>90</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C13" s="7">
         <v>35217</v>
@@ -1339,22 +1370,22 @@
         <v>11</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="H13" s="9"/>
+        <v>97</v>
+      </c>
+      <c r="H13" s="33"/>
       <c r="I13" s="6" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="335" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C14" s="7">
         <v>33117</v>
@@ -1366,25 +1397,25 @@
         <v>2</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>13</v>
+        <v>95</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="H14" s="11"/>
       <c r="I14" s="6" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="304" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C15" s="7">
         <v>32021</v>
@@ -1396,25 +1427,25 @@
         <v>2</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="H15" s="12"/>
+        <v>94</v>
+      </c>
+      <c r="H15" s="32"/>
       <c r="I15" s="6" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C16" s="7">
         <v>32295</v>
@@ -1426,25 +1457,25 @@
         <v>3</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H16" s="13"/>
       <c r="I16" s="6" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="112" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C17" s="7">
         <v>39417</v>
@@ -1456,25 +1487,25 @@
         <v>2</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="H17" s="20"/>
+        <v>88</v>
+      </c>
+      <c r="H17" s="19"/>
       <c r="I17" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="J17" s="21" t="s">
-        <v>66</v>
+        <v>55</v>
+      </c>
+      <c r="J17" s="20" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="128" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C18" s="7">
         <v>38749</v>
@@ -1486,25 +1517,25 @@
         <v>2</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H18" s="22"/>
+        <v>44</v>
+      </c>
+      <c r="H18" s="21"/>
       <c r="I18" s="6" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="112" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C19" s="7">
         <v>38384</v>
@@ -1516,25 +1547,25 @@
         <v>2</v>
       </c>
       <c r="F19" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H19" s="22"/>
+      <c r="I19" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="G19" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="H19" s="23"/>
-      <c r="I19" s="6" t="s">
+      <c r="J19" s="10" t="s">
         <v>64</v>
-      </c>
-      <c r="J19" s="10" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C20" s="7">
         <v>38018</v>
@@ -1546,25 +1577,25 @@
         <v>2</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="H20" s="24"/>
+        <v>50</v>
+      </c>
+      <c r="H20" s="23"/>
       <c r="I20" s="6" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="144" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C21" s="7">
         <v>37681</v>
@@ -1576,17 +1607,17 @@
         <v>2</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="H21" s="25"/>
+        <v>53</v>
+      </c>
+      <c r="H21" s="24"/>
       <c r="I21" s="6" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
README.md and jobs.xlsx updated
</commit_message>
<xml_diff>
--- a/static_content/jobs/jobs.xlsx
+++ b/static_content/jobs/jobs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10714"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbecker11/workspace-parallax/flock-of-postcards/static_content/jobs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2BD25A6-60FF-CC46-82B1-4AC487B9A01A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D082B8F-191F-4240-ADF3-12A7E2F5D950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-49320" yWindow="-10680" windowWidth="33600" windowHeight="15140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-31880" yWindow="3200" windowWidth="20480" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="jobs" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="97">
   <si>
     <t>role</t>
   </si>
@@ -298,9 +298,6 @@
   </si>
   <si>
     <t>Fannie Mae</t>
-  </si>
-  <si>
-    <t>CURRENT_DATE</t>
   </si>
   <si>
     <t>darkgreen</t>
@@ -972,8 +969,8 @@
   </sheetPr>
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1030,24 +1027,24 @@
       <c r="C2" s="7">
         <v>45339</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>77</v>
+      <c r="D2" s="7">
+        <v>45473</v>
       </c>
       <c r="E2" s="8">
         <v>1</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H2" s="29"/>
       <c r="I2" s="6" t="s">
         <v>54</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="160" x14ac:dyDescent="0.2">
@@ -1070,14 +1067,14 @@
         <v>11</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H3" s="9"/>
       <c r="I3" s="6" t="s">
         <v>54</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="176" x14ac:dyDescent="0.2">
@@ -1100,14 +1097,14 @@
         <v>18</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H4" s="30"/>
       <c r="I4" s="6" t="s">
         <v>54</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="208" x14ac:dyDescent="0.2">
@@ -1137,7 +1134,7 @@
         <v>54</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="32" x14ac:dyDescent="0.2">
@@ -1167,7 +1164,7 @@
         <v>54</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="64" x14ac:dyDescent="0.2">
@@ -1227,7 +1224,7 @@
         <v>54</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="80" x14ac:dyDescent="0.2">
@@ -1257,12 +1254,12 @@
         <v>54</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="350" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>26</v>
@@ -1287,12 +1284,12 @@
         <v>55</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="192" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>29</v>
@@ -1322,7 +1319,7 @@
     </row>
     <row r="12" spans="1:10" ht="240" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>32</v>
@@ -1337,10 +1334,10 @@
         <v>1</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H12" s="31"/>
       <c r="I12" s="6" t="s">
@@ -1352,7 +1349,7 @@
     </row>
     <row r="13" spans="1:10" ht="160" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>33</v>
@@ -1370,7 +1367,7 @@
         <v>11</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H13" s="33"/>
       <c r="I13" s="6" t="s">
@@ -1397,10 +1394,10 @@
         <v>2</v>
       </c>
       <c r="F14" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="G14" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>94</v>
       </c>
       <c r="H14" s="11"/>
       <c r="I14" s="6" t="s">
@@ -1430,7 +1427,7 @@
         <v>18</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H15" s="32"/>
       <c r="I15" s="6" t="s">
@@ -1490,7 +1487,7 @@
         <v>41</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H17" s="19"/>
       <c r="I17" s="6" t="s">

</xml_diff>

<commit_message>
Added Spexture from 2024-08 to present
</commit_message>
<xml_diff>
--- a/static_content/jobs/jobs.xlsx
+++ b/static_content/jobs/jobs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbecker11/workspace-parallax/flock-of-postcards/static_content/jobs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbecker11/workspace-flock/flock-of-postcards/static_content/jobs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D6A0FD-33A2-2143-ACCB-51085389D7CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855809F4-6252-ED4C-850E-0C52CABDF2BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60000" yWindow="-14480" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-33240" yWindow="2200" windowWidth="26580" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="jobs" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="101">
   <si>
     <t>role</t>
   </si>
@@ -360,13 +360,6 @@
     <t>Fannie Mae</t>
   </si>
   <si>
-    <t xml:space="preserve">Senior Data / Machine Learning Engineer </t>
-  </si>
-  <si>
-    <t xml:space="preserve">• Introductory phase in new role as senior data / machine learning engineer in the Risk &amp; Corporate Systems team at Fannie Mae GSE 
-</t>
-  </si>
-  <si>
     <t>#006900</t>
   </si>
   <si>
@@ -376,17 +369,40 @@
 • Worked with [Segment customer data platform](https://segment.com/customer-data-platform/), [Excel], and [Tableau] to create scheduled reports for the company's sales and finance teams.</t>
   </si>
   <si>
-    <t>• As a senior data engineer in the data cyber security team of the [Cigna Group](https://www.thecignagroup.com/) created a [REST API] using [Postman], [Bash], [Linux], and [OpenAPI] for pulling credentials from [CyberArk](https://www.cyberark.com/) using [OpenSSL] with [mutual TLS SSL authentication](https://docs.solace.com/Security/Two-Way-SSL-Authentication.htm) via [API Gateway]. 
-•  Migrated a suite of legacy [ETL][data pipeline] [Python] elements running on the [Unity IoC platform] with [PostgreSQL] and [S3] to pull credentials from the [CyberArk] identity service at runtime rather than using [Fernet](https://cryptography.io/en/latest/fernet/) encrypted local files. 
-•  Upgraded [GitHub] apps to use [Jenkins](https://docs.aws.amazon.com/apigateway/) [CI/CD pipeline] for build, applying software and cyber-security code checks, and on-prem server installation.</t>
-  </si>
-  <si>
     <t>• As a senior data engineer in the analytics team of [Warner Brothers](https://warnerbrosgames.com/) Division, implemented high-volume [ETL] [data pipeline] [integrations] transforming and sharing  game telemetry and [user PII data] between WB-distributed consumer games and [marketing service platforms] via [Segment customer data platform](https://segment.com/customer-data-platform/) using [Kafka](https://aws.amazon.com/msk/), [Amazon S3], [Redshift](https://aws.amazon.com/redshift/), and [Apache Airflow](https://airflow.apache.org). 
 • Employed [Python], [GitHub], [Bash], [Linux], [Amazon Glue](https://aws.amazon.com/glue/) and [Apache Airflow](https://airflow.apache.org/) for external [3rd-party integrations] and internal dev-ops integrations with [Jenkins], [PostgreSQL], [DataDog](https://www.datadoghq.com/),  [ZenDesk](https://zendesk.com). and [Tableau].
 • Integrated with [Google BigQuery](https://cloud.google.com/bigquery using  [Apache Airflow](https://aws.amazon.com/managed-workflows-for-apache-airflow/), [Amazon S3], and [Redshift](https://aws.amazon.com/redshift/).</t>
   </si>
   <si>
     <t>CURRENT_DATE</t>
+  </si>
+  <si>
+    <t>Spexture</t>
+  </si>
+  <si>
+    <t>#4EA200</t>
+  </si>
+  <si>
+    <t>•	Implementing end-to-end [MLOps] [CI/CD] pipeline with target-based design
+•	Hashicorp [Terraform] and [Vault] for multi-environment infrastructure and credentials
+•	[GitHub Actions] for CI/CD and [Argo CD] for change detection
+•	[Kubernetes] for orchestrating [Docker] containers running on an [EKS-managed cluster]
+•	[Amazon SageMaker] for ML model integration and real-time scoring
+•	[Amazon Managed Grafana] for real-time [data visualization]
+•	[dbt], PySpark] and [PySpark SQL] for [data quality validation], [data cleaning], and [feature engineering]
+•	[AWS Glue] for tracking data versioning/lineage, and enforcing [governance]</t>
+  </si>
+  <si>
+    <t>•	Extensive work with [SQL], [AWS Redshift]. [AWS Glue], [Airflow], S3, IAM, [Lambda], [REST], SNS, and [dbt\
+•	Created dbt-validated SQL code for data cleansing and [data lake ingestion] 
+•	Used [Amazon Glue] to track schema changes and revise [Redshift external views]
+•	Created custom views required for analysis and reporting in Redshift
+•	Documented processes to build, test, and deploy data pipeline components for in-house [ETL data pipeline]</t>
+  </si>
+  <si>
+    <t>• As a senior data engineer in the data [cyber security] team of the [Cigna Group](https://www.thecignagroup.com/) created a [REST API] using [Postman], [Bash], [Linux], and [OpenAPI] for pulling credentials from [CyberArk](https://www.cyberark.com/) using [OpenSSL] with [mutual TLS/SSL authentication](https://docs.solace.com/Security/Two-Way-SSL-Authentication.htm) via [API Gateway]. 
+•  Migrated a suite of legacy [ETL data pipeline] [Python] elements running on the [Unity IoC platform] with [PostgreSQL] and [S3] to pull credentials from the [CyberArk] identity service at runtime rather than using [Fernet](https://cryptography.io/en/latest/fernet/) encrypted local files. 
+•  Upgraded [GitHub] apps to use [Jenkins](https://docs.aws.amazon.com/apigateway/) [CI/CD pipeline] for build, applying software and cyber-security code checks, and [on-prem server installation]</t>
   </si>
 </sst>
 </file>
@@ -396,7 +412,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -417,8 +433,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -503,6 +525,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF006900"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4EA300"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -541,7 +569,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -631,6 +659,24 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -641,6 +687,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF4EA300"/>
       <color rgb="FF006900"/>
     </mruColors>
   </colors>
@@ -943,10 +990,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -993,603 +1040,633 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="48" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="C2" s="7">
-        <v>45339</v>
+    <row r="2" spans="1:10" s="35" customFormat="1" ht="152" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="32">
+        <v>45520</v>
       </c>
       <c r="D2" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="E2" s="33">
+        <v>1</v>
+      </c>
+      <c r="F2" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="H2" s="36"/>
+      <c r="I2" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="J2" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="E2" s="8">
-        <v>1</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="H2" s="30"/>
-      <c r="I2" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="144" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C3" s="7">
-        <v>45047</v>
+        <v>45339</v>
       </c>
       <c r="D3" s="7">
-        <v>45277</v>
+        <v>45474</v>
       </c>
       <c r="E3" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>11</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="9"/>
+        <v>92</v>
+      </c>
+      <c r="H3" s="30"/>
       <c r="I3" s="6" t="s">
         <v>63</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="176" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="144" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>76</v>
+        <v>10</v>
       </c>
       <c r="C4" s="7">
-        <v>44805</v>
+        <v>45047</v>
       </c>
       <c r="D4" s="7">
-        <v>45047</v>
+        <v>45277</v>
       </c>
       <c r="E4" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="H4" s="9"/>
       <c r="I4" s="6" t="s">
         <v>63</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="192" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="176" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>15</v>
+        <v>76</v>
       </c>
       <c r="C5" s="7">
-        <v>44501</v>
+        <v>44805</v>
       </c>
       <c r="D5" s="7">
-        <v>44805</v>
+        <v>45047</v>
       </c>
       <c r="E5" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="H5" s="11"/>
       <c r="I5" s="6" t="s">
         <v>63</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="192" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>77</v>
+        <v>15</v>
       </c>
       <c r="C6" s="7">
-        <v>44136</v>
+        <v>44501</v>
       </c>
       <c r="D6" s="7">
-        <v>44501</v>
+        <v>44805</v>
       </c>
       <c r="E6" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="13"/>
+        <v>17</v>
+      </c>
+      <c r="H6" s="12"/>
       <c r="I6" s="6" t="s">
         <v>63</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>68</v>
+        <v>23</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>20</v>
+        <v>77</v>
       </c>
       <c r="C7" s="7">
-        <v>43770</v>
+        <v>44136</v>
       </c>
       <c r="D7" s="7">
-        <v>44136</v>
+        <v>44501</v>
       </c>
       <c r="E7" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="14"/>
+        <v>19</v>
+      </c>
+      <c r="H7" s="13"/>
       <c r="I7" s="6" t="s">
         <v>63</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="335" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>23</v>
+        <v>68</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>65</v>
+        <v>20</v>
       </c>
       <c r="C8" s="7">
-        <v>42795</v>
+        <v>43770</v>
       </c>
       <c r="D8" s="7">
-        <v>43770</v>
+        <v>44136</v>
       </c>
       <c r="E8" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H8" s="15"/>
+        <v>22</v>
+      </c>
+      <c r="H8" s="14"/>
       <c r="I8" s="6" t="s">
         <v>63</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="335" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>69</v>
+        <v>23</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="C9" s="7">
-        <v>42705</v>
+        <v>42795</v>
       </c>
       <c r="D9" s="7">
-        <v>42795</v>
+        <v>43770</v>
       </c>
       <c r="E9" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="H9" s="16"/>
+        <v>25</v>
+      </c>
+      <c r="H9" s="15"/>
       <c r="I9" s="6" t="s">
         <v>63</v>
       </c>
       <c r="J9" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="7">
+        <v>42705</v>
+      </c>
+      <c r="D10" s="7">
+        <v>42795</v>
+      </c>
+      <c r="E10" s="8">
+        <v>1</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" s="16"/>
+      <c r="I10" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="J10" s="10" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="335" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
+    <row r="11" spans="1:10" ht="335" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B11" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C11" s="7">
         <v>40575</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D11" s="7">
         <v>42705</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E11" s="8">
         <v>2</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F11" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G11" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="17"/>
-      <c r="I10" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="J10" s="10" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="192" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="7">
-        <v>37561</v>
-      </c>
-      <c r="D11" s="7">
-        <v>40575</v>
-      </c>
-      <c r="E11" s="8">
-        <v>1</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H11" s="18"/>
+      <c r="H11" s="17"/>
       <c r="I11" s="6" t="s">
         <v>64</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="224" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="192" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C12" s="7">
-        <v>35827</v>
+        <v>37561</v>
       </c>
       <c r="D12" s="7">
-        <v>37561</v>
+        <v>40575</v>
       </c>
       <c r="E12" s="8">
         <v>1</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="H12" s="19"/>
+        <v>34</v>
+      </c>
+      <c r="H12" s="18"/>
       <c r="I12" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="144" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="224" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C13" s="7">
-        <v>35217</v>
+        <v>35827</v>
       </c>
       <c r="D13" s="7">
-        <v>35827</v>
+        <v>37561</v>
       </c>
       <c r="E13" s="8">
         <v>1</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="H13" s="9"/>
+        <v>37</v>
+      </c>
+      <c r="H13" s="19"/>
       <c r="I13" s="6" t="s">
         <v>63</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="335" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="144" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C14" s="7">
-        <v>33117</v>
+        <v>35217</v>
       </c>
       <c r="D14" s="7">
-        <v>35521</v>
+        <v>35827</v>
       </c>
       <c r="E14" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H14" s="11"/>
+        <v>40</v>
+      </c>
+      <c r="H14" s="9"/>
       <c r="I14" s="6" t="s">
         <v>63</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="304" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="335" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C15" s="7">
-        <v>32021</v>
+        <v>33117</v>
       </c>
       <c r="D15" s="7">
-        <v>33117</v>
+        <v>35521</v>
       </c>
       <c r="E15" s="8">
         <v>2</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="H15" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="H15" s="11"/>
       <c r="I15" s="6" t="s">
         <v>63</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="304" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>72</v>
+        <v>43</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C16" s="7">
-        <v>32295</v>
+        <v>32021</v>
       </c>
       <c r="D16" s="7">
-        <v>32752</v>
+        <v>33117</v>
       </c>
       <c r="E16" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H16" s="13"/>
+        <v>45</v>
+      </c>
+      <c r="H16" s="12"/>
       <c r="I16" s="6" t="s">
         <v>63</v>
       </c>
       <c r="J16" s="10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="7">
+        <v>32295</v>
+      </c>
+      <c r="D17" s="7">
+        <v>32752</v>
+      </c>
+      <c r="E17" s="8">
+        <v>3</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" s="13"/>
+      <c r="I17" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="J17" s="10" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="112" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
+    <row r="18" spans="1:10" ht="112" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B18" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C18" s="7">
         <v>39417</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D18" s="7">
         <v>40391</v>
-      </c>
-      <c r="E17" s="8">
-        <v>2</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="H17" s="20"/>
-      <c r="I17" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="J17" s="21" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="128" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" s="7">
-        <v>38749</v>
-      </c>
-      <c r="D18" s="7">
-        <v>39417</v>
       </c>
       <c r="E18" s="8">
         <v>2</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H18" s="22"/>
+        <v>50</v>
+      </c>
+      <c r="H18" s="20"/>
       <c r="I18" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="J18" s="10" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+      <c r="J18" s="21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="128" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C19" s="7">
-        <v>38384</v>
+        <v>38749</v>
       </c>
       <c r="D19" s="7">
-        <v>38749</v>
+        <v>39417</v>
       </c>
       <c r="E19" s="8">
         <v>2</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="H19" s="23"/>
+        <v>53</v>
+      </c>
+      <c r="H19" s="22"/>
       <c r="I19" s="6" t="s">
         <v>64</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C20" s="7">
-        <v>38018</v>
+        <v>38384</v>
       </c>
       <c r="D20" s="7">
-        <v>38384</v>
+        <v>38749</v>
       </c>
       <c r="E20" s="8">
         <v>2</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="H20" s="24"/>
+        <v>56</v>
+      </c>
+      <c r="H20" s="23"/>
       <c r="I20" s="6" t="s">
         <v>64</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="144" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>47</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C21" s="7">
-        <v>37681</v>
+        <v>38018</v>
       </c>
       <c r="D21" s="7">
-        <v>38018</v>
+        <v>38384</v>
       </c>
       <c r="E21" s="8">
         <v>2</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="H21" s="25"/>
+        <v>59</v>
+      </c>
+      <c r="H21" s="24"/>
       <c r="I21" s="6" t="s">
         <v>64</v>
       </c>
       <c r="J21" s="10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="144" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="7">
+        <v>37681</v>
+      </c>
+      <c r="D22" s="7">
+        <v>38018</v>
+      </c>
+      <c r="E22" s="8">
+        <v>2</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="H22" s="25"/>
+      <c r="I22" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="J22" s="10" t="s">
         <v>84</v>
       </c>
     </row>

</xml_diff>

<commit_message>
spexture added into jobs
</commit_message>
<xml_diff>
--- a/static_content/jobs/jobs.xlsx
+++ b/static_content/jobs/jobs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11207"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbecker11/workspace-parallax/flock-of-postcards/static_content/jobs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbecker11/workspace-flock/flock-of-postcards/static_content/jobs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D6A0FD-33A2-2143-ACCB-51085389D7CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A9B96C-B4F2-F04E-BFD7-89205D8D468E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60000" yWindow="-14480" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37460" yWindow="2180" windowWidth="25740" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="jobs" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="102">
   <si>
     <t>role</t>
   </si>
@@ -272,7 +272,94 @@
 • Internationalized content using [Adobe Experience Cloud](https://business.adobe.com/).</t>
   </si>
   <si>
-    <t>• As a senior data engineer for SeniorLink's [Vela project]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/Vela-150x126.png} a homeservices support platform, helped create [ETL](https://aws.amazon.com/what-is/etl/) processes using [Amazon Kinesis](https://aws.amazon.com/pm/kinesis/), [Python], [PySpark](https://spark.apache.org/), and [Amazon Data Pipeline](https://docs.aws.amazon.com/datapipeline/latest/DeveloperGuide/what-is-datapipeline.html) to load structured event data from [PostgreSQL] databases into [Redshift](https://aws.amazon.com/pm/redshift/). 
+    <t>• As lead software developer, built a CD-ROM-based home design application for selecting premium home design products for previewing in the context of images of any household rooms. 
+• Built the prototype using Adobe Photoshop and [Macromedia Director](https://macromedia.fandom.com/wiki/Macromedia_Director).
+• Built the actual application using using [Bash], [Linux], [Java] and [Marimba Bongo](https://www.thriftbooks.com/w/official-marimba-guide-to-bongo_danny-goodman/2574616/#edition=58026223&amp;idiq=42367912) widget layout tool.
+• Updates for the self-updating application were delivered over the internet using [Marimba Castanet](https://www.infoworld.com/article/2076707/marimba-launches-new-castanet-with-a-less-java-centric-focus.html) push-technology.</t>
+  </si>
+  <si>
+    <t>•  AMI (https://amientertainment.com/) was the internet-music distribution incarnation of Rowe International.  
+•  As a Sierra Vista Group project manager and technical lead, I helped design and implement their system for making monthly ACH royalty payments to music copyright owners for mechanical and performance licensing rights.
+•  Used [FileMaker Pro](https://www.claris.com/filemaker/), [Bash], [Linux], [HTML], [CSS], [JavaScript], [Java], and [Visio](https://www.microsoft.com/en-us/microsoft-365/visio/flowchart-software).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">•  [Rowe International](https://pitchbook.com/profiles/company/13178-08) was the leading manufacturer of music jukeboxes. 
+•  Sierra Vista Group was consulted to assess their available technologies and create a plan to build their back-end systems to let them become a leading provider of internet-based music.
+•  As project manager and technical lead created the project plan and led the development of a full-stack web application used by  jukebox owners and Rowe sales and marketing.
+•  Used [Java], [Bash], [Linux], [HTML], [CSS], [JavaScript], [ObjectDesign](https://object.design/), [MySQL](https://www.mysql.com/), and [Adobe Photoshop](https://www.adobe.com/products/photoshop.html). 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• [Eleven LLC](https://www.eleven.net/) built mobile apps used by beverage industry distributors to help manage placement  of their products in the shelves and coolers in retail locations. The work done by the Sierra Vista Group was instrumental in their company being acquired by [Trimble](https://help.trimblegeospatial.com/TMM/Home.htm). 
+• As the architect and team lead, we used [Java], [Bash], [GitHub], [Linux], and  [JBoss](https://developers.redhat.com/products/eap/overview) message-oriented middleware platform, [Sybase Anywhere](https://texas.gs.shi.com/Product/30451452/Sybase-SQL-Anywhere-Advanced-Edition) for the client/server based database, and [Windows Mobile](https://en.wikipedia.org/wiki/Windows_Mobile_5.0) running on ruggedized mobile devices. </t>
+  </si>
+  <si>
+    <t>• As co-founder and CTO, designed and led the development of a public website used by discerning home designers and builders called [HomePortfolio](https://HomePortfolio/). 
+• Hired a staff of  10 software and databases developers. 
+• Worked with data acquisition team to scan and tag over 700,000 premium home design products from over 2,000 manufactures and vendors.
+• Designed datamodel and data entry tools for category-specific product attribution. 
+• Helped extended the business model to provide online product selection tools for participating vendors and manufacturers.
+• Instrumental in raising over $70M in venture capital. 
+• Used [Oracle], [ATG Dyanamo]( https://docs.oracle.com/cd/E24152_01/Platform.10-1/ATGPersBusinessGuide/html/s0102dynamoapplicationframework01.html), [Java], [Akamai]{https://www.hiclipart.com/free-transparent-background-png-clipart-zkmsn}(https://www.akamai.com/), [WebTrends](https://www.webtrends.com/), [FileMakerPro], [ImageMagik](https://imagemagick.org/index.php), [Bash], [Linux], [HTML], [JavaScript], [CSS], and [Omnigraffle](https://www.omnigroup.com/omnigraffle) for data modeling and workflow designs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• As a senior software engineer for Data Laboratory, an internet company that provides daily lead reports for independent real-estage agents world-wide, I  [containerized] legacy web applications using [Bash], [Linux], [GitHub], [Docker](https://www.docker.com/) and [Amazon Secrets Manager](https://aws.amazon.com/secrets-manager/). 
+• Updated legacy web apps using [Bash], [Linux], [HTML], [CSS], [JavaScript], [PostgreSQL], [NGINX], and [OpenSSL].
+• Documented existing data architecture as [ERDs](https://www.lucidchart.com/pages/er-diagrams) using [DBeaver Enterprise](https://dbeaver.com/dbeaver-enterprise/). </t>
+  </si>
+  <si>
+    <t>Fannie Mae</t>
+  </si>
+  <si>
+    <t>#006900</t>
+  </si>
+  <si>
+    <t>• Senior data engineer for [Angel Studios](https://www.angel.com/home), a streaming media service that offers family-friendly entertainment that amplifies light, with titles including The Chosen, Dry Bar Comedy, and Tuttle Twins.
+• Used [Python], [GitHub], [Pandas], [Numpy], [Keras], [Bash], [Linux], [PostgreSQL], and [Jupyter](https://jupyter.org/) to build and tune hyperparameters of a [convolutional neural network](https://towardsdatascience.com/a-comprehensive-guide-to-convolutional-neural-networks-the-eli5-way-3bd2b1164a53) with [supervised learning] on [Amazon Sagemaker](https://aws.amazon.com/pm/sagemaker/) to classify movie frames from episodic programs stored in [Amazon S3](https://aws.amazon.com/s3/storage-classes). 
+• Built web client apps using [Python] with [Postman](https://www.postman.com/) that made [REST] requests to pull monthly usage data from various web marketing partners like [FaceBook Marketing](https://www.quora.com/What-is-Facebook-Marketing-1), [Google Play](https://play.google/howplayworks/) , and [Vimeo](https://vimeo.com/). 
+• Worked with [Segment customer data platform](https://segment.com/customer-data-platform/), [Excel], and [Tableau] to create scheduled reports for the company's sales and finance teams.</t>
+  </si>
+  <si>
+    <t>• As a senior data engineer in the data cyber security team of the [Cigna Group](https://www.thecignagroup.com/) created a [REST API] using [Postman], [Bash], [Linux], and [OpenAPI] for pulling credentials from [CyberArk](https://www.cyberark.com/) using [OpenSSL] with [mutual TLS SSL authentication](https://docs.solace.com/Security/Two-Way-SSL-Authentication.htm) via [API Gateway]. 
+•  Migrated a suite of legacy [ETL][data pipeline] [Python] elements running on the [Unity IoC platform] with [PostgreSQL] and [S3] to pull credentials from the [CyberArk] identity service at runtime rather than using [Fernet](https://cryptography.io/en/latest/fernet/) encrypted local files. 
+•  Upgraded [GitHub] apps to use [Jenkins](https://docs.aws.amazon.com/apigateway/) [CI/CD pipeline] for build, applying software and cyber-security code checks, and on-prem server installation.</t>
+  </si>
+  <si>
+    <t>• As a senior data engineer in the analytics team of [Warner Brothers](https://warnerbrosgames.com/) Division, implemented high-volume [ETL] [data pipeline] [integrations] transforming and sharing  game telemetry and [user PII data] between WB-distributed consumer games and [marketing service platforms] via [Segment customer data platform](https://segment.com/customer-data-platform/) using [Kafka](https://aws.amazon.com/msk/), [Amazon S3], [Redshift](https://aws.amazon.com/redshift/), and [Apache Airflow](https://airflow.apache.org). 
+• Employed [Python], [GitHub], [Bash], [Linux], [Amazon Glue](https://aws.amazon.com/glue/) and [Apache Airflow](https://airflow.apache.org/) for external [3rd-party integrations] and internal dev-ops integrations with [Jenkins], [PostgreSQL], [DataDog](https://www.datadoghq.com/),  [ZenDesk](https://zendesk.com). and [Tableau].
+• Integrated with [Google BigQuery](https://cloud.google.com/bigquery using  [Apache Airflow](https://aws.amazon.com/managed-workflows-for-apache-airflow/), [Amazon S3], and [Redshift](https://aws.amazon.com/redshift/).</t>
+  </si>
+  <si>
+    <t>CURRENT_DATE</t>
+  </si>
+  <si>
+    <t>Spexture</t>
+  </si>
+  <si>
+    <t>#608E52</t>
+  </si>
+  <si>
+    <t>darkspring</t>
+  </si>
+  <si>
+    <t>• Extensive work with SQL, AWS Redshift, Glue, Airflow, S3, IAM, Lambda, REST, SNS, and dbt
+• Created dbt-validated SQL code for data cleansing and data lake ingestion 
+• Used Amazon Glue to track schema changes and revise Redshift external views
+• Created custom views required for analysis and reporting in Redshift
+• Documented processes to build, test, and deploy data pipeline components for in-house ETL framework</t>
+  </si>
+  <si>
+    <t>• Implementing end-to-end MLOps CI/CD pipeline with target-based design
+• Hashicorp Terraform and Vault for multi-environment infrastructure and credentials
+• GitHub Actions for CI/CD and Argo CD for change detection
+• Kubernetes for orchestrating PySparkSQL Docker containers running on an EKS-managed cluster.
+• Amazon SageMaker for ML model integration, real-time scoring, and model versioning
+• Amazon Managed Grafana for real-time visualization
+• PySpark and PySpark SQL for data quality validation, data cleaning, and feature engineering 
+• AWS Glue for metadata tagging, tracking versioning/lineage, and enforcing governance</t>
+  </si>
+  <si>
+    <t>• As a senior data engineer for SeniorLink's [Vela project]{/static_content/portfolio/Vela-150x126.png} a homeservices support platform, helped create [ETL](https://aws.amazon.com/what-is/etl/) processes using [Amazon Kinesis](https://aws.amazon.com/pm/kinesis/), [Python], [PySpark](https://spark.apache.org/), and [Amazon Data Pipeline](https://docs.aws.amazon.com/datapipeline/latest/DeveloperGuide/what-is-datapipeline.html) to load structured event data from [PostgreSQL] databases into [Redshift](https://aws.amazon.com/pm/redshift/). 
 • Saved data to [Amazon S3] using [Amazon Kinesis] and triggered [Amazon Lambda](https://docs.aws.amazon.com/lambda/) jobs to aggregate steaming event data into [schema-on-read] file formats, [Apache Avro](https://avro.apache.org/) and [Apache Parquet](https://parquet.apache.org/).
 • Steered efforts in creating a [Data Lake](https://aws.amazon.com/big-data/datalakes-and-analytics/datalakes/) using [PostgreSQL] and [FlyWay](https://flywaydb.org/) with [Python] and [PySpark](https://spark.apache.org/docs/latest/api/python/index.html) pre-processing on [EC2 instances] using shared [Amazon EFS](https://zesty.co/blog/ebs-vs-efs-which-is-right) for staged storage.
 • Used streaming event messages queued in [RabbitMQ](https://docs.aws.amazon.com/amazon-mq/latest/developer-guide/working-with-rabbitmq.html) and [Amazon Kinesis] to build [type-2 slowly changing dimensions] and accumulative facts tables. 
@@ -280,7 +367,12 @@
 • [Test-driven development](https://www.pluralsight.com/blog/software-development/tdd-vs-bdd) using [Bash], [Linux], [Python], [PyCharm], [PyTest], [Unit-test], [GitHub], [Jira], and [Jenkins](https://www.jenkins.io/).</t>
   </si>
   <si>
-    <t>• Co-founded [ClipFile]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/clipfile-infrastructure-150x150.png}, a company that envisioned building a web destination where users could easily record and share their favorite pieces of content like facts, authored stories, quotes, articles, chapters, or personal thoughts, as a way of concretely defining their personal [mindset]{https://sourcesofinsight.com/wp-content/uploads/2014/04/Mindset-768x505.jpg}(https://sourcesofinsight.com/what-is-mindset/).
+    <t>• As a senior software engineer at [BigR.io]{/static_content/portfolio/Bigr.io_-150x106.png} I used [Amazon microservices] for custom voice-based [natural language processing] applications.
+• Used [Apache ActiveMQ](https://activemq.apache.org/), [Swagger](https://swagger.io/), [JSON], [Jackson](url), [AOP](https://www.baeldung.com/spring-aop), [Eclipse], [Maven], [GitHub], [Jira], [PostgreSQL], and [Jenkins].
+• [Java], [J2EE], [Servlets], [Spring], [SpringBoot], [JAX-RS], [Bash], [Linux], [JUnit], [JMeter], and [JProfile]</t>
+  </si>
+  <si>
+    <t>• Co-founded [ClipFile]{/static_content/portfolio/clipfile-infrastructure-150x150.png}, a company that envisioned building a web destination where users could easily record and share their favorite pieces of content like facts, authored stories, quotes, articles, chapters, or personal thoughts, as a way of concretely defining their personal [mindset]{https://sourcesofinsight.com/wp-content/uploads/2014/04/Mindset-768x505.jpg}(https://sourcesofinsight.com/what-is-mindset/).
 • Implemented [fuzzy matching](https://nanonets.com/blog/fuzzy-matching-fuzzy-logic/), [word clustering](https://www.ilc.cnr.it/EAGLES96/rep2/node37.html#:~:text=Word%20clustering%20is%20a%20technique,to%20information%20retrieval%20and%20filtering.), [semantic similarity scores](https://towardsdatascience.com/semantic-similarity-using-transformers-8f3cb5bf66d6), and [collaborative filtering](https://www.hindawi.com/journals/aai/2009/421425/) to help users find content that matched or differed from thieir own mindset.
 • Launched a novel [SaaS] using [Amazon Web Services] that let individuals and content creators search and share mindsets.
 • Conceptualized patented technology by designing and implementing a fuil-stack consumer-facing content management system that supported tuned matching among selected attributes.
@@ -289,29 +381,7 @@
 • Served as co-founder and co-authored [four patents](https://www.freepatentsonline.com/y2013/0325870.html).</t>
   </si>
   <si>
-    <t>• As lead software developer, built a CD-ROM-based home design application for selecting premium home design products for previewing in the context of images of any household rooms. 
-• Built the prototype using Adobe Photoshop and [Macromedia Director](https://macromedia.fandom.com/wiki/Macromedia_Director).
-• Built the actual application using using [Bash], [Linux], [Java] and [Marimba Bongo](https://www.thriftbooks.com/w/official-marimba-guide-to-bongo_danny-goodman/2574616/#edition=58026223&amp;idiq=42367912) widget layout tool.
-• Updates for the self-updating application were delivered over the internet using [Marimba Castanet](https://www.infoworld.com/article/2076707/marimba-launches-new-castanet-with-a-less-java-centric-focus.html) push-technology.</t>
-  </si>
-  <si>
-    <t>• Front-end software developer of a reverse kinametics path planning system for multi-axis industrial robots for [Cimmetrix]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/Cimetrix-PDF-combined-logo-150x100.png}.
-• Technologies used include [Bash], [Linux], [C programming language], [Bash](https://en.wikipedia.org/wiki/Bourne_shell), [X11] , [Xt toolkit intrinsics](https://en.wikipedia.org/wiki/X_Toolkit_Intrinsics), [Silicon Graphics Irix](https://en.wikipedia.org/wiki/Silicon_Graphics), and [HP-UX](https://en.wikipedia.org/wiki/HP-UX).</t>
-  </si>
-  <si>
-    <t>•  AMI (https://amientertainment.com/) was the internet-music distribution incarnation of Rowe International.  
-•  As a Sierra Vista Group project manager and technical lead, I helped design and implement their system for making monthly ACH royalty payments to music copyright owners for mechanical and performance licensing rights.
-•  Used [FileMaker Pro](https://www.claris.com/filemaker/), [Bash], [Linux], [HTML], [CSS], [JavaScript], [Java], and [Visio](https://www.microsoft.com/en-us/microsoft-365/visio/flowchart-software).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">•  [Rowe International](https://pitchbook.com/profiles/company/13178-08) was the leading manufacturer of music jukeboxes. 
-•  Sierra Vista Group was consulted to assess their available technologies and create a plan to build their back-end systems to let them become a leading provider of internet-based music.
-•  As project manager and technical lead created the project plan and led the development of a full-stack web application used by  jukebox owners and Rowe sales and marketing.
-•  Used [Java], [Bash], [Linux], [HTML], [CSS], [JavaScript], [ObjectDesign](https://object.design/), [MySQL](https://www.mysql.com/), and [Adobe Photoshop](https://www.adobe.com/products/photoshop.html). 
-</t>
-  </si>
-  <si>
-    <t>•	Doctor of Philosopy degree, [MIT]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/MIT-logo.png}, Cambridge, Massachusettes
+    <t>•	Doctor of Philosopy degree, [MIT]{/static_content/portfolio/MIT-logo.png}, Cambridge, Massachusettes
 •	Media Laboratory, Media Arts and Sciences
 •	Took courses in machine vision, signals and systems, digital signal processing, and stochastics.
 •	Helped build the operating system for the [Cheops multi-processor system](http://alumni.media.mit.edu/~wad/cheops_CSVT/cheops.html) used for digital video research and for holographic video
@@ -324,69 +394,18 @@
 • [C programming language], [TclTk], [X11], [HTML], [JavaScript],[CSS],[XMotif], [Bash], [Linux]</t>
   </si>
   <si>
-    <t xml:space="preserve">• [Eleven LLC](https://www.eleven.net/) built mobile apps used by beverage industry distributors to help manage placement  of their products in the shelves and coolers in retail locations. The work done by the Sierra Vista Group was instrumental in their company being acquired by [Trimble](https://help.trimblegeospatial.com/TMM/Home.htm). 
-• As the architect and team lead, we used [Java], [Bash], [GitHub], [Linux], and  [JBoss](https://developers.redhat.com/products/eap/overview) message-oriented middleware platform, [Sybase Anywhere](https://texas.gs.shi.com/Product/30451452/Sybase-SQL-Anywhere-Advanced-Edition) for the client/server based database, and [Windows Mobile](https://en.wikipedia.org/wiki/Windows_Mobile_5.0) running on ruggedized mobile devices. </t>
-  </si>
-  <si>
-    <t>• As co-founder and CTO, designed and led the development of a public website used by discerning home designers and builders called [HomePortfolio](https://HomePortfolio/). 
-• Hired a staff of  10 software and databases developers. 
-• Worked with data acquisition team to scan and tag over 700,000 premium home design products from over 2,000 manufactures and vendors.
-• Designed datamodel and data entry tools for category-specific product attribution. 
-• Helped extended the business model to provide online product selection tools for participating vendors and manufacturers.
-• Instrumental in raising over $70M in venture capital. 
-• Used [Oracle], [ATG Dyanamo]( https://docs.oracle.com/cd/E24152_01/Platform.10-1/ATGPersBusinessGuide/html/s0102dynamoapplicationframework01.html), [Java], [Akamai]{https://www.hiclipart.com/free-transparent-background-png-clipart-zkmsn}(https://www.akamai.com/), [WebTrends](https://www.webtrends.com/), [FileMakerPro], [ImageMagik](https://imagemagick.org/index.php), [Bash], [Linux], [HTML], [JavaScript], [CSS], and [Omnigraffle](https://www.omnigroup.com/omnigraffle) for data modeling and workflow designs.</t>
-  </si>
-  <si>
-    <t>• Masters of Science degree, [BYU]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/BYU-entrance-150x150.jpg}, Provo, Utah
+    <t>• Masters of Science degree, [BYU]{/static_content/portfolio/BYU-entrance-150x150.jpg}, Provo, Utah
 Took all courses required for both bachelors and masters degrees in Computer Science
 • Thesis project [“Interactive Measurement of Three-Dimensional Objects Using a Depth Buffer &amp; Linear Probe.”](https://dl.acm.org/doi/pdf/10.1145/108360.108446) CS MS Thesis, Shawn Becker, William A. Barrett &amp; Dan R. Olsen, ACM Transactions on Graphics, Vol. 10, No. 2, April 1991
 • Top Research Presentation – New Tech Research Conference - BYU – Provo, UT – March 1990
 • [“Fast Automated Object Detection Using Signature Parsing.”](https://www.spiedigitallibrary.org/conference-proceedings-of-spie/1192/1/Fast-Automated-Object-Detection-Using-Signature-Parsing/10.1117/12.969720.short) Tim Heaton; Shawn Becker; Kelley Anderson; William Barrett: Proceedings Volume 1192, Intelligent Robots &amp; Computer Vision VIII: Algorithms &amp; Techniques; (1990) https://doi.org/10.1117/12.969720
 • [“Probabilistic Segmentation of Myocardial Tissue by Deterministic Relaxation.”](https://scholarsarchive.byu.edu/cgi/viewcontent.cgi?article=1737&amp;context=facpub) Jerome A. Broekhuijsen, Shawn C. Becker, &amp; William A. Barrett: IEEE Proceedings of Computers in Cardiology, pp. 99-12, Jerusalem, September 1989.
-• [“Interactive Measurement of three-Dimensional Cardiac Morphology.”]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/BYU-MS-CS-Skull-Cross-Section-1.jpeg}(https://scholarsarchive.byu.edu/cgi/viewcontent.cgi?article=1736&amp;context=facpub) Shawn C Becker, William A Barrett, October 1989, DOI: 10.1109/CIC.1989.130586, Conference: Computers in Cardiology.
+• [“Interactive Measurement of three-Dimensional Cardiac Morphology.”]{/static_content/portfolio/BYU-MS-CS-Skull-Cross-Section-1.jpeg}(https://scholarsarchive.byu.edu/cgi/viewcontent.cgi?article=1736&amp;context=facpub) Shawn C Becker, William A Barrett, October 1989, DOI: 10.1109/CIC.1989.130586, Conference: Computers in Cardiology.
 • [C programming language], [Bash], [Linux], [XMotif], and [X11].</t>
   </si>
   <si>
-    <t>• As a senior software engineer at [BigR.io]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/Bigr.io_-150x106.png} I used [Amazon microservices] for custom voice-based [natural language processing] applications.
-• Used [Apache ActiveMQ](https://activemq.apache.org/), [Swagger](https://swagger.io/), [JSON], [Jackson](url), [AOP](https://www.baeldung.com/spring-aop), [Eclipse], [Maven], [GitHub], [Jira], [PostgreSQL], and [Jenkins].
-• [Java], [J2EE], [Servlets], [Spring], [SpringBoot], [JAX-RS], [Bash], [Linux], [JUnit], [JMeter], and [JProfile]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• As a senior software engineer for Data Laboratory, an internet company that provides daily lead reports for independent real-estage agents world-wide, I  [containerized] legacy web applications using [Bash], [Linux], [GitHub], [Docker](https://www.docker.com/) and [Amazon Secrets Manager](https://aws.amazon.com/secrets-manager/). 
-• Updated legacy web apps using [Bash], [Linux], [HTML], [CSS], [JavaScript], [PostgreSQL], [NGINX], and [OpenSSL].
-• Documented existing data architecture as [ERDs](https://www.lucidchart.com/pages/er-diagrams) using [DBeaver Enterprise](https://dbeaver.com/dbeaver-enterprise/). </t>
-  </si>
-  <si>
-    <t>Fannie Mae</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Senior Data / Machine Learning Engineer </t>
-  </si>
-  <si>
-    <t xml:space="preserve">• Introductory phase in new role as senior data / machine learning engineer in the Risk &amp; Corporate Systems team at Fannie Mae GSE 
-</t>
-  </si>
-  <si>
-    <t>#006900</t>
-  </si>
-  <si>
-    <t>• Senior data engineer for [Angel Studios](https://www.angel.com/home), a streaming media service that offers family-friendly entertainment that amplifies light, with titles including The Chosen, Dry Bar Comedy, and Tuttle Twins.
-• Used [Python], [GitHub], [Pandas], [Numpy], [Keras], [Bash], [Linux], [PostgreSQL], and [Jupyter](https://jupyter.org/) to build and tune hyperparameters of a [convolutional neural network](https://towardsdatascience.com/a-comprehensive-guide-to-convolutional-neural-networks-the-eli5-way-3bd2b1164a53) with [supervised learning] on [Amazon Sagemaker](https://aws.amazon.com/pm/sagemaker/) to classify movie frames from episodic programs stored in [Amazon S3](https://aws.amazon.com/s3/storage-classes). 
-• Built web client apps using [Python] with [Postman](https://www.postman.com/) that made [REST] requests to pull monthly usage data from various web marketing partners like [FaceBook Marketing](https://www.quora.com/What-is-Facebook-Marketing-1), [Google Play](https://play.google/howplayworks/) , and [Vimeo](https://vimeo.com/). 
-• Worked with [Segment customer data platform](https://segment.com/customer-data-platform/), [Excel], and [Tableau] to create scheduled reports for the company's sales and finance teams.</t>
-  </si>
-  <si>
-    <t>• As a senior data engineer in the data cyber security team of the [Cigna Group](https://www.thecignagroup.com/) created a [REST API] using [Postman], [Bash], [Linux], and [OpenAPI] for pulling credentials from [CyberArk](https://www.cyberark.com/) using [OpenSSL] with [mutual TLS SSL authentication](https://docs.solace.com/Security/Two-Way-SSL-Authentication.htm) via [API Gateway]. 
-•  Migrated a suite of legacy [ETL][data pipeline] [Python] elements running on the [Unity IoC platform] with [PostgreSQL] and [S3] to pull credentials from the [CyberArk] identity service at runtime rather than using [Fernet](https://cryptography.io/en/latest/fernet/) encrypted local files. 
-•  Upgraded [GitHub] apps to use [Jenkins](https://docs.aws.amazon.com/apigateway/) [CI/CD pipeline] for build, applying software and cyber-security code checks, and on-prem server installation.</t>
-  </si>
-  <si>
-    <t>• As a senior data engineer in the analytics team of [Warner Brothers](https://warnerbrosgames.com/) Division, implemented high-volume [ETL] [data pipeline] [integrations] transforming and sharing  game telemetry and [user PII data] between WB-distributed consumer games and [marketing service platforms] via [Segment customer data platform](https://segment.com/customer-data-platform/) using [Kafka](https://aws.amazon.com/msk/), [Amazon S3], [Redshift](https://aws.amazon.com/redshift/), and [Apache Airflow](https://airflow.apache.org). 
-• Employed [Python], [GitHub], [Bash], [Linux], [Amazon Glue](https://aws.amazon.com/glue/) and [Apache Airflow](https://airflow.apache.org/) for external [3rd-party integrations] and internal dev-ops integrations with [Jenkins], [PostgreSQL], [DataDog](https://www.datadoghq.com/),  [ZenDesk](https://zendesk.com). and [Tableau].
-• Integrated with [Google BigQuery](https://cloud.google.com/bigquery using  [Apache Airflow](https://aws.amazon.com/managed-workflows-for-apache-airflow/), [Amazon S3], and [Redshift](https://aws.amazon.com/redshift/).</t>
-  </si>
-  <si>
-    <t>CURRENT_DATE</t>
+    <t>• Front-end software developer of a reverse kinametics path planning system for multi-axis industrial robots for [Cimmetrix]{/static_content/portfolio/Cimetrix-PDF-combined-logo-150x100.png}.
+• Technologies used include [Bash], [Linux], [C programming language], [Bash](https://en.wikipedia.org/wiki/Bourne_shell), [X11] , [Xt toolkit intrinsics](https://en.wikipedia.org/wiki/X_Toolkit_Intrinsics), [Silicon Graphics Irix](https://en.wikipedia.org/wiki/Silicon_Graphics), and [HP-UX](https://en.wikipedia.org/wiki/HP-UX).</t>
   </si>
 </sst>
 </file>
@@ -418,7 +437,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -503,6 +522,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF006900"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF729D65"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -541,7 +566,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -631,6 +656,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -641,6 +669,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF729D65"/>
       <color rgb="FF006900"/>
     </mruColors>
   </colors>
@@ -943,10 +972,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="E9" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -993,604 +1022,634 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="128" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>92</v>
+        <v>23</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>91</v>
       </c>
       <c r="C2" s="7">
-        <v>45339</v>
+        <v>45519</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="E2" s="8">
         <v>1</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>11</v>
+        <v>93</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="H2" s="30"/>
+        <v>92</v>
+      </c>
+      <c r="H2" s="31"/>
       <c r="I2" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="144" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>10</v>
+        <v>85</v>
       </c>
       <c r="C3" s="7">
-        <v>45047</v>
+        <v>45339</v>
       </c>
       <c r="D3" s="7">
-        <v>45277</v>
+        <v>45470</v>
       </c>
       <c r="E3" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>11</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="9"/>
+        <v>86</v>
+      </c>
+      <c r="H3" s="30"/>
       <c r="I3" s="6" t="s">
         <v>63</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="176" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="144" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>76</v>
+        <v>10</v>
       </c>
       <c r="C4" s="7">
-        <v>44805</v>
+        <v>45047</v>
       </c>
       <c r="D4" s="7">
-        <v>45047</v>
+        <v>45277</v>
       </c>
       <c r="E4" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="H4" s="9"/>
       <c r="I4" s="6" t="s">
         <v>63</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="192" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="176" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>15</v>
+        <v>76</v>
       </c>
       <c r="C5" s="7">
-        <v>44501</v>
+        <v>44805</v>
       </c>
       <c r="D5" s="7">
-        <v>44805</v>
+        <v>45047</v>
       </c>
       <c r="E5" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="H5" s="11"/>
       <c r="I5" s="6" t="s">
         <v>63</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="192" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>77</v>
+        <v>15</v>
       </c>
       <c r="C6" s="7">
-        <v>44136</v>
+        <v>44501</v>
       </c>
       <c r="D6" s="7">
-        <v>44501</v>
+        <v>44805</v>
       </c>
       <c r="E6" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="13"/>
+        <v>17</v>
+      </c>
+      <c r="H6" s="12"/>
       <c r="I6" s="6" t="s">
         <v>63</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>68</v>
+        <v>23</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>20</v>
+        <v>77</v>
       </c>
       <c r="C7" s="7">
-        <v>43770</v>
+        <v>44136</v>
       </c>
       <c r="D7" s="7">
-        <v>44136</v>
+        <v>44501</v>
       </c>
       <c r="E7" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="14"/>
+        <v>19</v>
+      </c>
+      <c r="H7" s="13"/>
       <c r="I7" s="6" t="s">
         <v>63</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="335" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>23</v>
+        <v>68</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>65</v>
+        <v>20</v>
       </c>
       <c r="C8" s="7">
-        <v>42795</v>
+        <v>43770</v>
       </c>
       <c r="D8" s="7">
-        <v>43770</v>
+        <v>44136</v>
       </c>
       <c r="E8" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H8" s="15"/>
+        <v>22</v>
+      </c>
+      <c r="H8" s="14"/>
       <c r="I8" s="6" t="s">
         <v>63</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="335" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>69</v>
+        <v>23</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="C9" s="7">
-        <v>42705</v>
+        <v>42795</v>
       </c>
       <c r="D9" s="7">
-        <v>42795</v>
+        <v>43770</v>
       </c>
       <c r="E9" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="H9" s="16"/>
+        <v>25</v>
+      </c>
+      <c r="H9" s="15"/>
       <c r="I9" s="6" t="s">
         <v>63</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="335" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="7">
+        <v>42705</v>
+      </c>
+      <c r="D10" s="7">
+        <v>42795</v>
+      </c>
+      <c r="E10" s="8">
+        <v>1</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" s="16"/>
+      <c r="I10" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="335" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B11" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C11" s="7">
         <v>40575</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D11" s="7">
         <v>42705</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E11" s="8">
         <v>2</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F11" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G11" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="17"/>
-      <c r="I10" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="J10" s="10" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="192" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="7">
-        <v>37561</v>
-      </c>
-      <c r="D11" s="7">
-        <v>40575</v>
-      </c>
-      <c r="E11" s="8">
-        <v>1</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H11" s="18"/>
+      <c r="H11" s="17"/>
       <c r="I11" s="6" t="s">
         <v>64</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="224" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="192" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C12" s="7">
-        <v>35827</v>
+        <v>37561</v>
       </c>
       <c r="D12" s="7">
-        <v>37561</v>
+        <v>40575</v>
       </c>
       <c r="E12" s="8">
         <v>1</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="H12" s="19"/>
+        <v>34</v>
+      </c>
+      <c r="H12" s="18"/>
       <c r="I12" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="144" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="224" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C13" s="7">
-        <v>35217</v>
+        <v>35827</v>
       </c>
       <c r="D13" s="7">
-        <v>35827</v>
+        <v>37561</v>
       </c>
       <c r="E13" s="8">
         <v>1</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="H13" s="9"/>
+        <v>37</v>
+      </c>
+      <c r="H13" s="19"/>
       <c r="I13" s="6" t="s">
         <v>63</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="335" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="144" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C14" s="7">
-        <v>33117</v>
+        <v>35217</v>
       </c>
       <c r="D14" s="7">
-        <v>35521</v>
+        <v>35827</v>
       </c>
       <c r="E14" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H14" s="11"/>
+        <v>40</v>
+      </c>
+      <c r="H14" s="9"/>
       <c r="I14" s="6" t="s">
         <v>63</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="304" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="335" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C15" s="7">
-        <v>32021</v>
+        <v>33117</v>
       </c>
       <c r="D15" s="7">
-        <v>33117</v>
+        <v>35521</v>
       </c>
       <c r="E15" s="8">
         <v>2</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="H15" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="H15" s="11"/>
       <c r="I15" s="6" t="s">
         <v>63</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="304" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>72</v>
+        <v>43</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C16" s="7">
-        <v>32295</v>
+        <v>32021</v>
       </c>
       <c r="D16" s="7">
-        <v>32752</v>
+        <v>33117</v>
       </c>
       <c r="E16" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H16" s="13"/>
+        <v>45</v>
+      </c>
+      <c r="H16" s="12"/>
       <c r="I16" s="6" t="s">
         <v>63</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="112" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="7">
+        <v>32295</v>
+      </c>
+      <c r="D17" s="7">
+        <v>32752</v>
+      </c>
+      <c r="E17" s="8">
+        <v>3</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" s="13"/>
+      <c r="I17" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="J17" s="10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="112" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B18" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C18" s="7">
         <v>39417</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D18" s="7">
         <v>40391</v>
-      </c>
-      <c r="E17" s="8">
-        <v>2</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="H17" s="20"/>
-      <c r="I17" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="J17" s="21" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="128" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" s="7">
-        <v>38749</v>
-      </c>
-      <c r="D18" s="7">
-        <v>39417</v>
       </c>
       <c r="E18" s="8">
         <v>2</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H18" s="22"/>
+        <v>50</v>
+      </c>
+      <c r="H18" s="20"/>
       <c r="I18" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="J18" s="10" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+      <c r="J18" s="21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="128" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C19" s="7">
-        <v>38384</v>
+        <v>38749</v>
       </c>
       <c r="D19" s="7">
-        <v>38749</v>
+        <v>39417</v>
       </c>
       <c r="E19" s="8">
         <v>2</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="H19" s="23"/>
+        <v>53</v>
+      </c>
+      <c r="H19" s="22"/>
       <c r="I19" s="6" t="s">
         <v>64</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C20" s="7">
-        <v>38018</v>
+        <v>38384</v>
       </c>
       <c r="D20" s="7">
-        <v>38384</v>
+        <v>38749</v>
       </c>
       <c r="E20" s="8">
         <v>2</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="H20" s="24"/>
+        <v>56</v>
+      </c>
+      <c r="H20" s="23"/>
       <c r="I20" s="6" t="s">
         <v>64</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="144" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>47</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C21" s="7">
-        <v>37681</v>
+        <v>38018</v>
       </c>
       <c r="D21" s="7">
-        <v>38018</v>
+        <v>38384</v>
       </c>
       <c r="E21" s="8">
         <v>2</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="H21" s="25"/>
+        <v>59</v>
+      </c>
+      <c r="H21" s="24"/>
       <c r="I21" s="6" t="s">
         <v>64</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>84</v>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="144" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="7">
+        <v>37681</v>
+      </c>
+      <c r="D22" s="7">
+        <v>38018</v>
+      </c>
+      <c r="E22" s="8">
+        <v>2</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="H22" s="25"/>
+      <c r="I22" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="J22" s="10" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tweaked Spexture job color
</commit_message>
<xml_diff>
--- a/static_content/jobs/jobs.xlsx
+++ b/static_content/jobs/jobs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbecker11/workspace-flock/flock-of-postcards/static_content/jobs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A9B96C-B4F2-F04E-BFD7-89205D8D468E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388EC38A-F42F-FF48-96C5-5A028AB29F51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-37460" yWindow="2180" windowWidth="25740" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -336,9 +336,6 @@
     <t>Spexture</t>
   </si>
   <si>
-    <t>#608E52</t>
-  </si>
-  <si>
     <t>darkspring</t>
   </si>
   <si>
@@ -406,6 +403,9 @@
   <si>
     <t>• Front-end software developer of a reverse kinametics path planning system for multi-axis industrial robots for [Cimmetrix]{/static_content/portfolio/Cimetrix-PDF-combined-logo-150x100.png}.
 • Technologies used include [Bash], [Linux], [C programming language], [Bash](https://en.wikipedia.org/wiki/Bourne_shell), [X11] , [Xt toolkit intrinsics](https://en.wikipedia.org/wiki/X_Toolkit_Intrinsics), [Silicon Graphics Irix](https://en.wikipedia.org/wiki/Silicon_Graphics), and [HP-UX](https://en.wikipedia.org/wiki/HP-UX).</t>
+  </si>
+  <si>
+    <t>#118811</t>
   </si>
 </sst>
 </file>
@@ -527,7 +527,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF729D65"/>
+        <fgColor rgb="FF118810"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -669,6 +669,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF118810"/>
       <color rgb="FF729D65"/>
       <color rgb="FF006900"/>
     </mruColors>
@@ -974,8 +975,8 @@
   </sheetPr>
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E9" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1039,17 +1040,17 @@
         <v>1</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="H2" s="31"/>
       <c r="I2" s="6" t="s">
         <v>64</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="80" x14ac:dyDescent="0.2">
@@ -1079,7 +1080,7 @@
         <v>63</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="144" x14ac:dyDescent="0.2">
@@ -1232,7 +1233,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="335" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="320" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>23</v>
       </c>
@@ -1259,7 +1260,7 @@
         <v>63</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="80" x14ac:dyDescent="0.2">
@@ -1289,7 +1290,7 @@
         <v>63</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="335" x14ac:dyDescent="0.2">
@@ -1319,7 +1320,7 @@
         <v>64</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="192" x14ac:dyDescent="0.2">
@@ -1412,7 +1413,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="335" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="320" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>41</v>
       </c>
@@ -1439,10 +1440,10 @@
         <v>63</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="304" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="272" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>43</v>
       </c>
@@ -1469,7 +1470,7 @@
         <v>63</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="80" x14ac:dyDescent="0.2">
@@ -1499,7 +1500,7 @@
         <v>63</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="112" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
replacing invalid webpage and image urls with valid ones where possible.
</commit_message>
<xml_diff>
--- a/static_content/jobs/jobs.xlsx
+++ b/static_content/jobs/jobs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11207"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbecker11/workspace-parallax/flock-of-postcards/static_content/jobs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbecker11/workspace-flock/flock-of-postcards/static_content/jobs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D6A0FD-33A2-2143-ACCB-51085389D7CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F54C0BBC-A1EF-404C-8AD3-1D9202504A05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60000" yWindow="-14480" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30480" yWindow="2260" windowWidth="20480" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="jobs" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="103">
   <si>
     <t>role</t>
   </si>
@@ -266,27 +266,6 @@
   </si>
   <si>
     <t>Data Laboratory</t>
-  </si>
-  <si>
-    <t>• As a senior full stack developer for [NuSkin](https://www.nuskin.com/us/en/, an international company known for its excellent  skin and beauty products I created new [Vue.js](https://vuejs.org/), [Nuxt](https://nuxt.com/), and [Vuetify](https://vuetifyjs.com/en/) components using [Bash], [Linux], [GitHub], [NodeJS], [HTML] and [CSS].  
-• Internationalized content using [Adobe Experience Cloud](https://business.adobe.com/).</t>
-  </si>
-  <si>
-    <t>• As a senior data engineer for SeniorLink's [Vela project]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/Vela-150x126.png} a homeservices support platform, helped create [ETL](https://aws.amazon.com/what-is/etl/) processes using [Amazon Kinesis](https://aws.amazon.com/pm/kinesis/), [Python], [PySpark](https://spark.apache.org/), and [Amazon Data Pipeline](https://docs.aws.amazon.com/datapipeline/latest/DeveloperGuide/what-is-datapipeline.html) to load structured event data from [PostgreSQL] databases into [Redshift](https://aws.amazon.com/pm/redshift/). 
-• Saved data to [Amazon S3] using [Amazon Kinesis] and triggered [Amazon Lambda](https://docs.aws.amazon.com/lambda/) jobs to aggregate steaming event data into [schema-on-read] file formats, [Apache Avro](https://avro.apache.org/) and [Apache Parquet](https://parquet.apache.org/).
-• Steered efforts in creating a [Data Lake](https://aws.amazon.com/big-data/datalakes-and-analytics/datalakes/) using [PostgreSQL] and [FlyWay](https://flywaydb.org/) with [Python] and [PySpark](https://spark.apache.org/docs/latest/api/python/index.html) pre-processing on [EC2 instances] using shared [Amazon EFS](https://zesty.co/blog/ebs-vs-efs-which-is-right) for staged storage.
-• Used streaming event messages queued in [RabbitMQ](https://docs.aws.amazon.com/amazon-mq/latest/developer-guide/working-with-rabbitmq.html) and [Amazon Kinesis] to build [type-2 slowly changing dimensions] and accumulative facts tables. 
-• Designed and implemented a custom [star-schema warehouse](https://www.databricks.com/glossary/star-schema) and [ETL] processes to [de-normalize](https://en.wikipedia.org/wiki/Denormalization) and load data into [Redshift](https://aws.amazon.com/redshift/) data warehouse for BI reporting using [Tableau](https://www.tableau.com/).
-• [Test-driven development](https://www.pluralsight.com/blog/software-development/tdd-vs-bdd) using [Bash], [Linux], [Python], [PyCharm], [PyTest], [Unit-test], [GitHub], [Jira], and [Jenkins](https://www.jenkins.io/).</t>
-  </si>
-  <si>
-    <t>• Co-founded [ClipFile]{https://shawn.beckerstudio.com/wp-content/uploads/2023/05/clipfile-infrastructure-150x150.png}, a company that envisioned building a web destination where users could easily record and share their favorite pieces of content like facts, authored stories, quotes, articles, chapters, or personal thoughts, as a way of concretely defining their personal [mindset]{https://sourcesofinsight.com/wp-content/uploads/2014/04/Mindset-768x505.jpg}(https://sourcesofinsight.com/what-is-mindset/).
-• Implemented [fuzzy matching](https://nanonets.com/blog/fuzzy-matching-fuzzy-logic/), [word clustering](https://www.ilc.cnr.it/EAGLES96/rep2/node37.html#:~:text=Word%20clustering%20is%20a%20technique,to%20information%20retrieval%20and%20filtering.), [semantic similarity scores](https://towardsdatascience.com/semantic-similarity-using-transformers-8f3cb5bf66d6), and [collaborative filtering](https://www.hindawi.com/journals/aai/2009/421425/) to help users find content that matched or differed from thieir own mindset.
-• Launched a novel [SaaS] using [Amazon Web Services] that let individuals and content creators search and share mindsets.
-• Conceptualized patented technology by designing and implementing a fuil-stack consumer-facing content management system that supported tuned matching among selected attributes.
-• [Java], [J2EE], [JSP], [Servlets], [Spring], [Amazon services], [JavaScript], [JQuery], [HTML], [CSS], [JUnit], [JMeter], [JProfile].
-• Utilized [REST], [Swagger], [Apache Shiro](https://shiro.apache.org/), [Eclipse IDE](https://www.eclipse.org/home/whatis/), [Apache Maven](https://maven.apache.org/what-is-maven.html), [Apache Ant](https://ant.apache.org/), [GitHub], [Hibernate], [Amazon SimpleDB](https://aws.amazon.com/simpledb/), [Linux](https://www.centos.org/), [Apache Tomcat](https://tomcat.apache.org/), [Bash], [Linux], [Jetty](https://projects.eclipse.org/projects/rt.jetty), and [Spring MVC](https://docs.spring.io/spring-framework/reference/web/webmvc.html).
-• Served as co-founder and co-authored [four patents](https://www.freepatentsonline.com/y2013/0325870.html).</t>
   </si>
   <si>
     <t>• As lead software developer, built a CD-ROM-based home design application for selecting premium home design products for previewing in the context of images of any household rooms. 
@@ -352,41 +331,77 @@
 • [Java], [J2EE], [Servlets], [Spring], [SpringBoot], [JAX-RS], [Bash], [Linux], [JUnit], [JMeter], and [JProfile]</t>
   </si>
   <si>
-    <t xml:space="preserve">• As a senior software engineer for Data Laboratory, an internet company that provides daily lead reports for independent real-estage agents world-wide, I  [containerized] legacy web applications using [Bash], [Linux], [GitHub], [Docker](https://www.docker.com/) and [Amazon Secrets Manager](https://aws.amazon.com/secrets-manager/). 
-• Updated legacy web apps using [Bash], [Linux], [HTML], [CSS], [JavaScript], [PostgreSQL], [NGINX], and [OpenSSL].
-• Documented existing data architecture as [ERDs](https://www.lucidchart.com/pages/er-diagrams) using [DBeaver Enterprise](https://dbeaver.com/dbeaver-enterprise/). </t>
-  </si>
-  <si>
     <t>Fannie Mae</t>
   </si>
   <si>
-    <t xml:space="preserve">Senior Data / Machine Learning Engineer </t>
-  </si>
-  <si>
-    <t xml:space="preserve">• Introductory phase in new role as senior data / machine learning engineer in the Risk &amp; Corporate Systems team at Fannie Mae GSE 
-</t>
-  </si>
-  <si>
-    <t>#006900</t>
-  </si>
-  <si>
-    <t>• Senior data engineer for [Angel Studios](https://www.angel.com/home), a streaming media service that offers family-friendly entertainment that amplifies light, with titles including The Chosen, Dry Bar Comedy, and Tuttle Twins.
-• Used [Python], [GitHub], [Pandas], [Numpy], [Keras], [Bash], [Linux], [PostgreSQL], and [Jupyter](https://jupyter.org/) to build and tune hyperparameters of a [convolutional neural network](https://towardsdatascience.com/a-comprehensive-guide-to-convolutional-neural-networks-the-eli5-way-3bd2b1164a53) with [supervised learning] on [Amazon Sagemaker](https://aws.amazon.com/pm/sagemaker/) to classify movie frames from episodic programs stored in [Amazon S3](https://aws.amazon.com/s3/storage-classes). 
-• Built web client apps using [Python] with [Postman](https://www.postman.com/) that made [REST] requests to pull monthly usage data from various web marketing partners like [FaceBook Marketing](https://www.quora.com/What-is-Facebook-Marketing-1), [Google Play](https://play.google/howplayworks/) , and [Vimeo](https://vimeo.com/). 
-• Worked with [Segment customer data platform](https://segment.com/customer-data-platform/), [Excel], and [Tableau] to create scheduled reports for the company's sales and finance teams.</t>
-  </si>
-  <si>
-    <t>• As a senior data engineer in the data cyber security team of the [Cigna Group](https://www.thecignagroup.com/) created a [REST API] using [Postman], [Bash], [Linux], and [OpenAPI] for pulling credentials from [CyberArk](https://www.cyberark.com/) using [OpenSSL] with [mutual TLS SSL authentication](https://docs.solace.com/Security/Two-Way-SSL-Authentication.htm) via [API Gateway]. 
-•  Migrated a suite of legacy [ETL][data pipeline] [Python] elements running on the [Unity IoC platform] with [PostgreSQL] and [S3] to pull credentials from the [CyberArk] identity service at runtime rather than using [Fernet](https://cryptography.io/en/latest/fernet/) encrypted local files. 
-•  Upgraded [GitHub] apps to use [Jenkins](https://docs.aws.amazon.com/apigateway/) [CI/CD pipeline] for build, applying software and cyber-security code checks, and on-prem server installation.</t>
-  </si>
-  <si>
-    <t>• As a senior data engineer in the analytics team of [Warner Brothers](https://warnerbrosgames.com/) Division, implemented high-volume [ETL] [data pipeline] [integrations] transforming and sharing  game telemetry and [user PII data] between WB-distributed consumer games and [marketing service platforms] via [Segment customer data platform](https://segment.com/customer-data-platform/) using [Kafka](https://aws.amazon.com/msk/), [Amazon S3], [Redshift](https://aws.amazon.com/redshift/), and [Apache Airflow](https://airflow.apache.org). 
-• Employed [Python], [GitHub], [Bash], [Linux], [Amazon Glue](https://aws.amazon.com/glue/) and [Apache Airflow](https://airflow.apache.org/) for external [3rd-party integrations] and internal dev-ops integrations with [Jenkins], [PostgreSQL], [DataDog](https://www.datadoghq.com/),  [ZenDesk](https://zendesk.com). and [Tableau].
-• Integrated with [Google BigQuery](https://cloud.google.com/bigquery using  [Apache Airflow](https://aws.amazon.com/managed-workflows-for-apache-airflow/), [Amazon S3], and [Redshift](https://aws.amazon.com/redshift/).</t>
-  </si>
-  <si>
     <t>CURRENT_DATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Senior Software Engineer </t>
+  </si>
+  <si>
+    <t>Spexture</t>
+  </si>
+  <si>
+    <t>• Designed and implemented an end-to-end CI/CD pipeline using a target-based architecture to optimize model deployment. 
+Automated multi-environment infrastructure provisioning and credential management via Hashicorp Terraform and Vault.
+• Deployed PySpark SQL Docker containers on an EKS-managed Kubernetes cluster to enhance resource utilization and scalability for data processing workloads.
+• Ensured system transparency using real-time monitoring solutions and dashboards with Amazon Managed Grafana.
+• Utilized AWS Glue and PySpark for data ingress, cleansing, versioning, and lineage tracking, maintaining data integrity and regulatory compliance for security.</t>
+  </si>
+  <si>
+    <t>darkforest</t>
+  </si>
+  <si>
+    <t>#116611</t>
+  </si>
+  <si>
+    <t>#0069AC</t>
+  </si>
+  <si>
+    <t>•	Upgraded application deployment processes and improved build automation by leveraging Jenkins CI/CD pipelines, integrating SetupTools, Artifactory/PyPI, SonarQube, and Xray. 
+•	Improved build automation and migrated legacy ETL data pipeline components from on-prem Unity IoC applications to AWS cloud using CDC.
+•	Designed Python-based REST API with mutual TLS/SSL authentication via AWS API Gateway for secure CyberArk’s credential retrieval.
+•	Runtime credential extraction eliminated dependency on locally encrypted files, reduced engineering effort, and minimized cost by 95% per password rollover event.</t>
+  </si>
+  <si>
+    <t>•	Developed and maintained ETL pipelines across multiple environments using AWS (AWS Redshift, Glue, S3, IAM, Lambda, SNS) and tools (SQL, dbt, REST APIs, Postman).
+•	Ensured efficient data ingestion and processing through validated SQL code for data lakes.
+•	Automated schema change tracking and Redshift external view updates using Amazon Glue, reducing manual intervention.
+•	Earned Agile Scrum Master certification, demonstrating knowledge of Agile methodologies and best practices.</t>
+  </si>
+  <si>
+    <t>•	Performed statistical modeling on game marketing data using analytics stack (Pandas, NumPy, Sci-kit Learn, Keras) with data visualization libraries.
+•	Leveraged existing game telemetry infrastructure to build marketing analytics solutions using Twilio Segment CDP, Kafka, Redshift, and Airflow. 
+•	Built real-time status dashboards using DataDog and Amazon QuickSight to provide visibility into marketing campaign metrics.</t>
+  </si>
+  <si>
+    <t>•	Implemented and fine-tuned a CNN using AWS SageMaker, PyTorch, and Keras to classify movie frames for digital asset monetization.
+•	Created executive dashboards and KPI reports using Snowflake and Looker to track revenue metrics and campaign performance.</t>
+  </si>
+  <si>
+    <t>•	Developed data visualizations using Seaborn, Plotly, and Matplotlib. 
+Implemented CI/CD workflows using GitHub Actions, Coverage, SonarQube, and Xray to improve code quality.
+•	Architected and built a custom star-schema data warehouse on PostgreSQL while utilizing dimensional modeling and SCD Type-2 tables with a shared streaming facts table.
+•	Automated infrastructure provisioning across development, staging, and production environments using Terraform and Helm.
+•	Integrated RESTful APIs to facilitate seamless data exchange with real-estate data teams and external customers.</t>
+  </si>
+  <si>
+    <t>•	Redesigned and optimized site registration and login workflows using wireframes for improved UX.
+•	Developed reusable Vue components with Vuetify, NodeJS, and SCSS.
+•	Internationalized web content and unified customer data using Adobe Experience Cloud, CDP, and XDM for personalized global user experiences.</t>
+  </si>
+  <si>
+    <t>•	Built AWS-based data pipeline enabling HIPAA-compliant healthcare messaging and collaboration on the Vela platform.
+•	Orchestrated end-to-end data flow: ingesting API Gateway messages via Kinesis streams, transforming to Parquet in S3, and processing with PySpark on EMR for Redshift loading.
+•	Defined RESTful APIs for daily caregiver questionnaire submission and data retrieval through web applications.
+•	Followed privacy and encryption standards for sensitive data, including PII, PHI, PCI, Patient Data, FHIR, and HL7, as well as HIPAA and GDPR.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">•	Designed and launched an AWS-based SaaS platform for content discovery and curation.
+•	Implemented patented technology to deliver a consumer-facing CMS with fuzzy matching capabilities among user-curated quotes and text fragments. A fuzzy matching system uses ML techniques (PCA, dimensionality reduction, K-means clustering) to connect user-curated content.
+•	Built scalable backend using Spring Boot, PostgreSQL, and Java 8, with RESTful APIs serving web and mobile clients.
+•	Developed an NLP-based recommendation engine analyzing user preferences across curated content (books, articles, quotes) using collaborative filtering. </t>
   </si>
 </sst>
 </file>
@@ -418,7 +433,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -503,6 +518,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF006900"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0069AC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -541,7 +562,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -631,6 +652,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -641,7 +665,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF0069AC"/>
       <color rgb="FF006900"/>
+      <color rgb="FF114700"/>
     </mruColors>
   </colors>
   <extLst>
@@ -943,10 +969,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="I12" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -993,59 +1019,59 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="112" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="7">
+        <v>45521</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" s="8">
+        <v>2</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="C2" s="7">
-        <v>45339</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="E2" s="8">
-        <v>1</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>11</v>
-      </c>
       <c r="G2" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H2" s="30"/>
       <c r="I2" s="6" t="s">
         <v>63</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="144" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>23</v>
+        <v>89</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="C3" s="7">
-        <v>45047</v>
+        <v>45339</v>
       </c>
       <c r="D3" s="7">
-        <v>45277</v>
+        <v>45474</v>
       </c>
       <c r="E3" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>11</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="9"/>
+        <v>94</v>
+      </c>
+      <c r="H3" s="31"/>
       <c r="I3" s="6" t="s">
         <v>63</v>
       </c>
@@ -1053,544 +1079,574 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="176" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="128" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>76</v>
+        <v>10</v>
       </c>
       <c r="C4" s="7">
-        <v>44805</v>
+        <v>45047</v>
       </c>
       <c r="D4" s="7">
-        <v>45047</v>
+        <v>45277</v>
       </c>
       <c r="E4" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="H4" s="9"/>
       <c r="I4" s="6" t="s">
         <v>63</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="192" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>15</v>
+        <v>76</v>
       </c>
       <c r="C5" s="7">
-        <v>44501</v>
+        <v>44805</v>
       </c>
       <c r="D5" s="7">
-        <v>44805</v>
+        <v>45047</v>
       </c>
       <c r="E5" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="H5" s="11"/>
       <c r="I5" s="6" t="s">
         <v>63</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>77</v>
+        <v>15</v>
       </c>
       <c r="C6" s="7">
-        <v>44136</v>
+        <v>44501</v>
       </c>
       <c r="D6" s="7">
-        <v>44501</v>
+        <v>44805</v>
       </c>
       <c r="E6" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="13"/>
+        <v>17</v>
+      </c>
+      <c r="H6" s="12"/>
       <c r="I6" s="6" t="s">
         <v>63</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="112" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>68</v>
+        <v>23</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>20</v>
+        <v>77</v>
       </c>
       <c r="C7" s="7">
-        <v>43770</v>
+        <v>44136</v>
       </c>
       <c r="D7" s="7">
-        <v>44136</v>
+        <v>44501</v>
       </c>
       <c r="E7" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="14"/>
+        <v>19</v>
+      </c>
+      <c r="H7" s="13"/>
       <c r="I7" s="6" t="s">
         <v>63</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="335" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>23</v>
+        <v>68</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>65</v>
+        <v>20</v>
       </c>
       <c r="C8" s="7">
-        <v>42795</v>
+        <v>43770</v>
       </c>
       <c r="D8" s="7">
-        <v>43770</v>
+        <v>44136</v>
       </c>
       <c r="E8" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H8" s="15"/>
+        <v>22</v>
+      </c>
+      <c r="H8" s="14"/>
       <c r="I8" s="6" t="s">
         <v>63</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>69</v>
+        <v>23</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="C9" s="7">
-        <v>42705</v>
+        <v>42795</v>
       </c>
       <c r="D9" s="7">
-        <v>42795</v>
+        <v>43770</v>
       </c>
       <c r="E9" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="H9" s="16"/>
+        <v>25</v>
+      </c>
+      <c r="H9" s="15"/>
       <c r="I9" s="6" t="s">
         <v>63</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="335" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="7">
+        <v>42705</v>
+      </c>
+      <c r="D10" s="7">
+        <v>42795</v>
+      </c>
+      <c r="E10" s="8">
+        <v>1</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" s="16"/>
+      <c r="I10" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="112" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B11" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C11" s="7">
         <v>40575</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D11" s="7">
         <v>42705</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E11" s="8">
         <v>2</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F11" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G11" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="17"/>
-      <c r="I10" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="J10" s="10" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="192" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="7">
-        <v>37561</v>
-      </c>
-      <c r="D11" s="7">
-        <v>40575</v>
-      </c>
-      <c r="E11" s="8">
-        <v>1</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H11" s="18"/>
+      <c r="H11" s="17"/>
       <c r="I11" s="6" t="s">
         <v>64</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="224" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="192" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C12" s="7">
-        <v>35827</v>
+        <v>37561</v>
       </c>
       <c r="D12" s="7">
-        <v>37561</v>
+        <v>40575</v>
       </c>
       <c r="E12" s="8">
         <v>1</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="H12" s="19"/>
+        <v>34</v>
+      </c>
+      <c r="H12" s="18"/>
       <c r="I12" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="144" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="224" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C13" s="7">
-        <v>35217</v>
+        <v>35827</v>
       </c>
       <c r="D13" s="7">
-        <v>35827</v>
+        <v>37561</v>
       </c>
       <c r="E13" s="8">
         <v>1</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="H13" s="9"/>
+        <v>37</v>
+      </c>
+      <c r="H13" s="19"/>
       <c r="I13" s="6" t="s">
         <v>63</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="335" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="144" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C14" s="7">
-        <v>33117</v>
+        <v>35217</v>
       </c>
       <c r="D14" s="7">
-        <v>35521</v>
+        <v>35827</v>
       </c>
       <c r="E14" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H14" s="11"/>
+        <v>40</v>
+      </c>
+      <c r="H14" s="9"/>
       <c r="I14" s="6" t="s">
         <v>63</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="304" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="335" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C15" s="7">
-        <v>32021</v>
+        <v>33117</v>
       </c>
       <c r="D15" s="7">
-        <v>33117</v>
+        <v>35521</v>
       </c>
       <c r="E15" s="8">
         <v>2</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="H15" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="H15" s="11"/>
       <c r="I15" s="6" t="s">
         <v>63</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="304" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>72</v>
+        <v>43</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C16" s="7">
-        <v>32295</v>
+        <v>32021</v>
       </c>
       <c r="D16" s="7">
-        <v>32752</v>
+        <v>33117</v>
       </c>
       <c r="E16" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H16" s="13"/>
+        <v>45</v>
+      </c>
+      <c r="H16" s="12"/>
       <c r="I16" s="6" t="s">
         <v>63</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="112" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="7">
+        <v>32295</v>
+      </c>
+      <c r="D17" s="7">
+        <v>32752</v>
+      </c>
+      <c r="E17" s="8">
+        <v>3</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" s="13"/>
+      <c r="I17" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="J17" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="112" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B18" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C18" s="7">
         <v>39417</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D18" s="7">
         <v>40391</v>
-      </c>
-      <c r="E17" s="8">
-        <v>2</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="H17" s="20"/>
-      <c r="I17" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="J17" s="21" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="128" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" s="7">
-        <v>38749</v>
-      </c>
-      <c r="D18" s="7">
-        <v>39417</v>
       </c>
       <c r="E18" s="8">
         <v>2</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H18" s="22"/>
+        <v>50</v>
+      </c>
+      <c r="H18" s="20"/>
       <c r="I18" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="J18" s="10" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="96" x14ac:dyDescent="0.2">
+      <c r="J18" s="21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="128" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C19" s="7">
-        <v>38384</v>
+        <v>38749</v>
       </c>
       <c r="D19" s="7">
-        <v>38749</v>
+        <v>39417</v>
       </c>
       <c r="E19" s="8">
         <v>2</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="H19" s="23"/>
+        <v>53</v>
+      </c>
+      <c r="H19" s="22"/>
       <c r="I19" s="6" t="s">
         <v>64</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="96" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C20" s="7">
-        <v>38018</v>
+        <v>38384</v>
       </c>
       <c r="D20" s="7">
-        <v>38384</v>
+        <v>38749</v>
       </c>
       <c r="E20" s="8">
         <v>2</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="H20" s="24"/>
+        <v>56</v>
+      </c>
+      <c r="H20" s="23"/>
       <c r="I20" s="6" t="s">
         <v>64</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="144" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>47</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C21" s="7">
-        <v>37681</v>
+        <v>38018</v>
       </c>
       <c r="D21" s="7">
-        <v>38018</v>
+        <v>38384</v>
       </c>
       <c r="E21" s="8">
         <v>2</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="H21" s="25"/>
+        <v>59</v>
+      </c>
+      <c r="H21" s="24"/>
       <c r="I21" s="6" t="s">
         <v>64</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>84</v>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="144" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="7">
+        <v>37681</v>
+      </c>
+      <c r="D22" s="7">
+        <v>38018</v>
+      </c>
+      <c r="E22" s="8">
+        <v>2</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="H22" s="25"/>
+      <c r="I22" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="J22" s="10" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>